<commit_message>
VHAR-7623 - UREM-excelpohjan pienet viilaukset
 - Merkitty pituus pakolliseksi
 - Poistettu pinta-ala excel-pohjasta
</commit_message>
<xml_diff>
--- a/dev-resources/excel/harja_urapaikkaustoteumien_tuonti_pohja.xlsx
+++ b/dev-resources/excel/harja_urapaikkaustoteumien_tuonti_pohja.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_aa5\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="8_{523923E3-530A-4824-9E90-579B8B6498E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4AABA32-35FB-4303-AC6D-2C164E22AAAF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{775F82FF-7EC5-4CDC-AD2C-D27C06FB2DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>URAPAIKKAUSTOTEUMIEN TUONTI HARJAAN</t>
   </si>
@@ -81,7 +81,7 @@
     <t>L-et. *</t>
   </si>
   <si>
-    <t>Leveys</t>
+    <t>Leveys (m) *</t>
   </si>
   <si>
     <t>Ajourat</t>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>Kok. Massamäärä (t) *</t>
-  </si>
-  <si>
-    <t>Pinta-ala (m2) *</t>
   </si>
   <si>
     <t>Massatyyppi</t>
@@ -641,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R232"/>
+  <dimension ref="A1:Q232"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:R4"/>
+      <selection activeCell="R3" sqref="R3:R231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -656,7 +653,7 @@
     <col min="6" max="6" width="6.7109375" customWidth="1"/>
     <col min="7" max="7" width="7.5703125" customWidth="1"/>
     <col min="8" max="8" width="6.42578125" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
     <col min="10" max="10" width="8" customWidth="1"/>
     <col min="11" max="11" width="7.85546875" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" customWidth="1"/>
@@ -665,10 +662,9 @@
     <col min="15" max="15" width="10.5703125" customWidth="1"/>
     <col min="16" max="16" width="12" customWidth="1"/>
     <col min="17" max="17" width="20.5703125" customWidth="1"/>
-    <col min="18" max="18" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="21">
+    <row r="1" spans="1:17" ht="21">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -688,9 +684,8 @@
       <c r="O1" s="9"/>
       <c r="P1" s="9"/>
       <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-    </row>
-    <row r="2" spans="1:18">
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="2"/>
@@ -710,9 +705,8 @@
       <c r="O2" s="11"/>
       <c r="P2" s="11"/>
       <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-    </row>
-    <row r="3" spans="1:18">
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="4" t="s">
@@ -738,9 +732,8 @@
       <c r="Q3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="R3" s="3"/>
-    </row>
-    <row r="4" spans="1:18">
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -792,11 +785,8 @@
       <c r="Q4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="R4" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="8"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
@@ -814,9 +804,8 @@
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-    </row>
-    <row r="6" spans="1:18">
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" s="8"/>
       <c r="B6" s="5"/>
       <c r="C6" s="1"/>
@@ -834,9 +823,8 @@
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-    </row>
-    <row r="7" spans="1:18">
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" s="8"/>
       <c r="B7" s="5"/>
       <c r="C7" s="1"/>
@@ -854,9 +842,8 @@
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-    </row>
-    <row r="8" spans="1:18">
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" s="8"/>
       <c r="B8" s="5"/>
       <c r="C8" s="1"/>
@@ -874,9 +861,8 @@
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-    </row>
-    <row r="9" spans="1:18">
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" s="8"/>
       <c r="B9" s="5"/>
       <c r="C9" s="1"/>
@@ -894,9 +880,8 @@
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-    </row>
-    <row r="10" spans="1:18">
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" s="8"/>
       <c r="B10" s="5"/>
       <c r="C10" s="1"/>
@@ -914,9 +899,8 @@
       <c r="O10" s="7"/>
       <c r="P10" s="7"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-    </row>
-    <row r="11" spans="1:18">
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" s="8"/>
       <c r="B11" s="5"/>
       <c r="C11" s="1"/>
@@ -934,9 +918,8 @@
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-    </row>
-    <row r="12" spans="1:18">
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" s="8"/>
       <c r="B12" s="5"/>
       <c r="C12" s="1"/>
@@ -954,9 +937,8 @@
       <c r="O12" s="7"/>
       <c r="P12" s="7"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-    </row>
-    <row r="13" spans="1:18">
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" s="8"/>
       <c r="B13" s="5"/>
       <c r="C13" s="1"/>
@@ -974,9 +956,8 @@
       <c r="O13" s="7"/>
       <c r="P13" s="7"/>
       <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-    </row>
-    <row r="14" spans="1:18">
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" s="8"/>
       <c r="B14" s="5"/>
       <c r="C14" s="1"/>
@@ -994,9 +975,8 @@
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
       <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-    </row>
-    <row r="15" spans="1:18">
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" s="8"/>
       <c r="B15" s="5"/>
       <c r="C15" s="1"/>
@@ -1014,9 +994,8 @@
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
       <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-    </row>
-    <row r="16" spans="1:18">
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" s="8"/>
       <c r="B16" s="5"/>
       <c r="C16" s="1"/>
@@ -1034,9 +1013,8 @@
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
       <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-    </row>
-    <row r="17" spans="1:18">
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" s="8"/>
       <c r="B17" s="5"/>
       <c r="C17" s="1"/>
@@ -1054,9 +1032,8 @@
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
       <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-    </row>
-    <row r="18" spans="1:18">
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18" s="8"/>
       <c r="B18" s="5"/>
       <c r="C18" s="1"/>
@@ -1074,9 +1051,8 @@
       <c r="O18" s="7"/>
       <c r="P18" s="7"/>
       <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-    </row>
-    <row r="19" spans="1:18">
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19" s="8"/>
       <c r="B19" s="5"/>
       <c r="C19" s="1"/>
@@ -1094,9 +1070,8 @@
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
       <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-    </row>
-    <row r="20" spans="1:18">
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20" s="8"/>
       <c r="B20" s="5"/>
       <c r="C20" s="1"/>
@@ -1114,9 +1089,8 @@
       <c r="O20" s="7"/>
       <c r="P20" s="7"/>
       <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-    </row>
-    <row r="21" spans="1:18">
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21" s="8"/>
       <c r="B21" s="5"/>
       <c r="C21" s="1"/>
@@ -1134,9 +1108,8 @@
       <c r="O21" s="7"/>
       <c r="P21" s="7"/>
       <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-    </row>
-    <row r="22" spans="1:18">
+    </row>
+    <row r="22" spans="1:17">
       <c r="A22" s="8"/>
       <c r="B22" s="5"/>
       <c r="C22" s="1"/>
@@ -1154,9 +1127,8 @@
       <c r="O22" s="7"/>
       <c r="P22" s="7"/>
       <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-    </row>
-    <row r="23" spans="1:18">
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23" s="8"/>
       <c r="B23" s="5"/>
       <c r="C23" s="1"/>
@@ -1174,9 +1146,8 @@
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
       <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-    </row>
-    <row r="24" spans="1:18">
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24" s="8"/>
       <c r="B24" s="5"/>
       <c r="C24" s="1"/>
@@ -1194,9 +1165,8 @@
       <c r="O24" s="7"/>
       <c r="P24" s="7"/>
       <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-    </row>
-    <row r="25" spans="1:18">
+    </row>
+    <row r="25" spans="1:17">
       <c r="A25" s="8"/>
       <c r="B25" s="5"/>
       <c r="C25" s="1"/>
@@ -1214,9 +1184,8 @@
       <c r="O25" s="7"/>
       <c r="P25" s="7"/>
       <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-    </row>
-    <row r="26" spans="1:18">
+    </row>
+    <row r="26" spans="1:17">
       <c r="A26" s="8"/>
       <c r="B26" s="5"/>
       <c r="C26" s="1"/>
@@ -1234,9 +1203,8 @@
       <c r="O26" s="7"/>
       <c r="P26" s="7"/>
       <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
-    </row>
-    <row r="27" spans="1:18">
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27" s="8"/>
       <c r="B27" s="5"/>
       <c r="C27" s="1"/>
@@ -1254,9 +1222,8 @@
       <c r="O27" s="7"/>
       <c r="P27" s="7"/>
       <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
-    </row>
-    <row r="28" spans="1:18">
+    </row>
+    <row r="28" spans="1:17">
       <c r="A28" s="8"/>
       <c r="B28" s="5"/>
       <c r="C28" s="1"/>
@@ -1274,9 +1241,8 @@
       <c r="O28" s="7"/>
       <c r="P28" s="7"/>
       <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
-    </row>
-    <row r="29" spans="1:18">
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29" s="8"/>
       <c r="B29" s="5"/>
       <c r="C29" s="1"/>
@@ -1294,9 +1260,8 @@
       <c r="O29" s="7"/>
       <c r="P29" s="7"/>
       <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-    </row>
-    <row r="30" spans="1:18">
+    </row>
+    <row r="30" spans="1:17">
       <c r="A30" s="8"/>
       <c r="B30" s="5"/>
       <c r="C30" s="1"/>
@@ -1314,9 +1279,8 @@
       <c r="O30" s="7"/>
       <c r="P30" s="7"/>
       <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
-    </row>
-    <row r="31" spans="1:18">
+    </row>
+    <row r="31" spans="1:17">
       <c r="A31" s="8"/>
       <c r="B31" s="5"/>
       <c r="C31" s="1"/>
@@ -1334,9 +1298,8 @@
       <c r="O31" s="7"/>
       <c r="P31" s="7"/>
       <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
-    </row>
-    <row r="32" spans="1:18">
+    </row>
+    <row r="32" spans="1:17">
       <c r="A32" s="8"/>
       <c r="B32" s="5"/>
       <c r="C32" s="1"/>
@@ -1354,9 +1317,8 @@
       <c r="O32" s="7"/>
       <c r="P32" s="7"/>
       <c r="Q32" s="1"/>
-      <c r="R32" s="1"/>
-    </row>
-    <row r="33" spans="1:18">
+    </row>
+    <row r="33" spans="1:17">
       <c r="A33" s="8"/>
       <c r="B33" s="5"/>
       <c r="C33" s="1"/>
@@ -1374,9 +1336,8 @@
       <c r="O33" s="7"/>
       <c r="P33" s="7"/>
       <c r="Q33" s="1"/>
-      <c r="R33" s="1"/>
-    </row>
-    <row r="34" spans="1:18">
+    </row>
+    <row r="34" spans="1:17">
       <c r="A34" s="8"/>
       <c r="B34" s="5"/>
       <c r="C34" s="1"/>
@@ -1394,9 +1355,8 @@
       <c r="O34" s="7"/>
       <c r="P34" s="7"/>
       <c r="Q34" s="1"/>
-      <c r="R34" s="1"/>
-    </row>
-    <row r="35" spans="1:18">
+    </row>
+    <row r="35" spans="1:17">
       <c r="A35" s="8"/>
       <c r="B35" s="5"/>
       <c r="C35" s="1"/>
@@ -1414,9 +1374,8 @@
       <c r="O35" s="7"/>
       <c r="P35" s="7"/>
       <c r="Q35" s="1"/>
-      <c r="R35" s="1"/>
-    </row>
-    <row r="36" spans="1:18">
+    </row>
+    <row r="36" spans="1:17">
       <c r="A36" s="8"/>
       <c r="B36" s="5"/>
       <c r="C36" s="1"/>
@@ -1434,9 +1393,8 @@
       <c r="O36" s="7"/>
       <c r="P36" s="7"/>
       <c r="Q36" s="1"/>
-      <c r="R36" s="1"/>
-    </row>
-    <row r="37" spans="1:18">
+    </row>
+    <row r="37" spans="1:17">
       <c r="A37" s="8"/>
       <c r="B37" s="5"/>
       <c r="C37" s="1"/>
@@ -1454,9 +1412,8 @@
       <c r="O37" s="7"/>
       <c r="P37" s="7"/>
       <c r="Q37" s="1"/>
-      <c r="R37" s="1"/>
-    </row>
-    <row r="38" spans="1:18">
+    </row>
+    <row r="38" spans="1:17">
       <c r="A38" s="8"/>
       <c r="B38" s="5"/>
       <c r="C38" s="1"/>
@@ -1474,9 +1431,8 @@
       <c r="O38" s="7"/>
       <c r="P38" s="7"/>
       <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
-    </row>
-    <row r="39" spans="1:18">
+    </row>
+    <row r="39" spans="1:17">
       <c r="A39" s="8"/>
       <c r="B39" s="5"/>
       <c r="C39" s="1"/>
@@ -1494,9 +1450,8 @@
       <c r="O39" s="7"/>
       <c r="P39" s="7"/>
       <c r="Q39" s="1"/>
-      <c r="R39" s="1"/>
-    </row>
-    <row r="40" spans="1:18">
+    </row>
+    <row r="40" spans="1:17">
       <c r="A40" s="8"/>
       <c r="B40" s="5"/>
       <c r="C40" s="1"/>
@@ -1514,9 +1469,8 @@
       <c r="O40" s="7"/>
       <c r="P40" s="7"/>
       <c r="Q40" s="1"/>
-      <c r="R40" s="1"/>
-    </row>
-    <row r="41" spans="1:18">
+    </row>
+    <row r="41" spans="1:17">
       <c r="A41" s="8"/>
       <c r="B41" s="5"/>
       <c r="C41" s="1"/>
@@ -1534,9 +1488,8 @@
       <c r="O41" s="7"/>
       <c r="P41" s="7"/>
       <c r="Q41" s="1"/>
-      <c r="R41" s="1"/>
-    </row>
-    <row r="42" spans="1:18">
+    </row>
+    <row r="42" spans="1:17">
       <c r="A42" s="8"/>
       <c r="B42" s="5"/>
       <c r="C42" s="1"/>
@@ -1554,9 +1507,8 @@
       <c r="O42" s="7"/>
       <c r="P42" s="7"/>
       <c r="Q42" s="1"/>
-      <c r="R42" s="1"/>
-    </row>
-    <row r="43" spans="1:18">
+    </row>
+    <row r="43" spans="1:17">
       <c r="A43" s="8"/>
       <c r="B43" s="5"/>
       <c r="C43" s="1"/>
@@ -1574,9 +1526,8 @@
       <c r="O43" s="7"/>
       <c r="P43" s="7"/>
       <c r="Q43" s="1"/>
-      <c r="R43" s="1"/>
-    </row>
-    <row r="44" spans="1:18">
+    </row>
+    <row r="44" spans="1:17">
       <c r="A44" s="8"/>
       <c r="B44" s="5"/>
       <c r="C44" s="1"/>
@@ -1594,9 +1545,8 @@
       <c r="O44" s="7"/>
       <c r="P44" s="7"/>
       <c r="Q44" s="1"/>
-      <c r="R44" s="1"/>
-    </row>
-    <row r="45" spans="1:18">
+    </row>
+    <row r="45" spans="1:17">
       <c r="A45" s="8"/>
       <c r="B45" s="5"/>
       <c r="C45" s="1"/>
@@ -1614,9 +1564,8 @@
       <c r="O45" s="7"/>
       <c r="P45" s="7"/>
       <c r="Q45" s="1"/>
-      <c r="R45" s="1"/>
-    </row>
-    <row r="46" spans="1:18">
+    </row>
+    <row r="46" spans="1:17">
       <c r="A46" s="8"/>
       <c r="B46" s="5"/>
       <c r="C46" s="1"/>
@@ -1634,9 +1583,8 @@
       <c r="O46" s="7"/>
       <c r="P46" s="7"/>
       <c r="Q46" s="1"/>
-      <c r="R46" s="1"/>
-    </row>
-    <row r="47" spans="1:18">
+    </row>
+    <row r="47" spans="1:17">
       <c r="A47" s="8"/>
       <c r="B47" s="5"/>
       <c r="C47" s="1"/>
@@ -1654,9 +1602,8 @@
       <c r="O47" s="7"/>
       <c r="P47" s="7"/>
       <c r="Q47" s="1"/>
-      <c r="R47" s="1"/>
-    </row>
-    <row r="48" spans="1:18">
+    </row>
+    <row r="48" spans="1:17">
       <c r="A48" s="8"/>
       <c r="B48" s="5"/>
       <c r="C48" s="1"/>
@@ -1674,9 +1621,8 @@
       <c r="O48" s="7"/>
       <c r="P48" s="7"/>
       <c r="Q48" s="1"/>
-      <c r="R48" s="1"/>
-    </row>
-    <row r="49" spans="1:18">
+    </row>
+    <row r="49" spans="1:17">
       <c r="A49" s="8"/>
       <c r="B49" s="5"/>
       <c r="C49" s="1"/>
@@ -1694,9 +1640,8 @@
       <c r="O49" s="7"/>
       <c r="P49" s="7"/>
       <c r="Q49" s="1"/>
-      <c r="R49" s="1"/>
-    </row>
-    <row r="50" spans="1:18">
+    </row>
+    <row r="50" spans="1:17">
       <c r="A50" s="8"/>
       <c r="B50" s="5"/>
       <c r="C50" s="1"/>
@@ -1714,9 +1659,8 @@
       <c r="O50" s="7"/>
       <c r="P50" s="7"/>
       <c r="Q50" s="1"/>
-      <c r="R50" s="1"/>
-    </row>
-    <row r="51" spans="1:18">
+    </row>
+    <row r="51" spans="1:17">
       <c r="A51" s="8"/>
       <c r="B51" s="5"/>
       <c r="C51" s="1"/>
@@ -1734,9 +1678,8 @@
       <c r="O51" s="7"/>
       <c r="P51" s="7"/>
       <c r="Q51" s="1"/>
-      <c r="R51" s="1"/>
-    </row>
-    <row r="52" spans="1:18">
+    </row>
+    <row r="52" spans="1:17">
       <c r="A52" s="8"/>
       <c r="B52" s="5"/>
       <c r="C52" s="1"/>
@@ -1754,9 +1697,8 @@
       <c r="O52" s="7"/>
       <c r="P52" s="7"/>
       <c r="Q52" s="1"/>
-      <c r="R52" s="1"/>
-    </row>
-    <row r="53" spans="1:18">
+    </row>
+    <row r="53" spans="1:17">
       <c r="A53" s="8"/>
       <c r="B53" s="5"/>
       <c r="C53" s="1"/>
@@ -1774,9 +1716,8 @@
       <c r="O53" s="7"/>
       <c r="P53" s="7"/>
       <c r="Q53" s="1"/>
-      <c r="R53" s="1"/>
-    </row>
-    <row r="54" spans="1:18">
+    </row>
+    <row r="54" spans="1:17">
       <c r="A54" s="8"/>
       <c r="B54" s="5"/>
       <c r="C54" s="1"/>
@@ -1794,9 +1735,8 @@
       <c r="O54" s="7"/>
       <c r="P54" s="7"/>
       <c r="Q54" s="1"/>
-      <c r="R54" s="1"/>
-    </row>
-    <row r="55" spans="1:18">
+    </row>
+    <row r="55" spans="1:17">
       <c r="A55" s="8"/>
       <c r="B55" s="5"/>
       <c r="C55" s="1"/>
@@ -1814,9 +1754,8 @@
       <c r="O55" s="7"/>
       <c r="P55" s="7"/>
       <c r="Q55" s="1"/>
-      <c r="R55" s="1"/>
-    </row>
-    <row r="56" spans="1:18">
+    </row>
+    <row r="56" spans="1:17">
       <c r="A56" s="8"/>
       <c r="B56" s="5"/>
       <c r="C56" s="1"/>
@@ -1834,9 +1773,8 @@
       <c r="O56" s="7"/>
       <c r="P56" s="7"/>
       <c r="Q56" s="1"/>
-      <c r="R56" s="1"/>
-    </row>
-    <row r="57" spans="1:18">
+    </row>
+    <row r="57" spans="1:17">
       <c r="A57" s="8"/>
       <c r="B57" s="5"/>
       <c r="C57" s="1"/>
@@ -1854,9 +1792,8 @@
       <c r="O57" s="7"/>
       <c r="P57" s="7"/>
       <c r="Q57" s="1"/>
-      <c r="R57" s="1"/>
-    </row>
-    <row r="58" spans="1:18">
+    </row>
+    <row r="58" spans="1:17">
       <c r="A58" s="8"/>
       <c r="B58" s="5"/>
       <c r="C58" s="1"/>
@@ -1874,9 +1811,8 @@
       <c r="O58" s="7"/>
       <c r="P58" s="7"/>
       <c r="Q58" s="1"/>
-      <c r="R58" s="1"/>
-    </row>
-    <row r="59" spans="1:18">
+    </row>
+    <row r="59" spans="1:17">
       <c r="A59" s="8"/>
       <c r="B59" s="5"/>
       <c r="C59" s="1"/>
@@ -1894,9 +1830,8 @@
       <c r="O59" s="7"/>
       <c r="P59" s="7"/>
       <c r="Q59" s="1"/>
-      <c r="R59" s="1"/>
-    </row>
-    <row r="60" spans="1:18">
+    </row>
+    <row r="60" spans="1:17">
       <c r="A60" s="8"/>
       <c r="B60" s="5"/>
       <c r="C60" s="1"/>
@@ -1914,9 +1849,8 @@
       <c r="O60" s="7"/>
       <c r="P60" s="7"/>
       <c r="Q60" s="1"/>
-      <c r="R60" s="1"/>
-    </row>
-    <row r="61" spans="1:18">
+    </row>
+    <row r="61" spans="1:17">
       <c r="A61" s="8"/>
       <c r="B61" s="5"/>
       <c r="C61" s="1"/>
@@ -1934,9 +1868,8 @@
       <c r="O61" s="7"/>
       <c r="P61" s="7"/>
       <c r="Q61" s="1"/>
-      <c r="R61" s="1"/>
-    </row>
-    <row r="62" spans="1:18">
+    </row>
+    <row r="62" spans="1:17">
       <c r="A62" s="8"/>
       <c r="B62" s="5"/>
       <c r="C62" s="1"/>
@@ -1954,9 +1887,8 @@
       <c r="O62" s="7"/>
       <c r="P62" s="7"/>
       <c r="Q62" s="1"/>
-      <c r="R62" s="1"/>
-    </row>
-    <row r="63" spans="1:18">
+    </row>
+    <row r="63" spans="1:17">
       <c r="A63" s="8"/>
       <c r="B63" s="5"/>
       <c r="C63" s="1"/>
@@ -1974,9 +1906,8 @@
       <c r="O63" s="7"/>
       <c r="P63" s="7"/>
       <c r="Q63" s="1"/>
-      <c r="R63" s="1"/>
-    </row>
-    <row r="64" spans="1:18">
+    </row>
+    <row r="64" spans="1:17">
       <c r="A64" s="8"/>
       <c r="B64" s="5"/>
       <c r="C64" s="1"/>
@@ -1994,9 +1925,8 @@
       <c r="O64" s="7"/>
       <c r="P64" s="7"/>
       <c r="Q64" s="1"/>
-      <c r="R64" s="1"/>
-    </row>
-    <row r="65" spans="1:18">
+    </row>
+    <row r="65" spans="1:17">
       <c r="A65" s="8"/>
       <c r="B65" s="5"/>
       <c r="C65" s="1"/>
@@ -2014,9 +1944,8 @@
       <c r="O65" s="7"/>
       <c r="P65" s="7"/>
       <c r="Q65" s="1"/>
-      <c r="R65" s="1"/>
-    </row>
-    <row r="66" spans="1:18">
+    </row>
+    <row r="66" spans="1:17">
       <c r="A66" s="8"/>
       <c r="B66" s="5"/>
       <c r="C66" s="1"/>
@@ -2034,9 +1963,8 @@
       <c r="O66" s="7"/>
       <c r="P66" s="7"/>
       <c r="Q66" s="1"/>
-      <c r="R66" s="1"/>
-    </row>
-    <row r="67" spans="1:18">
+    </row>
+    <row r="67" spans="1:17">
       <c r="A67" s="8"/>
       <c r="B67" s="5"/>
       <c r="C67" s="1"/>
@@ -2054,9 +1982,8 @@
       <c r="O67" s="7"/>
       <c r="P67" s="7"/>
       <c r="Q67" s="1"/>
-      <c r="R67" s="1"/>
-    </row>
-    <row r="68" spans="1:18">
+    </row>
+    <row r="68" spans="1:17">
       <c r="A68" s="8"/>
       <c r="B68" s="5"/>
       <c r="C68" s="1"/>
@@ -2074,9 +2001,8 @@
       <c r="O68" s="7"/>
       <c r="P68" s="7"/>
       <c r="Q68" s="1"/>
-      <c r="R68" s="1"/>
-    </row>
-    <row r="69" spans="1:18">
+    </row>
+    <row r="69" spans="1:17">
       <c r="A69" s="8"/>
       <c r="B69" s="5"/>
       <c r="C69" s="1"/>
@@ -2094,9 +2020,8 @@
       <c r="O69" s="7"/>
       <c r="P69" s="7"/>
       <c r="Q69" s="1"/>
-      <c r="R69" s="1"/>
-    </row>
-    <row r="70" spans="1:18">
+    </row>
+    <row r="70" spans="1:17">
       <c r="A70" s="8"/>
       <c r="B70" s="5"/>
       <c r="C70" s="1"/>
@@ -2114,9 +2039,8 @@
       <c r="O70" s="7"/>
       <c r="P70" s="7"/>
       <c r="Q70" s="1"/>
-      <c r="R70" s="1"/>
-    </row>
-    <row r="71" spans="1:18">
+    </row>
+    <row r="71" spans="1:17">
       <c r="A71" s="8"/>
       <c r="B71" s="5"/>
       <c r="C71" s="1"/>
@@ -2134,9 +2058,8 @@
       <c r="O71" s="7"/>
       <c r="P71" s="7"/>
       <c r="Q71" s="1"/>
-      <c r="R71" s="1"/>
-    </row>
-    <row r="72" spans="1:18">
+    </row>
+    <row r="72" spans="1:17">
       <c r="A72" s="8"/>
       <c r="B72" s="5"/>
       <c r="C72" s="1"/>
@@ -2154,9 +2077,8 @@
       <c r="O72" s="7"/>
       <c r="P72" s="7"/>
       <c r="Q72" s="1"/>
-      <c r="R72" s="1"/>
-    </row>
-    <row r="73" spans="1:18">
+    </row>
+    <row r="73" spans="1:17">
       <c r="A73" s="8"/>
       <c r="B73" s="5"/>
       <c r="C73" s="1"/>
@@ -2174,9 +2096,8 @@
       <c r="O73" s="7"/>
       <c r="P73" s="7"/>
       <c r="Q73" s="1"/>
-      <c r="R73" s="1"/>
-    </row>
-    <row r="74" spans="1:18">
+    </row>
+    <row r="74" spans="1:17">
       <c r="A74" s="8"/>
       <c r="B74" s="5"/>
       <c r="C74" s="1"/>
@@ -2194,9 +2115,8 @@
       <c r="O74" s="7"/>
       <c r="P74" s="7"/>
       <c r="Q74" s="1"/>
-      <c r="R74" s="1"/>
-    </row>
-    <row r="75" spans="1:18">
+    </row>
+    <row r="75" spans="1:17">
       <c r="A75" s="8"/>
       <c r="B75" s="5"/>
       <c r="C75" s="1"/>
@@ -2214,9 +2134,8 @@
       <c r="O75" s="7"/>
       <c r="P75" s="7"/>
       <c r="Q75" s="1"/>
-      <c r="R75" s="1"/>
-    </row>
-    <row r="76" spans="1:18">
+    </row>
+    <row r="76" spans="1:17">
       <c r="A76" s="8"/>
       <c r="B76" s="5"/>
       <c r="C76" s="1"/>
@@ -2234,9 +2153,8 @@
       <c r="O76" s="7"/>
       <c r="P76" s="7"/>
       <c r="Q76" s="1"/>
-      <c r="R76" s="1"/>
-    </row>
-    <row r="77" spans="1:18">
+    </row>
+    <row r="77" spans="1:17">
       <c r="A77" s="8"/>
       <c r="B77" s="5"/>
       <c r="C77" s="1"/>
@@ -2254,9 +2172,8 @@
       <c r="O77" s="7"/>
       <c r="P77" s="7"/>
       <c r="Q77" s="1"/>
-      <c r="R77" s="1"/>
-    </row>
-    <row r="78" spans="1:18">
+    </row>
+    <row r="78" spans="1:17">
       <c r="A78" s="8"/>
       <c r="B78" s="5"/>
       <c r="C78" s="1"/>
@@ -2274,9 +2191,8 @@
       <c r="O78" s="7"/>
       <c r="P78" s="7"/>
       <c r="Q78" s="1"/>
-      <c r="R78" s="1"/>
-    </row>
-    <row r="79" spans="1:18">
+    </row>
+    <row r="79" spans="1:17">
       <c r="A79" s="8"/>
       <c r="B79" s="5"/>
       <c r="C79" s="1"/>
@@ -2294,9 +2210,8 @@
       <c r="O79" s="7"/>
       <c r="P79" s="7"/>
       <c r="Q79" s="1"/>
-      <c r="R79" s="1"/>
-    </row>
-    <row r="80" spans="1:18">
+    </row>
+    <row r="80" spans="1:17">
       <c r="A80" s="8"/>
       <c r="B80" s="5"/>
       <c r="C80" s="1"/>
@@ -2314,9 +2229,8 @@
       <c r="O80" s="7"/>
       <c r="P80" s="7"/>
       <c r="Q80" s="1"/>
-      <c r="R80" s="1"/>
-    </row>
-    <row r="81" spans="1:18">
+    </row>
+    <row r="81" spans="1:17">
       <c r="A81" s="8"/>
       <c r="B81" s="5"/>
       <c r="C81" s="1"/>
@@ -2334,9 +2248,8 @@
       <c r="O81" s="7"/>
       <c r="P81" s="7"/>
       <c r="Q81" s="1"/>
-      <c r="R81" s="1"/>
-    </row>
-    <row r="82" spans="1:18">
+    </row>
+    <row r="82" spans="1:17">
       <c r="A82" s="8"/>
       <c r="B82" s="5"/>
       <c r="C82" s="1"/>
@@ -2354,9 +2267,8 @@
       <c r="O82" s="7"/>
       <c r="P82" s="7"/>
       <c r="Q82" s="1"/>
-      <c r="R82" s="1"/>
-    </row>
-    <row r="83" spans="1:18">
+    </row>
+    <row r="83" spans="1:17">
       <c r="A83" s="8"/>
       <c r="B83" s="5"/>
       <c r="C83" s="1"/>
@@ -2374,9 +2286,8 @@
       <c r="O83" s="7"/>
       <c r="P83" s="7"/>
       <c r="Q83" s="1"/>
-      <c r="R83" s="1"/>
-    </row>
-    <row r="84" spans="1:18">
+    </row>
+    <row r="84" spans="1:17">
       <c r="A84" s="8"/>
       <c r="B84" s="5"/>
       <c r="C84" s="1"/>
@@ -2394,9 +2305,8 @@
       <c r="O84" s="7"/>
       <c r="P84" s="7"/>
       <c r="Q84" s="1"/>
-      <c r="R84" s="1"/>
-    </row>
-    <row r="85" spans="1:18">
+    </row>
+    <row r="85" spans="1:17">
       <c r="A85" s="8"/>
       <c r="B85" s="5"/>
       <c r="C85" s="1"/>
@@ -2414,9 +2324,8 @@
       <c r="O85" s="7"/>
       <c r="P85" s="7"/>
       <c r="Q85" s="1"/>
-      <c r="R85" s="1"/>
-    </row>
-    <row r="86" spans="1:18">
+    </row>
+    <row r="86" spans="1:17">
       <c r="A86" s="8"/>
       <c r="B86" s="5"/>
       <c r="C86" s="1"/>
@@ -2434,9 +2343,8 @@
       <c r="O86" s="7"/>
       <c r="P86" s="7"/>
       <c r="Q86" s="1"/>
-      <c r="R86" s="1"/>
-    </row>
-    <row r="87" spans="1:18">
+    </row>
+    <row r="87" spans="1:17">
       <c r="A87" s="8"/>
       <c r="B87" s="5"/>
       <c r="C87" s="1"/>
@@ -2454,9 +2362,8 @@
       <c r="O87" s="7"/>
       <c r="P87" s="7"/>
       <c r="Q87" s="1"/>
-      <c r="R87" s="1"/>
-    </row>
-    <row r="88" spans="1:18">
+    </row>
+    <row r="88" spans="1:17">
       <c r="A88" s="8"/>
       <c r="B88" s="5"/>
       <c r="C88" s="1"/>
@@ -2474,9 +2381,8 @@
       <c r="O88" s="7"/>
       <c r="P88" s="7"/>
       <c r="Q88" s="1"/>
-      <c r="R88" s="1"/>
-    </row>
-    <row r="89" spans="1:18">
+    </row>
+    <row r="89" spans="1:17">
       <c r="A89" s="8"/>
       <c r="B89" s="5"/>
       <c r="C89" s="1"/>
@@ -2494,9 +2400,8 @@
       <c r="O89" s="7"/>
       <c r="P89" s="7"/>
       <c r="Q89" s="1"/>
-      <c r="R89" s="1"/>
-    </row>
-    <row r="90" spans="1:18">
+    </row>
+    <row r="90" spans="1:17">
       <c r="A90" s="8"/>
       <c r="B90" s="5"/>
       <c r="C90" s="1"/>
@@ -2514,9 +2419,8 @@
       <c r="O90" s="7"/>
       <c r="P90" s="7"/>
       <c r="Q90" s="1"/>
-      <c r="R90" s="1"/>
-    </row>
-    <row r="91" spans="1:18">
+    </row>
+    <row r="91" spans="1:17">
       <c r="A91" s="8"/>
       <c r="B91" s="5"/>
       <c r="C91" s="1"/>
@@ -2534,9 +2438,8 @@
       <c r="O91" s="7"/>
       <c r="P91" s="7"/>
       <c r="Q91" s="1"/>
-      <c r="R91" s="1"/>
-    </row>
-    <row r="92" spans="1:18">
+    </row>
+    <row r="92" spans="1:17">
       <c r="A92" s="8"/>
       <c r="B92" s="5"/>
       <c r="C92" s="1"/>
@@ -2554,9 +2457,8 @@
       <c r="O92" s="7"/>
       <c r="P92" s="7"/>
       <c r="Q92" s="1"/>
-      <c r="R92" s="1"/>
-    </row>
-    <row r="93" spans="1:18">
+    </row>
+    <row r="93" spans="1:17">
       <c r="A93" s="8"/>
       <c r="B93" s="5"/>
       <c r="C93" s="1"/>
@@ -2574,9 +2476,8 @@
       <c r="O93" s="7"/>
       <c r="P93" s="7"/>
       <c r="Q93" s="1"/>
-      <c r="R93" s="1"/>
-    </row>
-    <row r="94" spans="1:18">
+    </row>
+    <row r="94" spans="1:17">
       <c r="A94" s="8"/>
       <c r="B94" s="5"/>
       <c r="C94" s="1"/>
@@ -2594,9 +2495,8 @@
       <c r="O94" s="7"/>
       <c r="P94" s="7"/>
       <c r="Q94" s="1"/>
-      <c r="R94" s="1"/>
-    </row>
-    <row r="95" spans="1:18">
+    </row>
+    <row r="95" spans="1:17">
       <c r="A95" s="8"/>
       <c r="B95" s="5"/>
       <c r="C95" s="1"/>
@@ -2614,9 +2514,8 @@
       <c r="O95" s="7"/>
       <c r="P95" s="7"/>
       <c r="Q95" s="1"/>
-      <c r="R95" s="1"/>
-    </row>
-    <row r="96" spans="1:18">
+    </row>
+    <row r="96" spans="1:17">
       <c r="A96" s="8"/>
       <c r="B96" s="5"/>
       <c r="C96" s="1"/>
@@ -2634,9 +2533,8 @@
       <c r="O96" s="7"/>
       <c r="P96" s="7"/>
       <c r="Q96" s="1"/>
-      <c r="R96" s="1"/>
-    </row>
-    <row r="97" spans="1:18">
+    </row>
+    <row r="97" spans="1:17">
       <c r="A97" s="8"/>
       <c r="B97" s="5"/>
       <c r="C97" s="1"/>
@@ -2654,9 +2552,8 @@
       <c r="O97" s="7"/>
       <c r="P97" s="7"/>
       <c r="Q97" s="1"/>
-      <c r="R97" s="1"/>
-    </row>
-    <row r="98" spans="1:18">
+    </row>
+    <row r="98" spans="1:17">
       <c r="A98" s="8"/>
       <c r="B98" s="5"/>
       <c r="C98" s="1"/>
@@ -2674,9 +2571,8 @@
       <c r="O98" s="7"/>
       <c r="P98" s="7"/>
       <c r="Q98" s="1"/>
-      <c r="R98" s="1"/>
-    </row>
-    <row r="99" spans="1:18">
+    </row>
+    <row r="99" spans="1:17">
       <c r="A99" s="8"/>
       <c r="B99" s="5"/>
       <c r="C99" s="1"/>
@@ -2694,9 +2590,8 @@
       <c r="O99" s="7"/>
       <c r="P99" s="7"/>
       <c r="Q99" s="1"/>
-      <c r="R99" s="1"/>
-    </row>
-    <row r="100" spans="1:18">
+    </row>
+    <row r="100" spans="1:17">
       <c r="A100" s="8"/>
       <c r="B100" s="5"/>
       <c r="C100" s="1"/>
@@ -2714,9 +2609,8 @@
       <c r="O100" s="7"/>
       <c r="P100" s="7"/>
       <c r="Q100" s="1"/>
-      <c r="R100" s="1"/>
-    </row>
-    <row r="101" spans="1:18">
+    </row>
+    <row r="101" spans="1:17">
       <c r="A101" s="8"/>
       <c r="B101" s="5"/>
       <c r="C101" s="1"/>
@@ -2734,9 +2628,8 @@
       <c r="O101" s="7"/>
       <c r="P101" s="7"/>
       <c r="Q101" s="1"/>
-      <c r="R101" s="1"/>
-    </row>
-    <row r="102" spans="1:18">
+    </row>
+    <row r="102" spans="1:17">
       <c r="A102" s="8"/>
       <c r="B102" s="5"/>
       <c r="C102" s="1"/>
@@ -2754,9 +2647,8 @@
       <c r="O102" s="7"/>
       <c r="P102" s="7"/>
       <c r="Q102" s="1"/>
-      <c r="R102" s="1"/>
-    </row>
-    <row r="103" spans="1:18">
+    </row>
+    <row r="103" spans="1:17">
       <c r="A103" s="8"/>
       <c r="B103" s="5"/>
       <c r="C103" s="1"/>
@@ -2774,9 +2666,8 @@
       <c r="O103" s="7"/>
       <c r="P103" s="7"/>
       <c r="Q103" s="1"/>
-      <c r="R103" s="1"/>
-    </row>
-    <row r="104" spans="1:18">
+    </row>
+    <row r="104" spans="1:17">
       <c r="A104" s="8"/>
       <c r="B104" s="5"/>
       <c r="C104" s="1"/>
@@ -2794,9 +2685,8 @@
       <c r="O104" s="7"/>
       <c r="P104" s="7"/>
       <c r="Q104" s="1"/>
-      <c r="R104" s="1"/>
-    </row>
-    <row r="105" spans="1:18">
+    </row>
+    <row r="105" spans="1:17">
       <c r="A105" s="8"/>
       <c r="B105" s="5"/>
       <c r="C105" s="1"/>
@@ -2814,9 +2704,8 @@
       <c r="O105" s="7"/>
       <c r="P105" s="7"/>
       <c r="Q105" s="1"/>
-      <c r="R105" s="1"/>
-    </row>
-    <row r="106" spans="1:18">
+    </row>
+    <row r="106" spans="1:17">
       <c r="A106" s="8"/>
       <c r="B106" s="5"/>
       <c r="C106" s="1"/>
@@ -2834,9 +2723,8 @@
       <c r="O106" s="7"/>
       <c r="P106" s="7"/>
       <c r="Q106" s="1"/>
-      <c r="R106" s="1"/>
-    </row>
-    <row r="107" spans="1:18">
+    </row>
+    <row r="107" spans="1:17">
       <c r="A107" s="8"/>
       <c r="B107" s="5"/>
       <c r="C107" s="1"/>
@@ -2854,9 +2742,8 @@
       <c r="O107" s="7"/>
       <c r="P107" s="7"/>
       <c r="Q107" s="1"/>
-      <c r="R107" s="1"/>
-    </row>
-    <row r="108" spans="1:18">
+    </row>
+    <row r="108" spans="1:17">
       <c r="A108" s="8"/>
       <c r="B108" s="5"/>
       <c r="C108" s="1"/>
@@ -2874,9 +2761,8 @@
       <c r="O108" s="7"/>
       <c r="P108" s="7"/>
       <c r="Q108" s="1"/>
-      <c r="R108" s="1"/>
-    </row>
-    <row r="109" spans="1:18">
+    </row>
+    <row r="109" spans="1:17">
       <c r="A109" s="8"/>
       <c r="B109" s="5"/>
       <c r="C109" s="1"/>
@@ -2894,9 +2780,8 @@
       <c r="O109" s="7"/>
       <c r="P109" s="7"/>
       <c r="Q109" s="1"/>
-      <c r="R109" s="1"/>
-    </row>
-    <row r="110" spans="1:18">
+    </row>
+    <row r="110" spans="1:17">
       <c r="A110" s="8"/>
       <c r="B110" s="5"/>
       <c r="C110" s="1"/>
@@ -2914,9 +2799,8 @@
       <c r="O110" s="7"/>
       <c r="P110" s="7"/>
       <c r="Q110" s="1"/>
-      <c r="R110" s="1"/>
-    </row>
-    <row r="111" spans="1:18">
+    </row>
+    <row r="111" spans="1:17">
       <c r="A111" s="8"/>
       <c r="B111" s="5"/>
       <c r="C111" s="1"/>
@@ -2934,9 +2818,8 @@
       <c r="O111" s="7"/>
       <c r="P111" s="7"/>
       <c r="Q111" s="1"/>
-      <c r="R111" s="1"/>
-    </row>
-    <row r="112" spans="1:18">
+    </row>
+    <row r="112" spans="1:17">
       <c r="A112" s="8"/>
       <c r="B112" s="5"/>
       <c r="C112" s="1"/>
@@ -2954,9 +2837,8 @@
       <c r="O112" s="7"/>
       <c r="P112" s="7"/>
       <c r="Q112" s="1"/>
-      <c r="R112" s="1"/>
-    </row>
-    <row r="113" spans="1:18">
+    </row>
+    <row r="113" spans="1:17">
       <c r="A113" s="8"/>
       <c r="B113" s="5"/>
       <c r="C113" s="1"/>
@@ -2974,9 +2856,8 @@
       <c r="O113" s="7"/>
       <c r="P113" s="7"/>
       <c r="Q113" s="1"/>
-      <c r="R113" s="1"/>
-    </row>
-    <row r="114" spans="1:18">
+    </row>
+    <row r="114" spans="1:17">
       <c r="A114" s="8"/>
       <c r="B114" s="5"/>
       <c r="C114" s="1"/>
@@ -2994,9 +2875,8 @@
       <c r="O114" s="7"/>
       <c r="P114" s="7"/>
       <c r="Q114" s="1"/>
-      <c r="R114" s="1"/>
-    </row>
-    <row r="115" spans="1:18">
+    </row>
+    <row r="115" spans="1:17">
       <c r="A115" s="8"/>
       <c r="B115" s="5"/>
       <c r="C115" s="1"/>
@@ -3014,9 +2894,8 @@
       <c r="O115" s="7"/>
       <c r="P115" s="7"/>
       <c r="Q115" s="1"/>
-      <c r="R115" s="1"/>
-    </row>
-    <row r="116" spans="1:18">
+    </row>
+    <row r="116" spans="1:17">
       <c r="A116" s="8"/>
       <c r="B116" s="5"/>
       <c r="C116" s="1"/>
@@ -3034,9 +2913,8 @@
       <c r="O116" s="7"/>
       <c r="P116" s="7"/>
       <c r="Q116" s="1"/>
-      <c r="R116" s="1"/>
-    </row>
-    <row r="117" spans="1:18">
+    </row>
+    <row r="117" spans="1:17">
       <c r="A117" s="8"/>
       <c r="B117" s="5"/>
       <c r="C117" s="1"/>
@@ -3054,9 +2932,8 @@
       <c r="O117" s="7"/>
       <c r="P117" s="7"/>
       <c r="Q117" s="1"/>
-      <c r="R117" s="1"/>
-    </row>
-    <row r="118" spans="1:18">
+    </row>
+    <row r="118" spans="1:17">
       <c r="A118" s="8"/>
       <c r="B118" s="5"/>
       <c r="C118" s="1"/>
@@ -3074,9 +2951,8 @@
       <c r="O118" s="7"/>
       <c r="P118" s="7"/>
       <c r="Q118" s="1"/>
-      <c r="R118" s="1"/>
-    </row>
-    <row r="119" spans="1:18">
+    </row>
+    <row r="119" spans="1:17">
       <c r="A119" s="8"/>
       <c r="B119" s="5"/>
       <c r="C119" s="1"/>
@@ -3094,9 +2970,8 @@
       <c r="O119" s="7"/>
       <c r="P119" s="7"/>
       <c r="Q119" s="1"/>
-      <c r="R119" s="1"/>
-    </row>
-    <row r="120" spans="1:18">
+    </row>
+    <row r="120" spans="1:17">
       <c r="A120" s="8"/>
       <c r="B120" s="5"/>
       <c r="C120" s="1"/>
@@ -3114,9 +2989,8 @@
       <c r="O120" s="7"/>
       <c r="P120" s="7"/>
       <c r="Q120" s="1"/>
-      <c r="R120" s="1"/>
-    </row>
-    <row r="121" spans="1:18">
+    </row>
+    <row r="121" spans="1:17">
       <c r="A121" s="8"/>
       <c r="B121" s="5"/>
       <c r="C121" s="1"/>
@@ -3134,9 +3008,8 @@
       <c r="O121" s="7"/>
       <c r="P121" s="7"/>
       <c r="Q121" s="1"/>
-      <c r="R121" s="1"/>
-    </row>
-    <row r="122" spans="1:18">
+    </row>
+    <row r="122" spans="1:17">
       <c r="A122" s="8"/>
       <c r="B122" s="5"/>
       <c r="C122" s="1"/>
@@ -3154,9 +3027,8 @@
       <c r="O122" s="7"/>
       <c r="P122" s="7"/>
       <c r="Q122" s="1"/>
-      <c r="R122" s="1"/>
-    </row>
-    <row r="123" spans="1:18">
+    </row>
+    <row r="123" spans="1:17">
       <c r="A123" s="8"/>
       <c r="B123" s="5"/>
       <c r="C123" s="1"/>
@@ -3174,9 +3046,8 @@
       <c r="O123" s="7"/>
       <c r="P123" s="7"/>
       <c r="Q123" s="1"/>
-      <c r="R123" s="1"/>
-    </row>
-    <row r="124" spans="1:18">
+    </row>
+    <row r="124" spans="1:17">
       <c r="A124" s="8"/>
       <c r="B124" s="5"/>
       <c r="C124" s="1"/>
@@ -3194,9 +3065,8 @@
       <c r="O124" s="7"/>
       <c r="P124" s="7"/>
       <c r="Q124" s="1"/>
-      <c r="R124" s="1"/>
-    </row>
-    <row r="125" spans="1:18">
+    </row>
+    <row r="125" spans="1:17">
       <c r="A125" s="8"/>
       <c r="B125" s="5"/>
       <c r="C125" s="1"/>
@@ -3214,9 +3084,8 @@
       <c r="O125" s="7"/>
       <c r="P125" s="7"/>
       <c r="Q125" s="1"/>
-      <c r="R125" s="1"/>
-    </row>
-    <row r="126" spans="1:18">
+    </row>
+    <row r="126" spans="1:17">
       <c r="A126" s="8"/>
       <c r="B126" s="5"/>
       <c r="C126" s="1"/>
@@ -3234,9 +3103,8 @@
       <c r="O126" s="7"/>
       <c r="P126" s="7"/>
       <c r="Q126" s="1"/>
-      <c r="R126" s="1"/>
-    </row>
-    <row r="127" spans="1:18">
+    </row>
+    <row r="127" spans="1:17">
       <c r="A127" s="8"/>
       <c r="B127" s="5"/>
       <c r="C127" s="1"/>
@@ -3254,9 +3122,8 @@
       <c r="O127" s="7"/>
       <c r="P127" s="7"/>
       <c r="Q127" s="1"/>
-      <c r="R127" s="1"/>
-    </row>
-    <row r="128" spans="1:18">
+    </row>
+    <row r="128" spans="1:17">
       <c r="A128" s="8"/>
       <c r="B128" s="5"/>
       <c r="C128" s="1"/>
@@ -3274,9 +3141,8 @@
       <c r="O128" s="7"/>
       <c r="P128" s="7"/>
       <c r="Q128" s="1"/>
-      <c r="R128" s="1"/>
-    </row>
-    <row r="129" spans="1:18">
+    </row>
+    <row r="129" spans="1:17">
       <c r="A129" s="8"/>
       <c r="B129" s="5"/>
       <c r="C129" s="1"/>
@@ -3294,9 +3160,8 @@
       <c r="O129" s="7"/>
       <c r="P129" s="7"/>
       <c r="Q129" s="1"/>
-      <c r="R129" s="1"/>
-    </row>
-    <row r="130" spans="1:18">
+    </row>
+    <row r="130" spans="1:17">
       <c r="A130" s="8"/>
       <c r="B130" s="5"/>
       <c r="C130" s="1"/>
@@ -3314,9 +3179,8 @@
       <c r="O130" s="7"/>
       <c r="P130" s="7"/>
       <c r="Q130" s="1"/>
-      <c r="R130" s="1"/>
-    </row>
-    <row r="131" spans="1:18">
+    </row>
+    <row r="131" spans="1:17">
       <c r="A131" s="8"/>
       <c r="B131" s="5"/>
       <c r="C131" s="1"/>
@@ -3334,9 +3198,8 @@
       <c r="O131" s="7"/>
       <c r="P131" s="7"/>
       <c r="Q131" s="1"/>
-      <c r="R131" s="1"/>
-    </row>
-    <row r="132" spans="1:18">
+    </row>
+    <row r="132" spans="1:17">
       <c r="A132" s="8"/>
       <c r="B132" s="5"/>
       <c r="C132" s="1"/>
@@ -3354,9 +3217,8 @@
       <c r="O132" s="7"/>
       <c r="P132" s="7"/>
       <c r="Q132" s="1"/>
-      <c r="R132" s="1"/>
-    </row>
-    <row r="133" spans="1:18">
+    </row>
+    <row r="133" spans="1:17">
       <c r="A133" s="8"/>
       <c r="B133" s="5"/>
       <c r="C133" s="1"/>
@@ -3374,9 +3236,8 @@
       <c r="O133" s="7"/>
       <c r="P133" s="7"/>
       <c r="Q133" s="1"/>
-      <c r="R133" s="1"/>
-    </row>
-    <row r="134" spans="1:18">
+    </row>
+    <row r="134" spans="1:17">
       <c r="A134" s="8"/>
       <c r="B134" s="5"/>
       <c r="C134" s="1"/>
@@ -3394,9 +3255,8 @@
       <c r="O134" s="7"/>
       <c r="P134" s="7"/>
       <c r="Q134" s="1"/>
-      <c r="R134" s="1"/>
-    </row>
-    <row r="135" spans="1:18">
+    </row>
+    <row r="135" spans="1:17">
       <c r="A135" s="8"/>
       <c r="B135" s="5"/>
       <c r="C135" s="1"/>
@@ -3414,9 +3274,8 @@
       <c r="O135" s="7"/>
       <c r="P135" s="7"/>
       <c r="Q135" s="1"/>
-      <c r="R135" s="1"/>
-    </row>
-    <row r="136" spans="1:18">
+    </row>
+    <row r="136" spans="1:17">
       <c r="A136" s="8"/>
       <c r="B136" s="5"/>
       <c r="C136" s="1"/>
@@ -3434,9 +3293,8 @@
       <c r="O136" s="7"/>
       <c r="P136" s="7"/>
       <c r="Q136" s="1"/>
-      <c r="R136" s="1"/>
-    </row>
-    <row r="137" spans="1:18">
+    </row>
+    <row r="137" spans="1:17">
       <c r="A137" s="8"/>
       <c r="B137" s="5"/>
       <c r="C137" s="1"/>
@@ -3454,9 +3312,8 @@
       <c r="O137" s="7"/>
       <c r="P137" s="7"/>
       <c r="Q137" s="1"/>
-      <c r="R137" s="1"/>
-    </row>
-    <row r="138" spans="1:18">
+    </row>
+    <row r="138" spans="1:17">
       <c r="A138" s="8"/>
       <c r="B138" s="5"/>
       <c r="C138" s="1"/>
@@ -3474,9 +3331,8 @@
       <c r="O138" s="7"/>
       <c r="P138" s="7"/>
       <c r="Q138" s="1"/>
-      <c r="R138" s="1"/>
-    </row>
-    <row r="139" spans="1:18">
+    </row>
+    <row r="139" spans="1:17">
       <c r="A139" s="8"/>
       <c r="B139" s="5"/>
       <c r="C139" s="1"/>
@@ -3494,9 +3350,8 @@
       <c r="O139" s="7"/>
       <c r="P139" s="7"/>
       <c r="Q139" s="1"/>
-      <c r="R139" s="1"/>
-    </row>
-    <row r="140" spans="1:18">
+    </row>
+    <row r="140" spans="1:17">
       <c r="A140" s="8"/>
       <c r="B140" s="5"/>
       <c r="C140" s="1"/>
@@ -3514,9 +3369,8 @@
       <c r="O140" s="7"/>
       <c r="P140" s="7"/>
       <c r="Q140" s="1"/>
-      <c r="R140" s="1"/>
-    </row>
-    <row r="141" spans="1:18">
+    </row>
+    <row r="141" spans="1:17">
       <c r="A141" s="8"/>
       <c r="B141" s="5"/>
       <c r="C141" s="1"/>
@@ -3534,9 +3388,8 @@
       <c r="O141" s="7"/>
       <c r="P141" s="7"/>
       <c r="Q141" s="1"/>
-      <c r="R141" s="1"/>
-    </row>
-    <row r="142" spans="1:18">
+    </row>
+    <row r="142" spans="1:17">
       <c r="A142" s="8"/>
       <c r="B142" s="5"/>
       <c r="C142" s="1"/>
@@ -3554,9 +3407,8 @@
       <c r="O142" s="7"/>
       <c r="P142" s="7"/>
       <c r="Q142" s="1"/>
-      <c r="R142" s="1"/>
-    </row>
-    <row r="143" spans="1:18">
+    </row>
+    <row r="143" spans="1:17">
       <c r="A143" s="8"/>
       <c r="B143" s="5"/>
       <c r="C143" s="1"/>
@@ -3574,9 +3426,8 @@
       <c r="O143" s="7"/>
       <c r="P143" s="7"/>
       <c r="Q143" s="1"/>
-      <c r="R143" s="1"/>
-    </row>
-    <row r="144" spans="1:18">
+    </row>
+    <row r="144" spans="1:17">
       <c r="A144" s="8"/>
       <c r="B144" s="5"/>
       <c r="C144" s="1"/>
@@ -3594,9 +3445,8 @@
       <c r="O144" s="7"/>
       <c r="P144" s="7"/>
       <c r="Q144" s="1"/>
-      <c r="R144" s="1"/>
-    </row>
-    <row r="145" spans="1:18">
+    </row>
+    <row r="145" spans="1:17">
       <c r="A145" s="8"/>
       <c r="B145" s="5"/>
       <c r="C145" s="1"/>
@@ -3614,9 +3464,8 @@
       <c r="O145" s="7"/>
       <c r="P145" s="7"/>
       <c r="Q145" s="1"/>
-      <c r="R145" s="1"/>
-    </row>
-    <row r="146" spans="1:18">
+    </row>
+    <row r="146" spans="1:17">
       <c r="A146" s="8"/>
       <c r="B146" s="5"/>
       <c r="C146" s="1"/>
@@ -3634,9 +3483,8 @@
       <c r="O146" s="7"/>
       <c r="P146" s="7"/>
       <c r="Q146" s="1"/>
-      <c r="R146" s="1"/>
-    </row>
-    <row r="147" spans="1:18">
+    </row>
+    <row r="147" spans="1:17">
       <c r="A147" s="8"/>
       <c r="B147" s="5"/>
       <c r="C147" s="1"/>
@@ -3654,9 +3502,8 @@
       <c r="O147" s="7"/>
       <c r="P147" s="7"/>
       <c r="Q147" s="1"/>
-      <c r="R147" s="1"/>
-    </row>
-    <row r="148" spans="1:18">
+    </row>
+    <row r="148" spans="1:17">
       <c r="A148" s="8"/>
       <c r="B148" s="5"/>
       <c r="C148" s="1"/>
@@ -3674,9 +3521,8 @@
       <c r="O148" s="7"/>
       <c r="P148" s="7"/>
       <c r="Q148" s="1"/>
-      <c r="R148" s="1"/>
-    </row>
-    <row r="149" spans="1:18">
+    </row>
+    <row r="149" spans="1:17">
       <c r="A149" s="8"/>
       <c r="B149" s="5"/>
       <c r="C149" s="1"/>
@@ -3694,9 +3540,8 @@
       <c r="O149" s="7"/>
       <c r="P149" s="7"/>
       <c r="Q149" s="1"/>
-      <c r="R149" s="1"/>
-    </row>
-    <row r="150" spans="1:18">
+    </row>
+    <row r="150" spans="1:17">
       <c r="A150" s="8"/>
       <c r="B150" s="5"/>
       <c r="C150" s="1"/>
@@ -3714,9 +3559,8 @@
       <c r="O150" s="7"/>
       <c r="P150" s="7"/>
       <c r="Q150" s="1"/>
-      <c r="R150" s="1"/>
-    </row>
-    <row r="151" spans="1:18">
+    </row>
+    <row r="151" spans="1:17">
       <c r="A151" s="8"/>
       <c r="B151" s="5"/>
       <c r="C151" s="1"/>
@@ -3734,9 +3578,8 @@
       <c r="O151" s="7"/>
       <c r="P151" s="7"/>
       <c r="Q151" s="1"/>
-      <c r="R151" s="1"/>
-    </row>
-    <row r="152" spans="1:18">
+    </row>
+    <row r="152" spans="1:17">
       <c r="A152" s="8"/>
       <c r="B152" s="5"/>
       <c r="C152" s="1"/>
@@ -3754,9 +3597,8 @@
       <c r="O152" s="7"/>
       <c r="P152" s="7"/>
       <c r="Q152" s="1"/>
-      <c r="R152" s="1"/>
-    </row>
-    <row r="153" spans="1:18">
+    </row>
+    <row r="153" spans="1:17">
       <c r="A153" s="8"/>
       <c r="B153" s="5"/>
       <c r="C153" s="1"/>
@@ -3774,9 +3616,8 @@
       <c r="O153" s="7"/>
       <c r="P153" s="7"/>
       <c r="Q153" s="1"/>
-      <c r="R153" s="1"/>
-    </row>
-    <row r="154" spans="1:18">
+    </row>
+    <row r="154" spans="1:17">
       <c r="A154" s="8"/>
       <c r="B154" s="5"/>
       <c r="C154" s="1"/>
@@ -3794,9 +3635,8 @@
       <c r="O154" s="7"/>
       <c r="P154" s="7"/>
       <c r="Q154" s="1"/>
-      <c r="R154" s="1"/>
-    </row>
-    <row r="155" spans="1:18">
+    </row>
+    <row r="155" spans="1:17">
       <c r="A155" s="8"/>
       <c r="B155" s="5"/>
       <c r="C155" s="1"/>
@@ -3814,9 +3654,8 @@
       <c r="O155" s="7"/>
       <c r="P155" s="7"/>
       <c r="Q155" s="1"/>
-      <c r="R155" s="1"/>
-    </row>
-    <row r="156" spans="1:18">
+    </row>
+    <row r="156" spans="1:17">
       <c r="A156" s="8"/>
       <c r="B156" s="5"/>
       <c r="C156" s="1"/>
@@ -3834,9 +3673,8 @@
       <c r="O156" s="7"/>
       <c r="P156" s="7"/>
       <c r="Q156" s="1"/>
-      <c r="R156" s="1"/>
-    </row>
-    <row r="157" spans="1:18">
+    </row>
+    <row r="157" spans="1:17">
       <c r="A157" s="8"/>
       <c r="B157" s="5"/>
       <c r="C157" s="1"/>
@@ -3854,9 +3692,8 @@
       <c r="O157" s="7"/>
       <c r="P157" s="7"/>
       <c r="Q157" s="1"/>
-      <c r="R157" s="1"/>
-    </row>
-    <row r="158" spans="1:18">
+    </row>
+    <row r="158" spans="1:17">
       <c r="A158" s="8"/>
       <c r="B158" s="5"/>
       <c r="C158" s="1"/>
@@ -3874,9 +3711,8 @@
       <c r="O158" s="7"/>
       <c r="P158" s="7"/>
       <c r="Q158" s="1"/>
-      <c r="R158" s="1"/>
-    </row>
-    <row r="159" spans="1:18">
+    </row>
+    <row r="159" spans="1:17">
       <c r="A159" s="8"/>
       <c r="B159" s="5"/>
       <c r="C159" s="1"/>
@@ -3894,9 +3730,8 @@
       <c r="O159" s="7"/>
       <c r="P159" s="7"/>
       <c r="Q159" s="1"/>
-      <c r="R159" s="1"/>
-    </row>
-    <row r="160" spans="1:18">
+    </row>
+    <row r="160" spans="1:17">
       <c r="A160" s="8"/>
       <c r="B160" s="5"/>
       <c r="C160" s="1"/>
@@ -3914,9 +3749,8 @@
       <c r="O160" s="7"/>
       <c r="P160" s="7"/>
       <c r="Q160" s="1"/>
-      <c r="R160" s="1"/>
-    </row>
-    <row r="161" spans="1:18">
+    </row>
+    <row r="161" spans="1:17">
       <c r="A161" s="8"/>
       <c r="B161" s="5"/>
       <c r="C161" s="1"/>
@@ -3934,9 +3768,8 @@
       <c r="O161" s="7"/>
       <c r="P161" s="7"/>
       <c r="Q161" s="1"/>
-      <c r="R161" s="1"/>
-    </row>
-    <row r="162" spans="1:18">
+    </row>
+    <row r="162" spans="1:17">
       <c r="A162" s="8"/>
       <c r="B162" s="5"/>
       <c r="C162" s="1"/>
@@ -3954,9 +3787,8 @@
       <c r="O162" s="7"/>
       <c r="P162" s="7"/>
       <c r="Q162" s="1"/>
-      <c r="R162" s="1"/>
-    </row>
-    <row r="163" spans="1:18">
+    </row>
+    <row r="163" spans="1:17">
       <c r="A163" s="8"/>
       <c r="B163" s="5"/>
       <c r="C163" s="1"/>
@@ -3974,9 +3806,8 @@
       <c r="O163" s="7"/>
       <c r="P163" s="7"/>
       <c r="Q163" s="1"/>
-      <c r="R163" s="1"/>
-    </row>
-    <row r="164" spans="1:18">
+    </row>
+    <row r="164" spans="1:17">
       <c r="A164" s="8"/>
       <c r="B164" s="5"/>
       <c r="C164" s="1"/>
@@ -3994,9 +3825,8 @@
       <c r="O164" s="7"/>
       <c r="P164" s="7"/>
       <c r="Q164" s="1"/>
-      <c r="R164" s="1"/>
-    </row>
-    <row r="165" spans="1:18">
+    </row>
+    <row r="165" spans="1:17">
       <c r="A165" s="8"/>
       <c r="B165" s="5"/>
       <c r="C165" s="1"/>
@@ -4014,9 +3844,8 @@
       <c r="O165" s="7"/>
       <c r="P165" s="7"/>
       <c r="Q165" s="1"/>
-      <c r="R165" s="1"/>
-    </row>
-    <row r="166" spans="1:18">
+    </row>
+    <row r="166" spans="1:17">
       <c r="A166" s="8"/>
       <c r="B166" s="5"/>
       <c r="C166" s="1"/>
@@ -4034,9 +3863,8 @@
       <c r="O166" s="7"/>
       <c r="P166" s="7"/>
       <c r="Q166" s="1"/>
-      <c r="R166" s="1"/>
-    </row>
-    <row r="167" spans="1:18">
+    </row>
+    <row r="167" spans="1:17">
       <c r="A167" s="8"/>
       <c r="B167" s="5"/>
       <c r="C167" s="1"/>
@@ -4054,9 +3882,8 @@
       <c r="O167" s="7"/>
       <c r="P167" s="7"/>
       <c r="Q167" s="1"/>
-      <c r="R167" s="1"/>
-    </row>
-    <row r="168" spans="1:18">
+    </row>
+    <row r="168" spans="1:17">
       <c r="A168" s="8"/>
       <c r="B168" s="5"/>
       <c r="C168" s="1"/>
@@ -4074,9 +3901,8 @@
       <c r="O168" s="7"/>
       <c r="P168" s="7"/>
       <c r="Q168" s="1"/>
-      <c r="R168" s="1"/>
-    </row>
-    <row r="169" spans="1:18">
+    </row>
+    <row r="169" spans="1:17">
       <c r="A169" s="8"/>
       <c r="B169" s="5"/>
       <c r="C169" s="1"/>
@@ -4094,9 +3920,8 @@
       <c r="O169" s="7"/>
       <c r="P169" s="7"/>
       <c r="Q169" s="1"/>
-      <c r="R169" s="1"/>
-    </row>
-    <row r="170" spans="1:18">
+    </row>
+    <row r="170" spans="1:17">
       <c r="A170" s="8"/>
       <c r="B170" s="5"/>
       <c r="C170" s="1"/>
@@ -4114,9 +3939,8 @@
       <c r="O170" s="7"/>
       <c r="P170" s="7"/>
       <c r="Q170" s="1"/>
-      <c r="R170" s="1"/>
-    </row>
-    <row r="171" spans="1:18">
+    </row>
+    <row r="171" spans="1:17">
       <c r="A171" s="8"/>
       <c r="B171" s="5"/>
       <c r="C171" s="1"/>
@@ -4134,9 +3958,8 @@
       <c r="O171" s="7"/>
       <c r="P171" s="7"/>
       <c r="Q171" s="1"/>
-      <c r="R171" s="1"/>
-    </row>
-    <row r="172" spans="1:18">
+    </row>
+    <row r="172" spans="1:17">
       <c r="A172" s="8"/>
       <c r="B172" s="5"/>
       <c r="C172" s="1"/>
@@ -4154,9 +3977,8 @@
       <c r="O172" s="7"/>
       <c r="P172" s="7"/>
       <c r="Q172" s="1"/>
-      <c r="R172" s="1"/>
-    </row>
-    <row r="173" spans="1:18">
+    </row>
+    <row r="173" spans="1:17">
       <c r="A173" s="8"/>
       <c r="B173" s="5"/>
       <c r="C173" s="1"/>
@@ -4174,9 +3996,8 @@
       <c r="O173" s="7"/>
       <c r="P173" s="7"/>
       <c r="Q173" s="1"/>
-      <c r="R173" s="1"/>
-    </row>
-    <row r="174" spans="1:18">
+    </row>
+    <row r="174" spans="1:17">
       <c r="A174" s="8"/>
       <c r="B174" s="5"/>
       <c r="C174" s="1"/>
@@ -4194,9 +4015,8 @@
       <c r="O174" s="7"/>
       <c r="P174" s="7"/>
       <c r="Q174" s="1"/>
-      <c r="R174" s="1"/>
-    </row>
-    <row r="175" spans="1:18">
+    </row>
+    <row r="175" spans="1:17">
       <c r="A175" s="8"/>
       <c r="B175" s="5"/>
       <c r="C175" s="1"/>
@@ -4214,9 +4034,8 @@
       <c r="O175" s="7"/>
       <c r="P175" s="7"/>
       <c r="Q175" s="1"/>
-      <c r="R175" s="1"/>
-    </row>
-    <row r="176" spans="1:18">
+    </row>
+    <row r="176" spans="1:17">
       <c r="A176" s="8"/>
       <c r="B176" s="5"/>
       <c r="C176" s="1"/>
@@ -4234,9 +4053,8 @@
       <c r="O176" s="7"/>
       <c r="P176" s="7"/>
       <c r="Q176" s="1"/>
-      <c r="R176" s="1"/>
-    </row>
-    <row r="177" spans="1:18">
+    </row>
+    <row r="177" spans="1:17">
       <c r="A177" s="8"/>
       <c r="B177" s="5"/>
       <c r="C177" s="1"/>
@@ -4254,9 +4072,8 @@
       <c r="O177" s="7"/>
       <c r="P177" s="7"/>
       <c r="Q177" s="1"/>
-      <c r="R177" s="1"/>
-    </row>
-    <row r="178" spans="1:18">
+    </row>
+    <row r="178" spans="1:17">
       <c r="A178" s="8"/>
       <c r="B178" s="5"/>
       <c r="C178" s="1"/>
@@ -4274,9 +4091,8 @@
       <c r="O178" s="7"/>
       <c r="P178" s="7"/>
       <c r="Q178" s="1"/>
-      <c r="R178" s="1"/>
-    </row>
-    <row r="179" spans="1:18">
+    </row>
+    <row r="179" spans="1:17">
       <c r="A179" s="8"/>
       <c r="B179" s="5"/>
       <c r="C179" s="1"/>
@@ -4294,9 +4110,8 @@
       <c r="O179" s="7"/>
       <c r="P179" s="7"/>
       <c r="Q179" s="1"/>
-      <c r="R179" s="1"/>
-    </row>
-    <row r="180" spans="1:18">
+    </row>
+    <row r="180" spans="1:17">
       <c r="A180" s="8"/>
       <c r="B180" s="5"/>
       <c r="C180" s="1"/>
@@ -4314,9 +4129,8 @@
       <c r="O180" s="7"/>
       <c r="P180" s="7"/>
       <c r="Q180" s="1"/>
-      <c r="R180" s="1"/>
-    </row>
-    <row r="181" spans="1:18">
+    </row>
+    <row r="181" spans="1:17">
       <c r="A181" s="8"/>
       <c r="B181" s="5"/>
       <c r="C181" s="1"/>
@@ -4334,9 +4148,8 @@
       <c r="O181" s="7"/>
       <c r="P181" s="7"/>
       <c r="Q181" s="1"/>
-      <c r="R181" s="1"/>
-    </row>
-    <row r="182" spans="1:18">
+    </row>
+    <row r="182" spans="1:17">
       <c r="A182" s="8"/>
       <c r="B182" s="5"/>
       <c r="C182" s="1"/>
@@ -4354,9 +4167,8 @@
       <c r="O182" s="7"/>
       <c r="P182" s="7"/>
       <c r="Q182" s="1"/>
-      <c r="R182" s="1"/>
-    </row>
-    <row r="183" spans="1:18">
+    </row>
+    <row r="183" spans="1:17">
       <c r="A183" s="8"/>
       <c r="B183" s="5"/>
       <c r="C183" s="1"/>
@@ -4374,9 +4186,8 @@
       <c r="O183" s="7"/>
       <c r="P183" s="7"/>
       <c r="Q183" s="1"/>
-      <c r="R183" s="1"/>
-    </row>
-    <row r="184" spans="1:18">
+    </row>
+    <row r="184" spans="1:17">
       <c r="A184" s="8"/>
       <c r="B184" s="5"/>
       <c r="C184" s="1"/>
@@ -4394,9 +4205,8 @@
       <c r="O184" s="7"/>
       <c r="P184" s="7"/>
       <c r="Q184" s="1"/>
-      <c r="R184" s="1"/>
-    </row>
-    <row r="185" spans="1:18">
+    </row>
+    <row r="185" spans="1:17">
       <c r="A185" s="8"/>
       <c r="B185" s="5"/>
       <c r="C185" s="1"/>
@@ -4414,9 +4224,8 @@
       <c r="O185" s="7"/>
       <c r="P185" s="7"/>
       <c r="Q185" s="1"/>
-      <c r="R185" s="1"/>
-    </row>
-    <row r="186" spans="1:18">
+    </row>
+    <row r="186" spans="1:17">
       <c r="A186" s="8"/>
       <c r="B186" s="5"/>
       <c r="C186" s="1"/>
@@ -4434,9 +4243,8 @@
       <c r="O186" s="7"/>
       <c r="P186" s="7"/>
       <c r="Q186" s="1"/>
-      <c r="R186" s="1"/>
-    </row>
-    <row r="187" spans="1:18">
+    </row>
+    <row r="187" spans="1:17">
       <c r="A187" s="8"/>
       <c r="B187" s="5"/>
       <c r="C187" s="1"/>
@@ -4454,9 +4262,8 @@
       <c r="O187" s="7"/>
       <c r="P187" s="7"/>
       <c r="Q187" s="1"/>
-      <c r="R187" s="1"/>
-    </row>
-    <row r="188" spans="1:18">
+    </row>
+    <row r="188" spans="1:17">
       <c r="A188" s="8"/>
       <c r="B188" s="5"/>
       <c r="C188" s="1"/>
@@ -4474,9 +4281,8 @@
       <c r="O188" s="7"/>
       <c r="P188" s="7"/>
       <c r="Q188" s="1"/>
-      <c r="R188" s="1"/>
-    </row>
-    <row r="189" spans="1:18">
+    </row>
+    <row r="189" spans="1:17">
       <c r="A189" s="8"/>
       <c r="B189" s="5"/>
       <c r="C189" s="1"/>
@@ -4494,9 +4300,8 @@
       <c r="O189" s="7"/>
       <c r="P189" s="7"/>
       <c r="Q189" s="1"/>
-      <c r="R189" s="1"/>
-    </row>
-    <row r="190" spans="1:18">
+    </row>
+    <row r="190" spans="1:17">
       <c r="A190" s="8"/>
       <c r="B190" s="5"/>
       <c r="C190" s="1"/>
@@ -4514,9 +4319,8 @@
       <c r="O190" s="7"/>
       <c r="P190" s="7"/>
       <c r="Q190" s="1"/>
-      <c r="R190" s="1"/>
-    </row>
-    <row r="191" spans="1:18">
+    </row>
+    <row r="191" spans="1:17">
       <c r="A191" s="8"/>
       <c r="B191" s="5"/>
       <c r="C191" s="1"/>
@@ -4534,9 +4338,8 @@
       <c r="O191" s="7"/>
       <c r="P191" s="7"/>
       <c r="Q191" s="1"/>
-      <c r="R191" s="1"/>
-    </row>
-    <row r="192" spans="1:18">
+    </row>
+    <row r="192" spans="1:17">
       <c r="A192" s="8"/>
       <c r="B192" s="5"/>
       <c r="C192" s="1"/>
@@ -4554,9 +4357,8 @@
       <c r="O192" s="7"/>
       <c r="P192" s="7"/>
       <c r="Q192" s="1"/>
-      <c r="R192" s="1"/>
-    </row>
-    <row r="193" spans="1:18">
+    </row>
+    <row r="193" spans="1:17">
       <c r="A193" s="8"/>
       <c r="B193" s="5"/>
       <c r="C193" s="1"/>
@@ -4574,9 +4376,8 @@
       <c r="O193" s="7"/>
       <c r="P193" s="7"/>
       <c r="Q193" s="1"/>
-      <c r="R193" s="1"/>
-    </row>
-    <row r="194" spans="1:18">
+    </row>
+    <row r="194" spans="1:17">
       <c r="A194" s="8"/>
       <c r="B194" s="5"/>
       <c r="C194" s="1"/>
@@ -4594,9 +4395,8 @@
       <c r="O194" s="7"/>
       <c r="P194" s="7"/>
       <c r="Q194" s="1"/>
-      <c r="R194" s="1"/>
-    </row>
-    <row r="195" spans="1:18">
+    </row>
+    <row r="195" spans="1:17">
       <c r="A195" s="8"/>
       <c r="B195" s="5"/>
       <c r="C195" s="1"/>
@@ -4614,9 +4414,8 @@
       <c r="O195" s="7"/>
       <c r="P195" s="7"/>
       <c r="Q195" s="1"/>
-      <c r="R195" s="1"/>
-    </row>
-    <row r="196" spans="1:18">
+    </row>
+    <row r="196" spans="1:17">
       <c r="A196" s="8"/>
       <c r="B196" s="5"/>
       <c r="C196" s="1"/>
@@ -4634,9 +4433,8 @@
       <c r="O196" s="7"/>
       <c r="P196" s="7"/>
       <c r="Q196" s="1"/>
-      <c r="R196" s="1"/>
-    </row>
-    <row r="197" spans="1:18">
+    </row>
+    <row r="197" spans="1:17">
       <c r="A197" s="8"/>
       <c r="B197" s="5"/>
       <c r="C197" s="1"/>
@@ -4654,9 +4452,8 @@
       <c r="O197" s="7"/>
       <c r="P197" s="7"/>
       <c r="Q197" s="1"/>
-      <c r="R197" s="1"/>
-    </row>
-    <row r="198" spans="1:18">
+    </row>
+    <row r="198" spans="1:17">
       <c r="A198" s="8"/>
       <c r="B198" s="5"/>
       <c r="C198" s="1"/>
@@ -4674,9 +4471,8 @@
       <c r="O198" s="7"/>
       <c r="P198" s="7"/>
       <c r="Q198" s="1"/>
-      <c r="R198" s="1"/>
-    </row>
-    <row r="199" spans="1:18">
+    </row>
+    <row r="199" spans="1:17">
       <c r="A199" s="8"/>
       <c r="B199" s="5"/>
       <c r="C199" s="1"/>
@@ -4694,9 +4490,8 @@
       <c r="O199" s="7"/>
       <c r="P199" s="7"/>
       <c r="Q199" s="1"/>
-      <c r="R199" s="1"/>
-    </row>
-    <row r="200" spans="1:18">
+    </row>
+    <row r="200" spans="1:17">
       <c r="A200" s="8"/>
       <c r="B200" s="5"/>
       <c r="C200" s="1"/>
@@ -4714,9 +4509,8 @@
       <c r="O200" s="7"/>
       <c r="P200" s="7"/>
       <c r="Q200" s="1"/>
-      <c r="R200" s="1"/>
-    </row>
-    <row r="201" spans="1:18">
+    </row>
+    <row r="201" spans="1:17">
       <c r="A201" s="8"/>
       <c r="B201" s="5"/>
       <c r="C201" s="1"/>
@@ -4734,9 +4528,8 @@
       <c r="O201" s="7"/>
       <c r="P201" s="7"/>
       <c r="Q201" s="1"/>
-      <c r="R201" s="1"/>
-    </row>
-    <row r="202" spans="1:18">
+    </row>
+    <row r="202" spans="1:17">
       <c r="A202" s="8"/>
       <c r="B202" s="5"/>
       <c r="C202" s="1"/>
@@ -4754,9 +4547,8 @@
       <c r="O202" s="7"/>
       <c r="P202" s="7"/>
       <c r="Q202" s="1"/>
-      <c r="R202" s="1"/>
-    </row>
-    <row r="203" spans="1:18">
+    </row>
+    <row r="203" spans="1:17">
       <c r="A203" s="8"/>
       <c r="B203" s="5"/>
       <c r="C203" s="1"/>
@@ -4774,9 +4566,8 @@
       <c r="O203" s="7"/>
       <c r="P203" s="7"/>
       <c r="Q203" s="1"/>
-      <c r="R203" s="1"/>
-    </row>
-    <row r="204" spans="1:18">
+    </row>
+    <row r="204" spans="1:17">
       <c r="A204" s="8"/>
       <c r="B204" s="5"/>
       <c r="C204" s="1"/>
@@ -4794,9 +4585,8 @@
       <c r="O204" s="7"/>
       <c r="P204" s="7"/>
       <c r="Q204" s="1"/>
-      <c r="R204" s="1"/>
-    </row>
-    <row r="205" spans="1:18">
+    </row>
+    <row r="205" spans="1:17">
       <c r="A205" s="8"/>
       <c r="B205" s="5"/>
       <c r="C205" s="1"/>
@@ -4814,9 +4604,8 @@
       <c r="O205" s="7"/>
       <c r="P205" s="7"/>
       <c r="Q205" s="1"/>
-      <c r="R205" s="1"/>
-    </row>
-    <row r="206" spans="1:18">
+    </row>
+    <row r="206" spans="1:17">
       <c r="A206" s="8"/>
       <c r="B206" s="5"/>
       <c r="C206" s="1"/>
@@ -4834,9 +4623,8 @@
       <c r="O206" s="7"/>
       <c r="P206" s="7"/>
       <c r="Q206" s="1"/>
-      <c r="R206" s="1"/>
-    </row>
-    <row r="207" spans="1:18">
+    </row>
+    <row r="207" spans="1:17">
       <c r="A207" s="8"/>
       <c r="B207" s="5"/>
       <c r="C207" s="1"/>
@@ -4854,9 +4642,8 @@
       <c r="O207" s="7"/>
       <c r="P207" s="7"/>
       <c r="Q207" s="1"/>
-      <c r="R207" s="1"/>
-    </row>
-    <row r="208" spans="1:18">
+    </row>
+    <row r="208" spans="1:17">
       <c r="A208" s="8"/>
       <c r="B208" s="5"/>
       <c r="C208" s="1"/>
@@ -4874,9 +4661,8 @@
       <c r="O208" s="7"/>
       <c r="P208" s="7"/>
       <c r="Q208" s="1"/>
-      <c r="R208" s="1"/>
-    </row>
-    <row r="209" spans="1:18">
+    </row>
+    <row r="209" spans="1:17">
       <c r="A209" s="8"/>
       <c r="B209" s="5"/>
       <c r="C209" s="1"/>
@@ -4894,9 +4680,8 @@
       <c r="O209" s="7"/>
       <c r="P209" s="7"/>
       <c r="Q209" s="1"/>
-      <c r="R209" s="1"/>
-    </row>
-    <row r="210" spans="1:18">
+    </row>
+    <row r="210" spans="1:17">
       <c r="A210" s="8"/>
       <c r="B210" s="5"/>
       <c r="C210" s="1"/>
@@ -4914,9 +4699,8 @@
       <c r="O210" s="7"/>
       <c r="P210" s="7"/>
       <c r="Q210" s="1"/>
-      <c r="R210" s="1"/>
-    </row>
-    <row r="211" spans="1:18">
+    </row>
+    <row r="211" spans="1:17">
       <c r="A211" s="8"/>
       <c r="B211" s="5"/>
       <c r="C211" s="1"/>
@@ -4934,9 +4718,8 @@
       <c r="O211" s="7"/>
       <c r="P211" s="7"/>
       <c r="Q211" s="1"/>
-      <c r="R211" s="1"/>
-    </row>
-    <row r="212" spans="1:18">
+    </row>
+    <row r="212" spans="1:17">
       <c r="A212" s="8"/>
       <c r="B212" s="5"/>
       <c r="C212" s="1"/>
@@ -4954,9 +4737,8 @@
       <c r="O212" s="7"/>
       <c r="P212" s="7"/>
       <c r="Q212" s="1"/>
-      <c r="R212" s="1"/>
-    </row>
-    <row r="213" spans="1:18">
+    </row>
+    <row r="213" spans="1:17">
       <c r="A213" s="8"/>
       <c r="B213" s="5"/>
       <c r="C213" s="1"/>
@@ -4974,9 +4756,8 @@
       <c r="O213" s="7"/>
       <c r="P213" s="7"/>
       <c r="Q213" s="1"/>
-      <c r="R213" s="1"/>
-    </row>
-    <row r="214" spans="1:18">
+    </row>
+    <row r="214" spans="1:17">
       <c r="A214" s="8"/>
       <c r="B214" s="5"/>
       <c r="C214" s="1"/>
@@ -4994,9 +4775,8 @@
       <c r="O214" s="7"/>
       <c r="P214" s="7"/>
       <c r="Q214" s="1"/>
-      <c r="R214" s="1"/>
-    </row>
-    <row r="215" spans="1:18">
+    </row>
+    <row r="215" spans="1:17">
       <c r="A215" s="8"/>
       <c r="B215" s="5"/>
       <c r="C215" s="1"/>
@@ -5014,9 +4794,8 @@
       <c r="O215" s="7"/>
       <c r="P215" s="7"/>
       <c r="Q215" s="1"/>
-      <c r="R215" s="1"/>
-    </row>
-    <row r="216" spans="1:18">
+    </row>
+    <row r="216" spans="1:17">
       <c r="A216" s="8"/>
       <c r="B216" s="5"/>
       <c r="C216" s="1"/>
@@ -5034,9 +4813,8 @@
       <c r="O216" s="7"/>
       <c r="P216" s="7"/>
       <c r="Q216" s="1"/>
-      <c r="R216" s="1"/>
-    </row>
-    <row r="217" spans="1:18">
+    </row>
+    <row r="217" spans="1:17">
       <c r="A217" s="8"/>
       <c r="B217" s="5"/>
       <c r="C217" s="1"/>
@@ -5054,9 +4832,8 @@
       <c r="O217" s="7"/>
       <c r="P217" s="7"/>
       <c r="Q217" s="1"/>
-      <c r="R217" s="1"/>
-    </row>
-    <row r="218" spans="1:18">
+    </row>
+    <row r="218" spans="1:17">
       <c r="A218" s="8"/>
       <c r="B218" s="5"/>
       <c r="C218" s="1"/>
@@ -5074,9 +4851,8 @@
       <c r="O218" s="7"/>
       <c r="P218" s="7"/>
       <c r="Q218" s="1"/>
-      <c r="R218" s="1"/>
-    </row>
-    <row r="219" spans="1:18">
+    </row>
+    <row r="219" spans="1:17">
       <c r="A219" s="8"/>
       <c r="B219" s="5"/>
       <c r="C219" s="1"/>
@@ -5094,9 +4870,8 @@
       <c r="O219" s="7"/>
       <c r="P219" s="7"/>
       <c r="Q219" s="1"/>
-      <c r="R219" s="1"/>
-    </row>
-    <row r="220" spans="1:18">
+    </row>
+    <row r="220" spans="1:17">
       <c r="A220" s="8"/>
       <c r="B220" s="5"/>
       <c r="C220" s="1"/>
@@ -5114,9 +4889,8 @@
       <c r="O220" s="7"/>
       <c r="P220" s="7"/>
       <c r="Q220" s="1"/>
-      <c r="R220" s="1"/>
-    </row>
-    <row r="221" spans="1:18">
+    </row>
+    <row r="221" spans="1:17">
       <c r="A221" s="8"/>
       <c r="B221" s="5"/>
       <c r="C221" s="1"/>
@@ -5134,9 +4908,8 @@
       <c r="O221" s="7"/>
       <c r="P221" s="7"/>
       <c r="Q221" s="1"/>
-      <c r="R221" s="1"/>
-    </row>
-    <row r="222" spans="1:18">
+    </row>
+    <row r="222" spans="1:17">
       <c r="A222" s="8"/>
       <c r="B222" s="5"/>
       <c r="C222" s="1"/>
@@ -5154,9 +4927,8 @@
       <c r="O222" s="7"/>
       <c r="P222" s="7"/>
       <c r="Q222" s="1"/>
-      <c r="R222" s="1"/>
-    </row>
-    <row r="223" spans="1:18">
+    </row>
+    <row r="223" spans="1:17">
       <c r="A223" s="8"/>
       <c r="B223" s="5"/>
       <c r="C223" s="1"/>
@@ -5174,9 +4946,8 @@
       <c r="O223" s="7"/>
       <c r="P223" s="7"/>
       <c r="Q223" s="1"/>
-      <c r="R223" s="1"/>
-    </row>
-    <row r="224" spans="1:18">
+    </row>
+    <row r="224" spans="1:17">
       <c r="A224" s="8"/>
       <c r="B224" s="5"/>
       <c r="C224" s="1"/>
@@ -5194,9 +4965,8 @@
       <c r="O224" s="7"/>
       <c r="P224" s="7"/>
       <c r="Q224" s="1"/>
-      <c r="R224" s="1"/>
-    </row>
-    <row r="225" spans="1:18">
+    </row>
+    <row r="225" spans="1:17">
       <c r="A225" s="8"/>
       <c r="B225" s="5"/>
       <c r="C225" s="1"/>
@@ -5214,9 +4984,8 @@
       <c r="O225" s="7"/>
       <c r="P225" s="7"/>
       <c r="Q225" s="1"/>
-      <c r="R225" s="1"/>
-    </row>
-    <row r="226" spans="1:18">
+    </row>
+    <row r="226" spans="1:17">
       <c r="A226" s="8"/>
       <c r="B226" s="5"/>
       <c r="C226" s="1"/>
@@ -5234,9 +5003,8 @@
       <c r="O226" s="7"/>
       <c r="P226" s="7"/>
       <c r="Q226" s="1"/>
-      <c r="R226" s="1"/>
-    </row>
-    <row r="227" spans="1:18">
+    </row>
+    <row r="227" spans="1:17">
       <c r="A227" s="8"/>
       <c r="B227" s="5"/>
       <c r="C227" s="1"/>
@@ -5254,9 +5022,8 @@
       <c r="O227" s="7"/>
       <c r="P227" s="7"/>
       <c r="Q227" s="1"/>
-      <c r="R227" s="1"/>
-    </row>
-    <row r="228" spans="1:18">
+    </row>
+    <row r="228" spans="1:17">
       <c r="A228" s="8"/>
       <c r="B228" s="5"/>
       <c r="C228" s="1"/>
@@ -5274,9 +5041,8 @@
       <c r="O228" s="7"/>
       <c r="P228" s="7"/>
       <c r="Q228" s="1"/>
-      <c r="R228" s="1"/>
-    </row>
-    <row r="229" spans="1:18">
+    </row>
+    <row r="229" spans="1:17">
       <c r="A229" s="8"/>
       <c r="B229" s="5"/>
       <c r="C229" s="1"/>
@@ -5294,9 +5060,8 @@
       <c r="O229" s="7"/>
       <c r="P229" s="7"/>
       <c r="Q229" s="1"/>
-      <c r="R229" s="1"/>
-    </row>
-    <row r="230" spans="1:18">
+    </row>
+    <row r="230" spans="1:17">
       <c r="A230" s="8"/>
       <c r="B230" s="5"/>
       <c r="C230" s="1"/>
@@ -5314,9 +5079,8 @@
       <c r="O230" s="7"/>
       <c r="P230" s="7"/>
       <c r="Q230" s="1"/>
-      <c r="R230" s="1"/>
-    </row>
-    <row r="231" spans="1:18">
+    </row>
+    <row r="231" spans="1:17">
       <c r="A231" s="8"/>
       <c r="B231" s="5"/>
       <c r="C231" s="1"/>
@@ -5334,15 +5098,14 @@
       <c r="O231" s="7"/>
       <c r="P231" s="7"/>
       <c r="Q231" s="1"/>
-      <c r="R231" s="1"/>
-    </row>
-    <row r="232" spans="1:18">
+    </row>
+    <row r="232" spans="1:17">
       <c r="A232" s="8"/>
       <c r="B232" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="N2:P2"/>
   </mergeCells>
@@ -5398,92 +5161,92 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5">
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6">
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7">
         <v>31</v>
       </c>
       <c r="C7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+      <c r="C8" t="s">
         <v>39</v>
       </c>
-      <c r="C8" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Päivitä testit ja excel-pohjat
</commit_message>
<xml_diff>
--- a/dev-resources/excel/harja_urapaikkaustoteumien_tuonti_pohja.xlsx
+++ b/dev-resources/excel/harja_urapaikkaustoteumien_tuonti_pohja.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_aa5\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{775F82FF-7EC5-4CDC-AD2C-D27C06FB2DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E150476B-3057-408F-BB4A-608924D21589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -166,8 +166,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-40B]d/m/yyyy\ hh:mm"/>
+    <numFmt numFmtId="166" formatCode="[$-40B]d:m:yyyy\ hh:mm"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -243,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -253,6 +254,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -640,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q232"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3:R231"/>
+    <sheetView tabSelected="1" topLeftCell="A219" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -665,29 +668,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -699,11 +702,11 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
-      <c r="N2" s="11" t="s">
+      <c r="N2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
       <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="1:17">
@@ -787,8 +790,8 @@
       </c>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="8"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -806,8 +809,8 @@
       <c r="Q5" s="6"/>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="8"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -825,8 +828,8 @@
       <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="8"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -844,8 +847,8 @@
       <c r="Q7" s="1"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="8"/>
-      <c r="B8" s="5"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -863,8 +866,8 @@
       <c r="Q8" s="1"/>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="8"/>
-      <c r="B9" s="5"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -882,8 +885,8 @@
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="8"/>
-      <c r="B10" s="5"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -901,8 +904,8 @@
       <c r="Q10" s="1"/>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="8"/>
-      <c r="B11" s="5"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -920,8 +923,8 @@
       <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="8"/>
-      <c r="B12" s="5"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -939,8 +942,8 @@
       <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="8"/>
-      <c r="B13" s="5"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="9"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -958,8 +961,8 @@
       <c r="Q13" s="1"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="8"/>
-      <c r="B14" s="5"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="9"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -977,8 +980,8 @@
       <c r="Q14" s="1"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="8"/>
-      <c r="B15" s="5"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -996,8 +999,8 @@
       <c r="Q15" s="1"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="8"/>
-      <c r="B16" s="5"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1015,8 +1018,8 @@
       <c r="Q16" s="1"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="8"/>
-      <c r="B17" s="5"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1034,8 +1037,8 @@
       <c r="Q17" s="1"/>
     </row>
     <row r="18" spans="1:17">
-      <c r="A18" s="8"/>
-      <c r="B18" s="5"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="9"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1053,8 +1056,8 @@
       <c r="Q18" s="1"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="8"/>
-      <c r="B19" s="5"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="9"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1072,8 +1075,8 @@
       <c r="Q19" s="1"/>
     </row>
     <row r="20" spans="1:17">
-      <c r="A20" s="8"/>
-      <c r="B20" s="5"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="9"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1091,8 +1094,8 @@
       <c r="Q20" s="1"/>
     </row>
     <row r="21" spans="1:17">
-      <c r="A21" s="8"/>
-      <c r="B21" s="5"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="9"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1110,8 +1113,8 @@
       <c r="Q21" s="1"/>
     </row>
     <row r="22" spans="1:17">
-      <c r="A22" s="8"/>
-      <c r="B22" s="5"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="9"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1129,8 +1132,8 @@
       <c r="Q22" s="1"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="8"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="9"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1148,8 +1151,8 @@
       <c r="Q23" s="1"/>
     </row>
     <row r="24" spans="1:17">
-      <c r="A24" s="8"/>
-      <c r="B24" s="5"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="9"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -1167,8 +1170,8 @@
       <c r="Q24" s="1"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="8"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="9"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1186,8 +1189,8 @@
       <c r="Q25" s="1"/>
     </row>
     <row r="26" spans="1:17">
-      <c r="A26" s="8"/>
-      <c r="B26" s="5"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="9"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1205,8 +1208,8 @@
       <c r="Q26" s="1"/>
     </row>
     <row r="27" spans="1:17">
-      <c r="A27" s="8"/>
-      <c r="B27" s="5"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="9"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1224,8 +1227,8 @@
       <c r="Q27" s="1"/>
     </row>
     <row r="28" spans="1:17">
-      <c r="A28" s="8"/>
-      <c r="B28" s="5"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="9"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1243,8 +1246,8 @@
       <c r="Q28" s="1"/>
     </row>
     <row r="29" spans="1:17">
-      <c r="A29" s="8"/>
-      <c r="B29" s="5"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="9"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1262,8 +1265,8 @@
       <c r="Q29" s="1"/>
     </row>
     <row r="30" spans="1:17">
-      <c r="A30" s="8"/>
-      <c r="B30" s="5"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="9"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1281,8 +1284,8 @@
       <c r="Q30" s="1"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="8"/>
-      <c r="B31" s="5"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="9"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -1300,8 +1303,8 @@
       <c r="Q31" s="1"/>
     </row>
     <row r="32" spans="1:17">
-      <c r="A32" s="8"/>
-      <c r="B32" s="5"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="9"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1319,8 +1322,8 @@
       <c r="Q32" s="1"/>
     </row>
     <row r="33" spans="1:17">
-      <c r="A33" s="8"/>
-      <c r="B33" s="5"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="9"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -1338,8 +1341,8 @@
       <c r="Q33" s="1"/>
     </row>
     <row r="34" spans="1:17">
-      <c r="A34" s="8"/>
-      <c r="B34" s="5"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="9"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1357,8 +1360,8 @@
       <c r="Q34" s="1"/>
     </row>
     <row r="35" spans="1:17">
-      <c r="A35" s="8"/>
-      <c r="B35" s="5"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="9"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1376,8 +1379,8 @@
       <c r="Q35" s="1"/>
     </row>
     <row r="36" spans="1:17">
-      <c r="A36" s="8"/>
-      <c r="B36" s="5"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="9"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -1395,8 +1398,8 @@
       <c r="Q36" s="1"/>
     </row>
     <row r="37" spans="1:17">
-      <c r="A37" s="8"/>
-      <c r="B37" s="5"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="9"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -1414,8 +1417,8 @@
       <c r="Q37" s="1"/>
     </row>
     <row r="38" spans="1:17">
-      <c r="A38" s="8"/>
-      <c r="B38" s="5"/>
+      <c r="A38" s="10"/>
+      <c r="B38" s="9"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -1433,8 +1436,8 @@
       <c r="Q38" s="1"/>
     </row>
     <row r="39" spans="1:17">
-      <c r="A39" s="8"/>
-      <c r="B39" s="5"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="9"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -1452,8 +1455,8 @@
       <c r="Q39" s="1"/>
     </row>
     <row r="40" spans="1:17">
-      <c r="A40" s="8"/>
-      <c r="B40" s="5"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="9"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -1471,8 +1474,8 @@
       <c r="Q40" s="1"/>
     </row>
     <row r="41" spans="1:17">
-      <c r="A41" s="8"/>
-      <c r="B41" s="5"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="9"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -1490,8 +1493,8 @@
       <c r="Q41" s="1"/>
     </row>
     <row r="42" spans="1:17">
-      <c r="A42" s="8"/>
-      <c r="B42" s="5"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="9"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -1509,8 +1512,8 @@
       <c r="Q42" s="1"/>
     </row>
     <row r="43" spans="1:17">
-      <c r="A43" s="8"/>
-      <c r="B43" s="5"/>
+      <c r="A43" s="10"/>
+      <c r="B43" s="9"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -1528,8 +1531,8 @@
       <c r="Q43" s="1"/>
     </row>
     <row r="44" spans="1:17">
-      <c r="A44" s="8"/>
-      <c r="B44" s="5"/>
+      <c r="A44" s="10"/>
+      <c r="B44" s="9"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -1547,8 +1550,8 @@
       <c r="Q44" s="1"/>
     </row>
     <row r="45" spans="1:17">
-      <c r="A45" s="8"/>
-      <c r="B45" s="5"/>
+      <c r="A45" s="10"/>
+      <c r="B45" s="9"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -1566,8 +1569,8 @@
       <c r="Q45" s="1"/>
     </row>
     <row r="46" spans="1:17">
-      <c r="A46" s="8"/>
-      <c r="B46" s="5"/>
+      <c r="A46" s="10"/>
+      <c r="B46" s="9"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -1585,8 +1588,8 @@
       <c r="Q46" s="1"/>
     </row>
     <row r="47" spans="1:17">
-      <c r="A47" s="8"/>
-      <c r="B47" s="5"/>
+      <c r="A47" s="10"/>
+      <c r="B47" s="9"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -1604,8 +1607,8 @@
       <c r="Q47" s="1"/>
     </row>
     <row r="48" spans="1:17">
-      <c r="A48" s="8"/>
-      <c r="B48" s="5"/>
+      <c r="A48" s="10"/>
+      <c r="B48" s="9"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -1623,8 +1626,8 @@
       <c r="Q48" s="1"/>
     </row>
     <row r="49" spans="1:17">
-      <c r="A49" s="8"/>
-      <c r="B49" s="5"/>
+      <c r="A49" s="10"/>
+      <c r="B49" s="9"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -1642,8 +1645,8 @@
       <c r="Q49" s="1"/>
     </row>
     <row r="50" spans="1:17">
-      <c r="A50" s="8"/>
-      <c r="B50" s="5"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="9"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -1661,8 +1664,8 @@
       <c r="Q50" s="1"/>
     </row>
     <row r="51" spans="1:17">
-      <c r="A51" s="8"/>
-      <c r="B51" s="5"/>
+      <c r="A51" s="10"/>
+      <c r="B51" s="9"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -1680,8 +1683,8 @@
       <c r="Q51" s="1"/>
     </row>
     <row r="52" spans="1:17">
-      <c r="A52" s="8"/>
-      <c r="B52" s="5"/>
+      <c r="A52" s="10"/>
+      <c r="B52" s="9"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -1699,8 +1702,8 @@
       <c r="Q52" s="1"/>
     </row>
     <row r="53" spans="1:17">
-      <c r="A53" s="8"/>
-      <c r="B53" s="5"/>
+      <c r="A53" s="10"/>
+      <c r="B53" s="9"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -1718,8 +1721,8 @@
       <c r="Q53" s="1"/>
     </row>
     <row r="54" spans="1:17">
-      <c r="A54" s="8"/>
-      <c r="B54" s="5"/>
+      <c r="A54" s="10"/>
+      <c r="B54" s="9"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -1737,8 +1740,8 @@
       <c r="Q54" s="1"/>
     </row>
     <row r="55" spans="1:17">
-      <c r="A55" s="8"/>
-      <c r="B55" s="5"/>
+      <c r="A55" s="10"/>
+      <c r="B55" s="9"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -1756,8 +1759,8 @@
       <c r="Q55" s="1"/>
     </row>
     <row r="56" spans="1:17">
-      <c r="A56" s="8"/>
-      <c r="B56" s="5"/>
+      <c r="A56" s="10"/>
+      <c r="B56" s="9"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -1775,8 +1778,8 @@
       <c r="Q56" s="1"/>
     </row>
     <row r="57" spans="1:17">
-      <c r="A57" s="8"/>
-      <c r="B57" s="5"/>
+      <c r="A57" s="10"/>
+      <c r="B57" s="9"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -1794,8 +1797,8 @@
       <c r="Q57" s="1"/>
     </row>
     <row r="58" spans="1:17">
-      <c r="A58" s="8"/>
-      <c r="B58" s="5"/>
+      <c r="A58" s="10"/>
+      <c r="B58" s="9"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
@@ -1813,8 +1816,8 @@
       <c r="Q58" s="1"/>
     </row>
     <row r="59" spans="1:17">
-      <c r="A59" s="8"/>
-      <c r="B59" s="5"/>
+      <c r="A59" s="10"/>
+      <c r="B59" s="9"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
@@ -1832,8 +1835,8 @@
       <c r="Q59" s="1"/>
     </row>
     <row r="60" spans="1:17">
-      <c r="A60" s="8"/>
-      <c r="B60" s="5"/>
+      <c r="A60" s="10"/>
+      <c r="B60" s="9"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
@@ -1851,8 +1854,8 @@
       <c r="Q60" s="1"/>
     </row>
     <row r="61" spans="1:17">
-      <c r="A61" s="8"/>
-      <c r="B61" s="5"/>
+      <c r="A61" s="10"/>
+      <c r="B61" s="9"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
@@ -1870,8 +1873,8 @@
       <c r="Q61" s="1"/>
     </row>
     <row r="62" spans="1:17">
-      <c r="A62" s="8"/>
-      <c r="B62" s="5"/>
+      <c r="A62" s="10"/>
+      <c r="B62" s="9"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
@@ -1889,8 +1892,8 @@
       <c r="Q62" s="1"/>
     </row>
     <row r="63" spans="1:17">
-      <c r="A63" s="8"/>
-      <c r="B63" s="5"/>
+      <c r="A63" s="10"/>
+      <c r="B63" s="9"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
@@ -1908,8 +1911,8 @@
       <c r="Q63" s="1"/>
     </row>
     <row r="64" spans="1:17">
-      <c r="A64" s="8"/>
-      <c r="B64" s="5"/>
+      <c r="A64" s="10"/>
+      <c r="B64" s="9"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
@@ -1927,8 +1930,8 @@
       <c r="Q64" s="1"/>
     </row>
     <row r="65" spans="1:17">
-      <c r="A65" s="8"/>
-      <c r="B65" s="5"/>
+      <c r="A65" s="10"/>
+      <c r="B65" s="9"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
@@ -1946,8 +1949,8 @@
       <c r="Q65" s="1"/>
     </row>
     <row r="66" spans="1:17">
-      <c r="A66" s="8"/>
-      <c r="B66" s="5"/>
+      <c r="A66" s="10"/>
+      <c r="B66" s="9"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
@@ -1965,8 +1968,8 @@
       <c r="Q66" s="1"/>
     </row>
     <row r="67" spans="1:17">
-      <c r="A67" s="8"/>
-      <c r="B67" s="5"/>
+      <c r="A67" s="10"/>
+      <c r="B67" s="9"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
@@ -1984,8 +1987,8 @@
       <c r="Q67" s="1"/>
     </row>
     <row r="68" spans="1:17">
-      <c r="A68" s="8"/>
-      <c r="B68" s="5"/>
+      <c r="A68" s="10"/>
+      <c r="B68" s="9"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
@@ -2003,8 +2006,8 @@
       <c r="Q68" s="1"/>
     </row>
     <row r="69" spans="1:17">
-      <c r="A69" s="8"/>
-      <c r="B69" s="5"/>
+      <c r="A69" s="10"/>
+      <c r="B69" s="9"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
@@ -2022,8 +2025,8 @@
       <c r="Q69" s="1"/>
     </row>
     <row r="70" spans="1:17">
-      <c r="A70" s="8"/>
-      <c r="B70" s="5"/>
+      <c r="A70" s="10"/>
+      <c r="B70" s="9"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
@@ -2041,8 +2044,8 @@
       <c r="Q70" s="1"/>
     </row>
     <row r="71" spans="1:17">
-      <c r="A71" s="8"/>
-      <c r="B71" s="5"/>
+      <c r="A71" s="10"/>
+      <c r="B71" s="9"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
@@ -2060,8 +2063,8 @@
       <c r="Q71" s="1"/>
     </row>
     <row r="72" spans="1:17">
-      <c r="A72" s="8"/>
-      <c r="B72" s="5"/>
+      <c r="A72" s="10"/>
+      <c r="B72" s="9"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
@@ -2079,8 +2082,8 @@
       <c r="Q72" s="1"/>
     </row>
     <row r="73" spans="1:17">
-      <c r="A73" s="8"/>
-      <c r="B73" s="5"/>
+      <c r="A73" s="10"/>
+      <c r="B73" s="9"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -2098,8 +2101,8 @@
       <c r="Q73" s="1"/>
     </row>
     <row r="74" spans="1:17">
-      <c r="A74" s="8"/>
-      <c r="B74" s="5"/>
+      <c r="A74" s="10"/>
+      <c r="B74" s="9"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
@@ -2117,8 +2120,8 @@
       <c r="Q74" s="1"/>
     </row>
     <row r="75" spans="1:17">
-      <c r="A75" s="8"/>
-      <c r="B75" s="5"/>
+      <c r="A75" s="10"/>
+      <c r="B75" s="9"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
@@ -2136,8 +2139,8 @@
       <c r="Q75" s="1"/>
     </row>
     <row r="76" spans="1:17">
-      <c r="A76" s="8"/>
-      <c r="B76" s="5"/>
+      <c r="A76" s="10"/>
+      <c r="B76" s="9"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
@@ -2155,8 +2158,8 @@
       <c r="Q76" s="1"/>
     </row>
     <row r="77" spans="1:17">
-      <c r="A77" s="8"/>
-      <c r="B77" s="5"/>
+      <c r="A77" s="10"/>
+      <c r="B77" s="9"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -2174,8 +2177,8 @@
       <c r="Q77" s="1"/>
     </row>
     <row r="78" spans="1:17">
-      <c r="A78" s="8"/>
-      <c r="B78" s="5"/>
+      <c r="A78" s="10"/>
+      <c r="B78" s="9"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
@@ -2193,8 +2196,8 @@
       <c r="Q78" s="1"/>
     </row>
     <row r="79" spans="1:17">
-      <c r="A79" s="8"/>
-      <c r="B79" s="5"/>
+      <c r="A79" s="10"/>
+      <c r="B79" s="9"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
@@ -2212,8 +2215,8 @@
       <c r="Q79" s="1"/>
     </row>
     <row r="80" spans="1:17">
-      <c r="A80" s="8"/>
-      <c r="B80" s="5"/>
+      <c r="A80" s="10"/>
+      <c r="B80" s="9"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
@@ -2231,8 +2234,8 @@
       <c r="Q80" s="1"/>
     </row>
     <row r="81" spans="1:17">
-      <c r="A81" s="8"/>
-      <c r="B81" s="5"/>
+      <c r="A81" s="10"/>
+      <c r="B81" s="9"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
@@ -2250,8 +2253,8 @@
       <c r="Q81" s="1"/>
     </row>
     <row r="82" spans="1:17">
-      <c r="A82" s="8"/>
-      <c r="B82" s="5"/>
+      <c r="A82" s="10"/>
+      <c r="B82" s="9"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
@@ -2269,8 +2272,8 @@
       <c r="Q82" s="1"/>
     </row>
     <row r="83" spans="1:17">
-      <c r="A83" s="8"/>
-      <c r="B83" s="5"/>
+      <c r="A83" s="10"/>
+      <c r="B83" s="9"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
@@ -2288,8 +2291,8 @@
       <c r="Q83" s="1"/>
     </row>
     <row r="84" spans="1:17">
-      <c r="A84" s="8"/>
-      <c r="B84" s="5"/>
+      <c r="A84" s="10"/>
+      <c r="B84" s="9"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
@@ -2307,8 +2310,8 @@
       <c r="Q84" s="1"/>
     </row>
     <row r="85" spans="1:17">
-      <c r="A85" s="8"/>
-      <c r="B85" s="5"/>
+      <c r="A85" s="10"/>
+      <c r="B85" s="9"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
@@ -2326,8 +2329,8 @@
       <c r="Q85" s="1"/>
     </row>
     <row r="86" spans="1:17">
-      <c r="A86" s="8"/>
-      <c r="B86" s="5"/>
+      <c r="A86" s="10"/>
+      <c r="B86" s="9"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
@@ -2345,8 +2348,8 @@
       <c r="Q86" s="1"/>
     </row>
     <row r="87" spans="1:17">
-      <c r="A87" s="8"/>
-      <c r="B87" s="5"/>
+      <c r="A87" s="10"/>
+      <c r="B87" s="9"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
@@ -2364,8 +2367,8 @@
       <c r="Q87" s="1"/>
     </row>
     <row r="88" spans="1:17">
-      <c r="A88" s="8"/>
-      <c r="B88" s="5"/>
+      <c r="A88" s="10"/>
+      <c r="B88" s="9"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
@@ -2383,8 +2386,8 @@
       <c r="Q88" s="1"/>
     </row>
     <row r="89" spans="1:17">
-      <c r="A89" s="8"/>
-      <c r="B89" s="5"/>
+      <c r="A89" s="10"/>
+      <c r="B89" s="9"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
@@ -2402,8 +2405,8 @@
       <c r="Q89" s="1"/>
     </row>
     <row r="90" spans="1:17">
-      <c r="A90" s="8"/>
-      <c r="B90" s="5"/>
+      <c r="A90" s="10"/>
+      <c r="B90" s="9"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
@@ -2421,8 +2424,8 @@
       <c r="Q90" s="1"/>
     </row>
     <row r="91" spans="1:17">
-      <c r="A91" s="8"/>
-      <c r="B91" s="5"/>
+      <c r="A91" s="10"/>
+      <c r="B91" s="9"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
@@ -2440,8 +2443,8 @@
       <c r="Q91" s="1"/>
     </row>
     <row r="92" spans="1:17">
-      <c r="A92" s="8"/>
-      <c r="B92" s="5"/>
+      <c r="A92" s="10"/>
+      <c r="B92" s="9"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
@@ -2459,8 +2462,8 @@
       <c r="Q92" s="1"/>
     </row>
     <row r="93" spans="1:17">
-      <c r="A93" s="8"/>
-      <c r="B93" s="5"/>
+      <c r="A93" s="10"/>
+      <c r="B93" s="9"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
@@ -2478,8 +2481,8 @@
       <c r="Q93" s="1"/>
     </row>
     <row r="94" spans="1:17">
-      <c r="A94" s="8"/>
-      <c r="B94" s="5"/>
+      <c r="A94" s="10"/>
+      <c r="B94" s="9"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
@@ -2497,8 +2500,8 @@
       <c r="Q94" s="1"/>
     </row>
     <row r="95" spans="1:17">
-      <c r="A95" s="8"/>
-      <c r="B95" s="5"/>
+      <c r="A95" s="10"/>
+      <c r="B95" s="9"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
@@ -2516,8 +2519,8 @@
       <c r="Q95" s="1"/>
     </row>
     <row r="96" spans="1:17">
-      <c r="A96" s="8"/>
-      <c r="B96" s="5"/>
+      <c r="A96" s="10"/>
+      <c r="B96" s="9"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
@@ -2535,8 +2538,8 @@
       <c r="Q96" s="1"/>
     </row>
     <row r="97" spans="1:17">
-      <c r="A97" s="8"/>
-      <c r="B97" s="5"/>
+      <c r="A97" s="10"/>
+      <c r="B97" s="9"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
@@ -2554,8 +2557,8 @@
       <c r="Q97" s="1"/>
     </row>
     <row r="98" spans="1:17">
-      <c r="A98" s="8"/>
-      <c r="B98" s="5"/>
+      <c r="A98" s="10"/>
+      <c r="B98" s="9"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
@@ -2573,8 +2576,8 @@
       <c r="Q98" s="1"/>
     </row>
     <row r="99" spans="1:17">
-      <c r="A99" s="8"/>
-      <c r="B99" s="5"/>
+      <c r="A99" s="10"/>
+      <c r="B99" s="9"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
@@ -2592,8 +2595,8 @@
       <c r="Q99" s="1"/>
     </row>
     <row r="100" spans="1:17">
-      <c r="A100" s="8"/>
-      <c r="B100" s="5"/>
+      <c r="A100" s="10"/>
+      <c r="B100" s="9"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
@@ -2611,8 +2614,8 @@
       <c r="Q100" s="1"/>
     </row>
     <row r="101" spans="1:17">
-      <c r="A101" s="8"/>
-      <c r="B101" s="5"/>
+      <c r="A101" s="10"/>
+      <c r="B101" s="9"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
@@ -2630,8 +2633,8 @@
       <c r="Q101" s="1"/>
     </row>
     <row r="102" spans="1:17">
-      <c r="A102" s="8"/>
-      <c r="B102" s="5"/>
+      <c r="A102" s="10"/>
+      <c r="B102" s="9"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
@@ -2649,8 +2652,8 @@
       <c r="Q102" s="1"/>
     </row>
     <row r="103" spans="1:17">
-      <c r="A103" s="8"/>
-      <c r="B103" s="5"/>
+      <c r="A103" s="10"/>
+      <c r="B103" s="9"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
@@ -2668,8 +2671,8 @@
       <c r="Q103" s="1"/>
     </row>
     <row r="104" spans="1:17">
-      <c r="A104" s="8"/>
-      <c r="B104" s="5"/>
+      <c r="A104" s="10"/>
+      <c r="B104" s="9"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
@@ -2687,8 +2690,8 @@
       <c r="Q104" s="1"/>
     </row>
     <row r="105" spans="1:17">
-      <c r="A105" s="8"/>
-      <c r="B105" s="5"/>
+      <c r="A105" s="10"/>
+      <c r="B105" s="9"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
@@ -2706,8 +2709,8 @@
       <c r="Q105" s="1"/>
     </row>
     <row r="106" spans="1:17">
-      <c r="A106" s="8"/>
-      <c r="B106" s="5"/>
+      <c r="A106" s="10"/>
+      <c r="B106" s="9"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
@@ -2725,8 +2728,8 @@
       <c r="Q106" s="1"/>
     </row>
     <row r="107" spans="1:17">
-      <c r="A107" s="8"/>
-      <c r="B107" s="5"/>
+      <c r="A107" s="10"/>
+      <c r="B107" s="9"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
@@ -2744,8 +2747,8 @@
       <c r="Q107" s="1"/>
     </row>
     <row r="108" spans="1:17">
-      <c r="A108" s="8"/>
-      <c r="B108" s="5"/>
+      <c r="A108" s="10"/>
+      <c r="B108" s="9"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
@@ -2763,8 +2766,8 @@
       <c r="Q108" s="1"/>
     </row>
     <row r="109" spans="1:17">
-      <c r="A109" s="8"/>
-      <c r="B109" s="5"/>
+      <c r="A109" s="10"/>
+      <c r="B109" s="9"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
@@ -2782,8 +2785,8 @@
       <c r="Q109" s="1"/>
     </row>
     <row r="110" spans="1:17">
-      <c r="A110" s="8"/>
-      <c r="B110" s="5"/>
+      <c r="A110" s="10"/>
+      <c r="B110" s="9"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
@@ -2801,8 +2804,8 @@
       <c r="Q110" s="1"/>
     </row>
     <row r="111" spans="1:17">
-      <c r="A111" s="8"/>
-      <c r="B111" s="5"/>
+      <c r="A111" s="10"/>
+      <c r="B111" s="9"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
@@ -2820,8 +2823,8 @@
       <c r="Q111" s="1"/>
     </row>
     <row r="112" spans="1:17">
-      <c r="A112" s="8"/>
-      <c r="B112" s="5"/>
+      <c r="A112" s="10"/>
+      <c r="B112" s="9"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
@@ -2839,8 +2842,8 @@
       <c r="Q112" s="1"/>
     </row>
     <row r="113" spans="1:17">
-      <c r="A113" s="8"/>
-      <c r="B113" s="5"/>
+      <c r="A113" s="10"/>
+      <c r="B113" s="9"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
@@ -2858,8 +2861,8 @@
       <c r="Q113" s="1"/>
     </row>
     <row r="114" spans="1:17">
-      <c r="A114" s="8"/>
-      <c r="B114" s="5"/>
+      <c r="A114" s="10"/>
+      <c r="B114" s="9"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
@@ -2877,8 +2880,8 @@
       <c r="Q114" s="1"/>
     </row>
     <row r="115" spans="1:17">
-      <c r="A115" s="8"/>
-      <c r="B115" s="5"/>
+      <c r="A115" s="10"/>
+      <c r="B115" s="9"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
@@ -2896,8 +2899,8 @@
       <c r="Q115" s="1"/>
     </row>
     <row r="116" spans="1:17">
-      <c r="A116" s="8"/>
-      <c r="B116" s="5"/>
+      <c r="A116" s="10"/>
+      <c r="B116" s="9"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
@@ -2915,8 +2918,8 @@
       <c r="Q116" s="1"/>
     </row>
     <row r="117" spans="1:17">
-      <c r="A117" s="8"/>
-      <c r="B117" s="5"/>
+      <c r="A117" s="10"/>
+      <c r="B117" s="9"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
@@ -2934,8 +2937,8 @@
       <c r="Q117" s="1"/>
     </row>
     <row r="118" spans="1:17">
-      <c r="A118" s="8"/>
-      <c r="B118" s="5"/>
+      <c r="A118" s="10"/>
+      <c r="B118" s="9"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
@@ -2953,8 +2956,8 @@
       <c r="Q118" s="1"/>
     </row>
     <row r="119" spans="1:17">
-      <c r="A119" s="8"/>
-      <c r="B119" s="5"/>
+      <c r="A119" s="10"/>
+      <c r="B119" s="9"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
@@ -2972,8 +2975,8 @@
       <c r="Q119" s="1"/>
     </row>
     <row r="120" spans="1:17">
-      <c r="A120" s="8"/>
-      <c r="B120" s="5"/>
+      <c r="A120" s="10"/>
+      <c r="B120" s="9"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
@@ -2991,8 +2994,8 @@
       <c r="Q120" s="1"/>
     </row>
     <row r="121" spans="1:17">
-      <c r="A121" s="8"/>
-      <c r="B121" s="5"/>
+      <c r="A121" s="10"/>
+      <c r="B121" s="9"/>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
@@ -3010,8 +3013,8 @@
       <c r="Q121" s="1"/>
     </row>
     <row r="122" spans="1:17">
-      <c r="A122" s="8"/>
-      <c r="B122" s="5"/>
+      <c r="A122" s="10"/>
+      <c r="B122" s="9"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
@@ -3029,8 +3032,8 @@
       <c r="Q122" s="1"/>
     </row>
     <row r="123" spans="1:17">
-      <c r="A123" s="8"/>
-      <c r="B123" s="5"/>
+      <c r="A123" s="10"/>
+      <c r="B123" s="9"/>
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
@@ -3048,8 +3051,8 @@
       <c r="Q123" s="1"/>
     </row>
     <row r="124" spans="1:17">
-      <c r="A124" s="8"/>
-      <c r="B124" s="5"/>
+      <c r="A124" s="10"/>
+      <c r="B124" s="9"/>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
@@ -3067,8 +3070,8 @@
       <c r="Q124" s="1"/>
     </row>
     <row r="125" spans="1:17">
-      <c r="A125" s="8"/>
-      <c r="B125" s="5"/>
+      <c r="A125" s="10"/>
+      <c r="B125" s="9"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
@@ -3086,8 +3089,8 @@
       <c r="Q125" s="1"/>
     </row>
     <row r="126" spans="1:17">
-      <c r="A126" s="8"/>
-      <c r="B126" s="5"/>
+      <c r="A126" s="10"/>
+      <c r="B126" s="9"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
@@ -3105,8 +3108,8 @@
       <c r="Q126" s="1"/>
     </row>
     <row r="127" spans="1:17">
-      <c r="A127" s="8"/>
-      <c r="B127" s="5"/>
+      <c r="A127" s="10"/>
+      <c r="B127" s="9"/>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
@@ -3124,8 +3127,8 @@
       <c r="Q127" s="1"/>
     </row>
     <row r="128" spans="1:17">
-      <c r="A128" s="8"/>
-      <c r="B128" s="5"/>
+      <c r="A128" s="10"/>
+      <c r="B128" s="9"/>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
@@ -3143,8 +3146,8 @@
       <c r="Q128" s="1"/>
     </row>
     <row r="129" spans="1:17">
-      <c r="A129" s="8"/>
-      <c r="B129" s="5"/>
+      <c r="A129" s="10"/>
+      <c r="B129" s="9"/>
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
@@ -3162,8 +3165,8 @@
       <c r="Q129" s="1"/>
     </row>
     <row r="130" spans="1:17">
-      <c r="A130" s="8"/>
-      <c r="B130" s="5"/>
+      <c r="A130" s="10"/>
+      <c r="B130" s="9"/>
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
@@ -3181,8 +3184,8 @@
       <c r="Q130" s="1"/>
     </row>
     <row r="131" spans="1:17">
-      <c r="A131" s="8"/>
-      <c r="B131" s="5"/>
+      <c r="A131" s="10"/>
+      <c r="B131" s="9"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
@@ -3200,8 +3203,8 @@
       <c r="Q131" s="1"/>
     </row>
     <row r="132" spans="1:17">
-      <c r="A132" s="8"/>
-      <c r="B132" s="5"/>
+      <c r="A132" s="10"/>
+      <c r="B132" s="9"/>
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
@@ -3219,8 +3222,8 @@
       <c r="Q132" s="1"/>
     </row>
     <row r="133" spans="1:17">
-      <c r="A133" s="8"/>
-      <c r="B133" s="5"/>
+      <c r="A133" s="10"/>
+      <c r="B133" s="9"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
@@ -3238,8 +3241,8 @@
       <c r="Q133" s="1"/>
     </row>
     <row r="134" spans="1:17">
-      <c r="A134" s="8"/>
-      <c r="B134" s="5"/>
+      <c r="A134" s="10"/>
+      <c r="B134" s="9"/>
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
@@ -3257,8 +3260,8 @@
       <c r="Q134" s="1"/>
     </row>
     <row r="135" spans="1:17">
-      <c r="A135" s="8"/>
-      <c r="B135" s="5"/>
+      <c r="A135" s="10"/>
+      <c r="B135" s="9"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
@@ -3276,8 +3279,8 @@
       <c r="Q135" s="1"/>
     </row>
     <row r="136" spans="1:17">
-      <c r="A136" s="8"/>
-      <c r="B136" s="5"/>
+      <c r="A136" s="10"/>
+      <c r="B136" s="9"/>
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
@@ -3295,8 +3298,8 @@
       <c r="Q136" s="1"/>
     </row>
     <row r="137" spans="1:17">
-      <c r="A137" s="8"/>
-      <c r="B137" s="5"/>
+      <c r="A137" s="10"/>
+      <c r="B137" s="9"/>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
@@ -3314,8 +3317,8 @@
       <c r="Q137" s="1"/>
     </row>
     <row r="138" spans="1:17">
-      <c r="A138" s="8"/>
-      <c r="B138" s="5"/>
+      <c r="A138" s="10"/>
+      <c r="B138" s="9"/>
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
@@ -3333,8 +3336,8 @@
       <c r="Q138" s="1"/>
     </row>
     <row r="139" spans="1:17">
-      <c r="A139" s="8"/>
-      <c r="B139" s="5"/>
+      <c r="A139" s="10"/>
+      <c r="B139" s="9"/>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
@@ -3352,8 +3355,8 @@
       <c r="Q139" s="1"/>
     </row>
     <row r="140" spans="1:17">
-      <c r="A140" s="8"/>
-      <c r="B140" s="5"/>
+      <c r="A140" s="10"/>
+      <c r="B140" s="9"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
       <c r="E140" s="1"/>
@@ -3371,8 +3374,8 @@
       <c r="Q140" s="1"/>
     </row>
     <row r="141" spans="1:17">
-      <c r="A141" s="8"/>
-      <c r="B141" s="5"/>
+      <c r="A141" s="10"/>
+      <c r="B141" s="9"/>
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
@@ -3390,8 +3393,8 @@
       <c r="Q141" s="1"/>
     </row>
     <row r="142" spans="1:17">
-      <c r="A142" s="8"/>
-      <c r="B142" s="5"/>
+      <c r="A142" s="10"/>
+      <c r="B142" s="9"/>
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
@@ -3409,8 +3412,8 @@
       <c r="Q142" s="1"/>
     </row>
     <row r="143" spans="1:17">
-      <c r="A143" s="8"/>
-      <c r="B143" s="5"/>
+      <c r="A143" s="10"/>
+      <c r="B143" s="9"/>
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
@@ -3428,8 +3431,8 @@
       <c r="Q143" s="1"/>
     </row>
     <row r="144" spans="1:17">
-      <c r="A144" s="8"/>
-      <c r="B144" s="5"/>
+      <c r="A144" s="10"/>
+      <c r="B144" s="9"/>
       <c r="C144" s="1"/>
       <c r="D144" s="1"/>
       <c r="E144" s="1"/>
@@ -3447,8 +3450,8 @@
       <c r="Q144" s="1"/>
     </row>
     <row r="145" spans="1:17">
-      <c r="A145" s="8"/>
-      <c r="B145" s="5"/>
+      <c r="A145" s="10"/>
+      <c r="B145" s="9"/>
       <c r="C145" s="1"/>
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
@@ -3466,8 +3469,8 @@
       <c r="Q145" s="1"/>
     </row>
     <row r="146" spans="1:17">
-      <c r="A146" s="8"/>
-      <c r="B146" s="5"/>
+      <c r="A146" s="10"/>
+      <c r="B146" s="9"/>
       <c r="C146" s="1"/>
       <c r="D146" s="1"/>
       <c r="E146" s="1"/>
@@ -3485,8 +3488,8 @@
       <c r="Q146" s="1"/>
     </row>
     <row r="147" spans="1:17">
-      <c r="A147" s="8"/>
-      <c r="B147" s="5"/>
+      <c r="A147" s="10"/>
+      <c r="B147" s="9"/>
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
       <c r="E147" s="1"/>
@@ -3504,8 +3507,8 @@
       <c r="Q147" s="1"/>
     </row>
     <row r="148" spans="1:17">
-      <c r="A148" s="8"/>
-      <c r="B148" s="5"/>
+      <c r="A148" s="10"/>
+      <c r="B148" s="9"/>
       <c r="C148" s="1"/>
       <c r="D148" s="1"/>
       <c r="E148" s="1"/>
@@ -3523,8 +3526,8 @@
       <c r="Q148" s="1"/>
     </row>
     <row r="149" spans="1:17">
-      <c r="A149" s="8"/>
-      <c r="B149" s="5"/>
+      <c r="A149" s="10"/>
+      <c r="B149" s="9"/>
       <c r="C149" s="1"/>
       <c r="D149" s="1"/>
       <c r="E149" s="1"/>
@@ -3542,8 +3545,8 @@
       <c r="Q149" s="1"/>
     </row>
     <row r="150" spans="1:17">
-      <c r="A150" s="8"/>
-      <c r="B150" s="5"/>
+      <c r="A150" s="10"/>
+      <c r="B150" s="9"/>
       <c r="C150" s="1"/>
       <c r="D150" s="1"/>
       <c r="E150" s="1"/>
@@ -3561,8 +3564,8 @@
       <c r="Q150" s="1"/>
     </row>
     <row r="151" spans="1:17">
-      <c r="A151" s="8"/>
-      <c r="B151" s="5"/>
+      <c r="A151" s="10"/>
+      <c r="B151" s="9"/>
       <c r="C151" s="1"/>
       <c r="D151" s="1"/>
       <c r="E151" s="1"/>
@@ -3580,8 +3583,8 @@
       <c r="Q151" s="1"/>
     </row>
     <row r="152" spans="1:17">
-      <c r="A152" s="8"/>
-      <c r="B152" s="5"/>
+      <c r="A152" s="10"/>
+      <c r="B152" s="9"/>
       <c r="C152" s="1"/>
       <c r="D152" s="1"/>
       <c r="E152" s="1"/>
@@ -3599,8 +3602,8 @@
       <c r="Q152" s="1"/>
     </row>
     <row r="153" spans="1:17">
-      <c r="A153" s="8"/>
-      <c r="B153" s="5"/>
+      <c r="A153" s="10"/>
+      <c r="B153" s="9"/>
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
       <c r="E153" s="1"/>
@@ -3618,8 +3621,8 @@
       <c r="Q153" s="1"/>
     </row>
     <row r="154" spans="1:17">
-      <c r="A154" s="8"/>
-      <c r="B154" s="5"/>
+      <c r="A154" s="10"/>
+      <c r="B154" s="9"/>
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
       <c r="E154" s="1"/>
@@ -3637,8 +3640,8 @@
       <c r="Q154" s="1"/>
     </row>
     <row r="155" spans="1:17">
-      <c r="A155" s="8"/>
-      <c r="B155" s="5"/>
+      <c r="A155" s="10"/>
+      <c r="B155" s="9"/>
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
       <c r="E155" s="1"/>
@@ -3656,8 +3659,8 @@
       <c r="Q155" s="1"/>
     </row>
     <row r="156" spans="1:17">
-      <c r="A156" s="8"/>
-      <c r="B156" s="5"/>
+      <c r="A156" s="10"/>
+      <c r="B156" s="9"/>
       <c r="C156" s="1"/>
       <c r="D156" s="1"/>
       <c r="E156" s="1"/>
@@ -3675,8 +3678,8 @@
       <c r="Q156" s="1"/>
     </row>
     <row r="157" spans="1:17">
-      <c r="A157" s="8"/>
-      <c r="B157" s="5"/>
+      <c r="A157" s="10"/>
+      <c r="B157" s="9"/>
       <c r="C157" s="1"/>
       <c r="D157" s="1"/>
       <c r="E157" s="1"/>
@@ -3694,8 +3697,8 @@
       <c r="Q157" s="1"/>
     </row>
     <row r="158" spans="1:17">
-      <c r="A158" s="8"/>
-      <c r="B158" s="5"/>
+      <c r="A158" s="10"/>
+      <c r="B158" s="9"/>
       <c r="C158" s="1"/>
       <c r="D158" s="1"/>
       <c r="E158" s="1"/>
@@ -3713,8 +3716,8 @@
       <c r="Q158" s="1"/>
     </row>
     <row r="159" spans="1:17">
-      <c r="A159" s="8"/>
-      <c r="B159" s="5"/>
+      <c r="A159" s="10"/>
+      <c r="B159" s="9"/>
       <c r="C159" s="1"/>
       <c r="D159" s="1"/>
       <c r="E159" s="1"/>
@@ -3732,8 +3735,8 @@
       <c r="Q159" s="1"/>
     </row>
     <row r="160" spans="1:17">
-      <c r="A160" s="8"/>
-      <c r="B160" s="5"/>
+      <c r="A160" s="10"/>
+      <c r="B160" s="9"/>
       <c r="C160" s="1"/>
       <c r="D160" s="1"/>
       <c r="E160" s="1"/>
@@ -3751,8 +3754,8 @@
       <c r="Q160" s="1"/>
     </row>
     <row r="161" spans="1:17">
-      <c r="A161" s="8"/>
-      <c r="B161" s="5"/>
+      <c r="A161" s="10"/>
+      <c r="B161" s="9"/>
       <c r="C161" s="1"/>
       <c r="D161" s="1"/>
       <c r="E161" s="1"/>
@@ -3770,8 +3773,8 @@
       <c r="Q161" s="1"/>
     </row>
     <row r="162" spans="1:17">
-      <c r="A162" s="8"/>
-      <c r="B162" s="5"/>
+      <c r="A162" s="10"/>
+      <c r="B162" s="9"/>
       <c r="C162" s="1"/>
       <c r="D162" s="1"/>
       <c r="E162" s="1"/>
@@ -3789,8 +3792,8 @@
       <c r="Q162" s="1"/>
     </row>
     <row r="163" spans="1:17">
-      <c r="A163" s="8"/>
-      <c r="B163" s="5"/>
+      <c r="A163" s="10"/>
+      <c r="B163" s="9"/>
       <c r="C163" s="1"/>
       <c r="D163" s="1"/>
       <c r="E163" s="1"/>
@@ -3808,8 +3811,8 @@
       <c r="Q163" s="1"/>
     </row>
     <row r="164" spans="1:17">
-      <c r="A164" s="8"/>
-      <c r="B164" s="5"/>
+      <c r="A164" s="10"/>
+      <c r="B164" s="9"/>
       <c r="C164" s="1"/>
       <c r="D164" s="1"/>
       <c r="E164" s="1"/>
@@ -3827,8 +3830,8 @@
       <c r="Q164" s="1"/>
     </row>
     <row r="165" spans="1:17">
-      <c r="A165" s="8"/>
-      <c r="B165" s="5"/>
+      <c r="A165" s="10"/>
+      <c r="B165" s="9"/>
       <c r="C165" s="1"/>
       <c r="D165" s="1"/>
       <c r="E165" s="1"/>
@@ -3846,8 +3849,8 @@
       <c r="Q165" s="1"/>
     </row>
     <row r="166" spans="1:17">
-      <c r="A166" s="8"/>
-      <c r="B166" s="5"/>
+      <c r="A166" s="10"/>
+      <c r="B166" s="9"/>
       <c r="C166" s="1"/>
       <c r="D166" s="1"/>
       <c r="E166" s="1"/>
@@ -3865,8 +3868,8 @@
       <c r="Q166" s="1"/>
     </row>
     <row r="167" spans="1:17">
-      <c r="A167" s="8"/>
-      <c r="B167" s="5"/>
+      <c r="A167" s="10"/>
+      <c r="B167" s="9"/>
       <c r="C167" s="1"/>
       <c r="D167" s="1"/>
       <c r="E167" s="1"/>
@@ -3884,8 +3887,8 @@
       <c r="Q167" s="1"/>
     </row>
     <row r="168" spans="1:17">
-      <c r="A168" s="8"/>
-      <c r="B168" s="5"/>
+      <c r="A168" s="10"/>
+      <c r="B168" s="9"/>
       <c r="C168" s="1"/>
       <c r="D168" s="1"/>
       <c r="E168" s="1"/>
@@ -3903,8 +3906,8 @@
       <c r="Q168" s="1"/>
     </row>
     <row r="169" spans="1:17">
-      <c r="A169" s="8"/>
-      <c r="B169" s="5"/>
+      <c r="A169" s="10"/>
+      <c r="B169" s="9"/>
       <c r="C169" s="1"/>
       <c r="D169" s="1"/>
       <c r="E169" s="1"/>
@@ -3922,8 +3925,8 @@
       <c r="Q169" s="1"/>
     </row>
     <row r="170" spans="1:17">
-      <c r="A170" s="8"/>
-      <c r="B170" s="5"/>
+      <c r="A170" s="10"/>
+      <c r="B170" s="9"/>
       <c r="C170" s="1"/>
       <c r="D170" s="1"/>
       <c r="E170" s="1"/>
@@ -3941,8 +3944,8 @@
       <c r="Q170" s="1"/>
     </row>
     <row r="171" spans="1:17">
-      <c r="A171" s="8"/>
-      <c r="B171" s="5"/>
+      <c r="A171" s="10"/>
+      <c r="B171" s="9"/>
       <c r="C171" s="1"/>
       <c r="D171" s="1"/>
       <c r="E171" s="1"/>
@@ -3960,8 +3963,8 @@
       <c r="Q171" s="1"/>
     </row>
     <row r="172" spans="1:17">
-      <c r="A172" s="8"/>
-      <c r="B172" s="5"/>
+      <c r="A172" s="10"/>
+      <c r="B172" s="9"/>
       <c r="C172" s="1"/>
       <c r="D172" s="1"/>
       <c r="E172" s="1"/>
@@ -3979,8 +3982,8 @@
       <c r="Q172" s="1"/>
     </row>
     <row r="173" spans="1:17">
-      <c r="A173" s="8"/>
-      <c r="B173" s="5"/>
+      <c r="A173" s="10"/>
+      <c r="B173" s="9"/>
       <c r="C173" s="1"/>
       <c r="D173" s="1"/>
       <c r="E173" s="1"/>
@@ -3998,8 +4001,8 @@
       <c r="Q173" s="1"/>
     </row>
     <row r="174" spans="1:17">
-      <c r="A174" s="8"/>
-      <c r="B174" s="5"/>
+      <c r="A174" s="10"/>
+      <c r="B174" s="9"/>
       <c r="C174" s="1"/>
       <c r="D174" s="1"/>
       <c r="E174" s="1"/>
@@ -4017,8 +4020,8 @@
       <c r="Q174" s="1"/>
     </row>
     <row r="175" spans="1:17">
-      <c r="A175" s="8"/>
-      <c r="B175" s="5"/>
+      <c r="A175" s="10"/>
+      <c r="B175" s="9"/>
       <c r="C175" s="1"/>
       <c r="D175" s="1"/>
       <c r="E175" s="1"/>
@@ -4036,8 +4039,8 @@
       <c r="Q175" s="1"/>
     </row>
     <row r="176" spans="1:17">
-      <c r="A176" s="8"/>
-      <c r="B176" s="5"/>
+      <c r="A176" s="10"/>
+      <c r="B176" s="9"/>
       <c r="C176" s="1"/>
       <c r="D176" s="1"/>
       <c r="E176" s="1"/>
@@ -4055,8 +4058,8 @@
       <c r="Q176" s="1"/>
     </row>
     <row r="177" spans="1:17">
-      <c r="A177" s="8"/>
-      <c r="B177" s="5"/>
+      <c r="A177" s="10"/>
+      <c r="B177" s="9"/>
       <c r="C177" s="1"/>
       <c r="D177" s="1"/>
       <c r="E177" s="1"/>
@@ -4074,8 +4077,8 @@
       <c r="Q177" s="1"/>
     </row>
     <row r="178" spans="1:17">
-      <c r="A178" s="8"/>
-      <c r="B178" s="5"/>
+      <c r="A178" s="10"/>
+      <c r="B178" s="9"/>
       <c r="C178" s="1"/>
       <c r="D178" s="1"/>
       <c r="E178" s="1"/>
@@ -4093,8 +4096,8 @@
       <c r="Q178" s="1"/>
     </row>
     <row r="179" spans="1:17">
-      <c r="A179" s="8"/>
-      <c r="B179" s="5"/>
+      <c r="A179" s="10"/>
+      <c r="B179" s="9"/>
       <c r="C179" s="1"/>
       <c r="D179" s="1"/>
       <c r="E179" s="1"/>
@@ -4112,8 +4115,8 @@
       <c r="Q179" s="1"/>
     </row>
     <row r="180" spans="1:17">
-      <c r="A180" s="8"/>
-      <c r="B180" s="5"/>
+      <c r="A180" s="10"/>
+      <c r="B180" s="9"/>
       <c r="C180" s="1"/>
       <c r="D180" s="1"/>
       <c r="E180" s="1"/>
@@ -4131,8 +4134,8 @@
       <c r="Q180" s="1"/>
     </row>
     <row r="181" spans="1:17">
-      <c r="A181" s="8"/>
-      <c r="B181" s="5"/>
+      <c r="A181" s="10"/>
+      <c r="B181" s="9"/>
       <c r="C181" s="1"/>
       <c r="D181" s="1"/>
       <c r="E181" s="1"/>
@@ -4150,8 +4153,8 @@
       <c r="Q181" s="1"/>
     </row>
     <row r="182" spans="1:17">
-      <c r="A182" s="8"/>
-      <c r="B182" s="5"/>
+      <c r="A182" s="10"/>
+      <c r="B182" s="9"/>
       <c r="C182" s="1"/>
       <c r="D182" s="1"/>
       <c r="E182" s="1"/>
@@ -4169,8 +4172,8 @@
       <c r="Q182" s="1"/>
     </row>
     <row r="183" spans="1:17">
-      <c r="A183" s="8"/>
-      <c r="B183" s="5"/>
+      <c r="A183" s="10"/>
+      <c r="B183" s="9"/>
       <c r="C183" s="1"/>
       <c r="D183" s="1"/>
       <c r="E183" s="1"/>
@@ -4188,8 +4191,8 @@
       <c r="Q183" s="1"/>
     </row>
     <row r="184" spans="1:17">
-      <c r="A184" s="8"/>
-      <c r="B184" s="5"/>
+      <c r="A184" s="10"/>
+      <c r="B184" s="9"/>
       <c r="C184" s="1"/>
       <c r="D184" s="1"/>
       <c r="E184" s="1"/>
@@ -4207,8 +4210,8 @@
       <c r="Q184" s="1"/>
     </row>
     <row r="185" spans="1:17">
-      <c r="A185" s="8"/>
-      <c r="B185" s="5"/>
+      <c r="A185" s="10"/>
+      <c r="B185" s="9"/>
       <c r="C185" s="1"/>
       <c r="D185" s="1"/>
       <c r="E185" s="1"/>
@@ -4226,8 +4229,8 @@
       <c r="Q185" s="1"/>
     </row>
     <row r="186" spans="1:17">
-      <c r="A186" s="8"/>
-      <c r="B186" s="5"/>
+      <c r="A186" s="10"/>
+      <c r="B186" s="9"/>
       <c r="C186" s="1"/>
       <c r="D186" s="1"/>
       <c r="E186" s="1"/>
@@ -4245,8 +4248,8 @@
       <c r="Q186" s="1"/>
     </row>
     <row r="187" spans="1:17">
-      <c r="A187" s="8"/>
-      <c r="B187" s="5"/>
+      <c r="A187" s="10"/>
+      <c r="B187" s="9"/>
       <c r="C187" s="1"/>
       <c r="D187" s="1"/>
       <c r="E187" s="1"/>
@@ -4264,8 +4267,8 @@
       <c r="Q187" s="1"/>
     </row>
     <row r="188" spans="1:17">
-      <c r="A188" s="8"/>
-      <c r="B188" s="5"/>
+      <c r="A188" s="10"/>
+      <c r="B188" s="9"/>
       <c r="C188" s="1"/>
       <c r="D188" s="1"/>
       <c r="E188" s="1"/>
@@ -4283,8 +4286,8 @@
       <c r="Q188" s="1"/>
     </row>
     <row r="189" spans="1:17">
-      <c r="A189" s="8"/>
-      <c r="B189" s="5"/>
+      <c r="A189" s="10"/>
+      <c r="B189" s="9"/>
       <c r="C189" s="1"/>
       <c r="D189" s="1"/>
       <c r="E189" s="1"/>
@@ -4302,8 +4305,8 @@
       <c r="Q189" s="1"/>
     </row>
     <row r="190" spans="1:17">
-      <c r="A190" s="8"/>
-      <c r="B190" s="5"/>
+      <c r="A190" s="10"/>
+      <c r="B190" s="9"/>
       <c r="C190" s="1"/>
       <c r="D190" s="1"/>
       <c r="E190" s="1"/>
@@ -4321,8 +4324,8 @@
       <c r="Q190" s="1"/>
     </row>
     <row r="191" spans="1:17">
-      <c r="A191" s="8"/>
-      <c r="B191" s="5"/>
+      <c r="A191" s="10"/>
+      <c r="B191" s="9"/>
       <c r="C191" s="1"/>
       <c r="D191" s="1"/>
       <c r="E191" s="1"/>
@@ -4340,8 +4343,8 @@
       <c r="Q191" s="1"/>
     </row>
     <row r="192" spans="1:17">
-      <c r="A192" s="8"/>
-      <c r="B192" s="5"/>
+      <c r="A192" s="10"/>
+      <c r="B192" s="9"/>
       <c r="C192" s="1"/>
       <c r="D192" s="1"/>
       <c r="E192" s="1"/>
@@ -4359,8 +4362,8 @@
       <c r="Q192" s="1"/>
     </row>
     <row r="193" spans="1:17">
-      <c r="A193" s="8"/>
-      <c r="B193" s="5"/>
+      <c r="A193" s="10"/>
+      <c r="B193" s="9"/>
       <c r="C193" s="1"/>
       <c r="D193" s="1"/>
       <c r="E193" s="1"/>
@@ -4378,8 +4381,8 @@
       <c r="Q193" s="1"/>
     </row>
     <row r="194" spans="1:17">
-      <c r="A194" s="8"/>
-      <c r="B194" s="5"/>
+      <c r="A194" s="10"/>
+      <c r="B194" s="9"/>
       <c r="C194" s="1"/>
       <c r="D194" s="1"/>
       <c r="E194" s="1"/>
@@ -4397,8 +4400,8 @@
       <c r="Q194" s="1"/>
     </row>
     <row r="195" spans="1:17">
-      <c r="A195" s="8"/>
-      <c r="B195" s="5"/>
+      <c r="A195" s="10"/>
+      <c r="B195" s="9"/>
       <c r="C195" s="1"/>
       <c r="D195" s="1"/>
       <c r="E195" s="1"/>
@@ -4416,8 +4419,8 @@
       <c r="Q195" s="1"/>
     </row>
     <row r="196" spans="1:17">
-      <c r="A196" s="8"/>
-      <c r="B196" s="5"/>
+      <c r="A196" s="10"/>
+      <c r="B196" s="9"/>
       <c r="C196" s="1"/>
       <c r="D196" s="1"/>
       <c r="E196" s="1"/>
@@ -4435,8 +4438,8 @@
       <c r="Q196" s="1"/>
     </row>
     <row r="197" spans="1:17">
-      <c r="A197" s="8"/>
-      <c r="B197" s="5"/>
+      <c r="A197" s="10"/>
+      <c r="B197" s="9"/>
       <c r="C197" s="1"/>
       <c r="D197" s="1"/>
       <c r="E197" s="1"/>
@@ -4454,8 +4457,8 @@
       <c r="Q197" s="1"/>
     </row>
     <row r="198" spans="1:17">
-      <c r="A198" s="8"/>
-      <c r="B198" s="5"/>
+      <c r="A198" s="10"/>
+      <c r="B198" s="9"/>
       <c r="C198" s="1"/>
       <c r="D198" s="1"/>
       <c r="E198" s="1"/>
@@ -4473,8 +4476,8 @@
       <c r="Q198" s="1"/>
     </row>
     <row r="199" spans="1:17">
-      <c r="A199" s="8"/>
-      <c r="B199" s="5"/>
+      <c r="A199" s="10"/>
+      <c r="B199" s="9"/>
       <c r="C199" s="1"/>
       <c r="D199" s="1"/>
       <c r="E199" s="1"/>
@@ -4492,8 +4495,8 @@
       <c r="Q199" s="1"/>
     </row>
     <row r="200" spans="1:17">
-      <c r="A200" s="8"/>
-      <c r="B200" s="5"/>
+      <c r="A200" s="10"/>
+      <c r="B200" s="9"/>
       <c r="C200" s="1"/>
       <c r="D200" s="1"/>
       <c r="E200" s="1"/>
@@ -4511,8 +4514,8 @@
       <c r="Q200" s="1"/>
     </row>
     <row r="201" spans="1:17">
-      <c r="A201" s="8"/>
-      <c r="B201" s="5"/>
+      <c r="A201" s="10"/>
+      <c r="B201" s="9"/>
       <c r="C201" s="1"/>
       <c r="D201" s="1"/>
       <c r="E201" s="1"/>
@@ -4530,8 +4533,8 @@
       <c r="Q201" s="1"/>
     </row>
     <row r="202" spans="1:17">
-      <c r="A202" s="8"/>
-      <c r="B202" s="5"/>
+      <c r="A202" s="10"/>
+      <c r="B202" s="9"/>
       <c r="C202" s="1"/>
       <c r="D202" s="1"/>
       <c r="E202" s="1"/>
@@ -4549,8 +4552,8 @@
       <c r="Q202" s="1"/>
     </row>
     <row r="203" spans="1:17">
-      <c r="A203" s="8"/>
-      <c r="B203" s="5"/>
+      <c r="A203" s="10"/>
+      <c r="B203" s="9"/>
       <c r="C203" s="1"/>
       <c r="D203" s="1"/>
       <c r="E203" s="1"/>
@@ -4568,8 +4571,8 @@
       <c r="Q203" s="1"/>
     </row>
     <row r="204" spans="1:17">
-      <c r="A204" s="8"/>
-      <c r="B204" s="5"/>
+      <c r="A204" s="10"/>
+      <c r="B204" s="9"/>
       <c r="C204" s="1"/>
       <c r="D204" s="1"/>
       <c r="E204" s="1"/>
@@ -4587,8 +4590,8 @@
       <c r="Q204" s="1"/>
     </row>
     <row r="205" spans="1:17">
-      <c r="A205" s="8"/>
-      <c r="B205" s="5"/>
+      <c r="A205" s="10"/>
+      <c r="B205" s="9"/>
       <c r="C205" s="1"/>
       <c r="D205" s="1"/>
       <c r="E205" s="1"/>
@@ -4606,8 +4609,8 @@
       <c r="Q205" s="1"/>
     </row>
     <row r="206" spans="1:17">
-      <c r="A206" s="8"/>
-      <c r="B206" s="5"/>
+      <c r="A206" s="10"/>
+      <c r="B206" s="9"/>
       <c r="C206" s="1"/>
       <c r="D206" s="1"/>
       <c r="E206" s="1"/>
@@ -4625,8 +4628,8 @@
       <c r="Q206" s="1"/>
     </row>
     <row r="207" spans="1:17">
-      <c r="A207" s="8"/>
-      <c r="B207" s="5"/>
+      <c r="A207" s="10"/>
+      <c r="B207" s="9"/>
       <c r="C207" s="1"/>
       <c r="D207" s="1"/>
       <c r="E207" s="1"/>
@@ -4644,8 +4647,8 @@
       <c r="Q207" s="1"/>
     </row>
     <row r="208" spans="1:17">
-      <c r="A208" s="8"/>
-      <c r="B208" s="5"/>
+      <c r="A208" s="10"/>
+      <c r="B208" s="9"/>
       <c r="C208" s="1"/>
       <c r="D208" s="1"/>
       <c r="E208" s="1"/>
@@ -4663,8 +4666,8 @@
       <c r="Q208" s="1"/>
     </row>
     <row r="209" spans="1:17">
-      <c r="A209" s="8"/>
-      <c r="B209" s="5"/>
+      <c r="A209" s="10"/>
+      <c r="B209" s="9"/>
       <c r="C209" s="1"/>
       <c r="D209" s="1"/>
       <c r="E209" s="1"/>
@@ -4682,8 +4685,8 @@
       <c r="Q209" s="1"/>
     </row>
     <row r="210" spans="1:17">
-      <c r="A210" s="8"/>
-      <c r="B210" s="5"/>
+      <c r="A210" s="10"/>
+      <c r="B210" s="9"/>
       <c r="C210" s="1"/>
       <c r="D210" s="1"/>
       <c r="E210" s="1"/>
@@ -4701,8 +4704,8 @@
       <c r="Q210" s="1"/>
     </row>
     <row r="211" spans="1:17">
-      <c r="A211" s="8"/>
-      <c r="B211" s="5"/>
+      <c r="A211" s="10"/>
+      <c r="B211" s="9"/>
       <c r="C211" s="1"/>
       <c r="D211" s="1"/>
       <c r="E211" s="1"/>
@@ -4720,8 +4723,8 @@
       <c r="Q211" s="1"/>
     </row>
     <row r="212" spans="1:17">
-      <c r="A212" s="8"/>
-      <c r="B212" s="5"/>
+      <c r="A212" s="10"/>
+      <c r="B212" s="9"/>
       <c r="C212" s="1"/>
       <c r="D212" s="1"/>
       <c r="E212" s="1"/>
@@ -4739,8 +4742,8 @@
       <c r="Q212" s="1"/>
     </row>
     <row r="213" spans="1:17">
-      <c r="A213" s="8"/>
-      <c r="B213" s="5"/>
+      <c r="A213" s="10"/>
+      <c r="B213" s="9"/>
       <c r="C213" s="1"/>
       <c r="D213" s="1"/>
       <c r="E213" s="1"/>
@@ -4758,8 +4761,8 @@
       <c r="Q213" s="1"/>
     </row>
     <row r="214" spans="1:17">
-      <c r="A214" s="8"/>
-      <c r="B214" s="5"/>
+      <c r="A214" s="10"/>
+      <c r="B214" s="9"/>
       <c r="C214" s="1"/>
       <c r="D214" s="1"/>
       <c r="E214" s="1"/>
@@ -4777,8 +4780,8 @@
       <c r="Q214" s="1"/>
     </row>
     <row r="215" spans="1:17">
-      <c r="A215" s="8"/>
-      <c r="B215" s="5"/>
+      <c r="A215" s="10"/>
+      <c r="B215" s="9"/>
       <c r="C215" s="1"/>
       <c r="D215" s="1"/>
       <c r="E215" s="1"/>
@@ -4796,8 +4799,8 @@
       <c r="Q215" s="1"/>
     </row>
     <row r="216" spans="1:17">
-      <c r="A216" s="8"/>
-      <c r="B216" s="5"/>
+      <c r="A216" s="10"/>
+      <c r="B216" s="9"/>
       <c r="C216" s="1"/>
       <c r="D216" s="1"/>
       <c r="E216" s="1"/>
@@ -4815,8 +4818,8 @@
       <c r="Q216" s="1"/>
     </row>
     <row r="217" spans="1:17">
-      <c r="A217" s="8"/>
-      <c r="B217" s="5"/>
+      <c r="A217" s="10"/>
+      <c r="B217" s="9"/>
       <c r="C217" s="1"/>
       <c r="D217" s="1"/>
       <c r="E217" s="1"/>
@@ -4834,8 +4837,8 @@
       <c r="Q217" s="1"/>
     </row>
     <row r="218" spans="1:17">
-      <c r="A218" s="8"/>
-      <c r="B218" s="5"/>
+      <c r="A218" s="10"/>
+      <c r="B218" s="9"/>
       <c r="C218" s="1"/>
       <c r="D218" s="1"/>
       <c r="E218" s="1"/>
@@ -4853,8 +4856,8 @@
       <c r="Q218" s="1"/>
     </row>
     <row r="219" spans="1:17">
-      <c r="A219" s="8"/>
-      <c r="B219" s="5"/>
+      <c r="A219" s="10"/>
+      <c r="B219" s="9"/>
       <c r="C219" s="1"/>
       <c r="D219" s="1"/>
       <c r="E219" s="1"/>
@@ -4872,8 +4875,8 @@
       <c r="Q219" s="1"/>
     </row>
     <row r="220" spans="1:17">
-      <c r="A220" s="8"/>
-      <c r="B220" s="5"/>
+      <c r="A220" s="10"/>
+      <c r="B220" s="9"/>
       <c r="C220" s="1"/>
       <c r="D220" s="1"/>
       <c r="E220" s="1"/>
@@ -4891,8 +4894,8 @@
       <c r="Q220" s="1"/>
     </row>
     <row r="221" spans="1:17">
-      <c r="A221" s="8"/>
-      <c r="B221" s="5"/>
+      <c r="A221" s="10"/>
+      <c r="B221" s="9"/>
       <c r="C221" s="1"/>
       <c r="D221" s="1"/>
       <c r="E221" s="1"/>
@@ -4910,8 +4913,8 @@
       <c r="Q221" s="1"/>
     </row>
     <row r="222" spans="1:17">
-      <c r="A222" s="8"/>
-      <c r="B222" s="5"/>
+      <c r="A222" s="10"/>
+      <c r="B222" s="9"/>
       <c r="C222" s="1"/>
       <c r="D222" s="1"/>
       <c r="E222" s="1"/>
@@ -4929,8 +4932,8 @@
       <c r="Q222" s="1"/>
     </row>
     <row r="223" spans="1:17">
-      <c r="A223" s="8"/>
-      <c r="B223" s="5"/>
+      <c r="A223" s="10"/>
+      <c r="B223" s="9"/>
       <c r="C223" s="1"/>
       <c r="D223" s="1"/>
       <c r="E223" s="1"/>
@@ -4948,8 +4951,8 @@
       <c r="Q223" s="1"/>
     </row>
     <row r="224" spans="1:17">
-      <c r="A224" s="8"/>
-      <c r="B224" s="5"/>
+      <c r="A224" s="10"/>
+      <c r="B224" s="9"/>
       <c r="C224" s="1"/>
       <c r="D224" s="1"/>
       <c r="E224" s="1"/>
@@ -4967,8 +4970,8 @@
       <c r="Q224" s="1"/>
     </row>
     <row r="225" spans="1:17">
-      <c r="A225" s="8"/>
-      <c r="B225" s="5"/>
+      <c r="A225" s="10"/>
+      <c r="B225" s="9"/>
       <c r="C225" s="1"/>
       <c r="D225" s="1"/>
       <c r="E225" s="1"/>
@@ -4986,8 +4989,8 @@
       <c r="Q225" s="1"/>
     </row>
     <row r="226" spans="1:17">
-      <c r="A226" s="8"/>
-      <c r="B226" s="5"/>
+      <c r="A226" s="10"/>
+      <c r="B226" s="9"/>
       <c r="C226" s="1"/>
       <c r="D226" s="1"/>
       <c r="E226" s="1"/>
@@ -5005,8 +5008,8 @@
       <c r="Q226" s="1"/>
     </row>
     <row r="227" spans="1:17">
-      <c r="A227" s="8"/>
-      <c r="B227" s="5"/>
+      <c r="A227" s="10"/>
+      <c r="B227" s="9"/>
       <c r="C227" s="1"/>
       <c r="D227" s="1"/>
       <c r="E227" s="1"/>
@@ -5024,8 +5027,8 @@
       <c r="Q227" s="1"/>
     </row>
     <row r="228" spans="1:17">
-      <c r="A228" s="8"/>
-      <c r="B228" s="5"/>
+      <c r="A228" s="10"/>
+      <c r="B228" s="9"/>
       <c r="C228" s="1"/>
       <c r="D228" s="1"/>
       <c r="E228" s="1"/>
@@ -5043,8 +5046,8 @@
       <c r="Q228" s="1"/>
     </row>
     <row r="229" spans="1:17">
-      <c r="A229" s="8"/>
-      <c r="B229" s="5"/>
+      <c r="A229" s="10"/>
+      <c r="B229" s="9"/>
       <c r="C229" s="1"/>
       <c r="D229" s="1"/>
       <c r="E229" s="1"/>
@@ -5062,8 +5065,8 @@
       <c r="Q229" s="1"/>
     </row>
     <row r="230" spans="1:17">
-      <c r="A230" s="8"/>
-      <c r="B230" s="5"/>
+      <c r="A230" s="10"/>
+      <c r="B230" s="9"/>
       <c r="C230" s="1"/>
       <c r="D230" s="1"/>
       <c r="E230" s="1"/>
@@ -5081,7 +5084,7 @@
       <c r="Q230" s="1"/>
     </row>
     <row r="231" spans="1:17">
-      <c r="A231" s="8"/>
+      <c r="A231" s="10"/>
       <c r="B231" s="5"/>
       <c r="C231" s="1"/>
       <c r="D231" s="1"/>

</xml_diff>

<commit_message>
Lisää paikkauskohteen kokonaismassamäärä UREM-Exceliin
</commit_message>
<xml_diff>
--- a/dev-resources/excel/harja_urapaikkaustoteumien_tuonti_pohja.xlsx
+++ b/dev-resources/excel/harja_urapaikkaustoteumien_tuonti_pohja.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_aa5\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarnova/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E150476B-3057-408F-BB4A-608924D21589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC63463F-30EF-CA47-B5AF-2835C7687D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="56200" yWindow="9880" windowWidth="40040" windowHeight="22460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Urapaikkaustoteumien tuonti" sheetId="1" r:id="rId1"/>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Materiaali</t>
-  </si>
-  <si>
-    <t>Määrä</t>
   </si>
   <si>
     <t>Työ alkoi *</t>
@@ -103,9 +100,6 @@
   </si>
   <si>
     <t>KM-luokka *</t>
-  </si>
-  <si>
-    <t>Kok. Massamäärä (t) *</t>
   </si>
   <si>
     <t>Massatyyppi</t>
@@ -161,6 +155,12 @@
   <si>
     <t>SOP, Soratien pintaus</t>
   </si>
+  <si>
+    <t xml:space="preserve">Kohteen kokonaismassamäärä (t) *: </t>
+  </si>
+  <si>
+    <t>&lt;- Syötä kohteen kokonaismassamäärä tonneissa. Harjassa lasketaan pinta-alan perusteella rivikohtainen suhteellinen tonnimäärä ja massamenekki (kg/m2)</t>
+  </si>
 </sst>
 </file>
 
@@ -168,9 +168,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-40B]d/m/yyyy\ hh:mm"/>
-    <numFmt numFmtId="166" formatCode="[$-40B]d:m:yyyy\ hh:mm"/>
+    <numFmt numFmtId="165" formatCode="[$-40B]d:m:yyyy\ hh:mm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -180,15 +180,18 @@
     <font>
       <sz val="16"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -217,7 +220,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -240,11 +243,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -254,14 +292,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -641,231 +691,222 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q232"/>
+  <dimension ref="A1:P235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A219" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B230"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" customWidth="1"/>
+    <col min="1" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.83203125" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" customWidth="1"/>
+    <col min="7" max="7" width="7.5" customWidth="1"/>
+    <col min="8" max="8" width="6.5" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
     <col min="10" max="10" width="8" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" customWidth="1"/>
-    <col min="14" max="14" width="27.5703125" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.83203125" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" customWidth="1"/>
+    <col min="13" max="13" width="12.5" customWidth="1"/>
+    <col min="14" max="14" width="27.5" customWidth="1"/>
+    <col min="15" max="15" width="10.5" customWidth="1"/>
     <col min="16" max="16" width="12" customWidth="1"/>
-    <col min="17" max="17" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="21">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="13" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+    </row>
+    <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+    </row>
+    <row r="3" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+    </row>
+    <row r="4" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+    </row>
+    <row r="5" spans="1:16" ht="14" x14ac:dyDescent="0.2">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="2"/>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4" t="s">
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+    </row>
+    <row r="6" spans="1:16" ht="14" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="3" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="4" t="s">
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="3" t="s">
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+    </row>
+    <row r="7" spans="1:16" ht="14" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="O7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="P7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="P4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="10"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="6"/>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" s="10"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="10"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="1"/>
-    </row>
-    <row r="8" spans="1:17">
+    </row>
+    <row r="8" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="9"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>
-      <c r="Q8" s="1"/>
-    </row>
-    <row r="9" spans="1:17">
+    </row>
+    <row r="9" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
       <c r="B9" s="9"/>
       <c r="C9" s="1"/>
@@ -882,9 +923,8 @@
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
-      <c r="Q9" s="1"/>
-    </row>
-    <row r="10" spans="1:17">
+    </row>
+    <row r="10" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A10" s="10"/>
       <c r="B10" s="9"/>
       <c r="C10" s="1"/>
@@ -901,9 +941,8 @@
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
       <c r="P10" s="7"/>
-      <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="1:17">
+    </row>
+    <row r="11" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
       <c r="B11" s="9"/>
       <c r="C11" s="1"/>
@@ -920,9 +959,8 @@
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
-      <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="1:17">
+    </row>
+    <row r="12" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A12" s="10"/>
       <c r="B12" s="9"/>
       <c r="C12" s="1"/>
@@ -939,9 +977,8 @@
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
       <c r="P12" s="7"/>
-      <c r="Q12" s="1"/>
-    </row>
-    <row r="13" spans="1:17">
+    </row>
+    <row r="13" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
       <c r="B13" s="9"/>
       <c r="C13" s="1"/>
@@ -958,9 +995,8 @@
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
       <c r="P13" s="7"/>
-      <c r="Q13" s="1"/>
-    </row>
-    <row r="14" spans="1:17">
+    </row>
+    <row r="14" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
       <c r="B14" s="9"/>
       <c r="C14" s="1"/>
@@ -977,9 +1013,8 @@
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
-      <c r="Q14" s="1"/>
-    </row>
-    <row r="15" spans="1:17">
+    </row>
+    <row r="15" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
       <c r="B15" s="9"/>
       <c r="C15" s="1"/>
@@ -996,9 +1031,8 @@
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
-      <c r="Q15" s="1"/>
-    </row>
-    <row r="16" spans="1:17">
+    </row>
+    <row r="16" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A16" s="10"/>
       <c r="B16" s="9"/>
       <c r="C16" s="1"/>
@@ -1015,9 +1049,8 @@
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
-      <c r="Q16" s="1"/>
-    </row>
-    <row r="17" spans="1:17">
+    </row>
+    <row r="17" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A17" s="10"/>
       <c r="B17" s="9"/>
       <c r="C17" s="1"/>
@@ -1034,9 +1067,8 @@
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
-      <c r="Q17" s="1"/>
-    </row>
-    <row r="18" spans="1:17">
+    </row>
+    <row r="18" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A18" s="10"/>
       <c r="B18" s="9"/>
       <c r="C18" s="1"/>
@@ -1053,9 +1085,8 @@
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
       <c r="P18" s="7"/>
-      <c r="Q18" s="1"/>
-    </row>
-    <row r="19" spans="1:17">
+    </row>
+    <row r="19" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A19" s="10"/>
       <c r="B19" s="9"/>
       <c r="C19" s="1"/>
@@ -1072,9 +1103,8 @@
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
-      <c r="Q19" s="1"/>
-    </row>
-    <row r="20" spans="1:17">
+    </row>
+    <row r="20" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A20" s="10"/>
       <c r="B20" s="9"/>
       <c r="C20" s="1"/>
@@ -1091,9 +1121,8 @@
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
       <c r="P20" s="7"/>
-      <c r="Q20" s="1"/>
-    </row>
-    <row r="21" spans="1:17">
+    </row>
+    <row r="21" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
       <c r="B21" s="9"/>
       <c r="C21" s="1"/>
@@ -1110,9 +1139,8 @@
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
       <c r="P21" s="7"/>
-      <c r="Q21" s="1"/>
-    </row>
-    <row r="22" spans="1:17">
+    </row>
+    <row r="22" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
       <c r="B22" s="9"/>
       <c r="C22" s="1"/>
@@ -1129,9 +1157,8 @@
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
       <c r="P22" s="7"/>
-      <c r="Q22" s="1"/>
-    </row>
-    <row r="23" spans="1:17">
+    </row>
+    <row r="23" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A23" s="10"/>
       <c r="B23" s="9"/>
       <c r="C23" s="1"/>
@@ -1148,9 +1175,8 @@
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
-      <c r="Q23" s="1"/>
-    </row>
-    <row r="24" spans="1:17">
+    </row>
+    <row r="24" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A24" s="10"/>
       <c r="B24" s="9"/>
       <c r="C24" s="1"/>
@@ -1167,9 +1193,8 @@
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
       <c r="P24" s="7"/>
-      <c r="Q24" s="1"/>
-    </row>
-    <row r="25" spans="1:17">
+    </row>
+    <row r="25" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A25" s="10"/>
       <c r="B25" s="9"/>
       <c r="C25" s="1"/>
@@ -1186,9 +1211,8 @@
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
       <c r="P25" s="7"/>
-      <c r="Q25" s="1"/>
-    </row>
-    <row r="26" spans="1:17">
+    </row>
+    <row r="26" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
       <c r="B26" s="9"/>
       <c r="C26" s="1"/>
@@ -1205,9 +1229,8 @@
       <c r="N26" s="7"/>
       <c r="O26" s="7"/>
       <c r="P26" s="7"/>
-      <c r="Q26" s="1"/>
-    </row>
-    <row r="27" spans="1:17">
+    </row>
+    <row r="27" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
       <c r="B27" s="9"/>
       <c r="C27" s="1"/>
@@ -1224,9 +1247,8 @@
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
       <c r="P27" s="7"/>
-      <c r="Q27" s="1"/>
-    </row>
-    <row r="28" spans="1:17">
+    </row>
+    <row r="28" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A28" s="10"/>
       <c r="B28" s="9"/>
       <c r="C28" s="1"/>
@@ -1243,9 +1265,8 @@
       <c r="N28" s="7"/>
       <c r="O28" s="7"/>
       <c r="P28" s="7"/>
-      <c r="Q28" s="1"/>
-    </row>
-    <row r="29" spans="1:17">
+    </row>
+    <row r="29" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A29" s="10"/>
       <c r="B29" s="9"/>
       <c r="C29" s="1"/>
@@ -1262,9 +1283,8 @@
       <c r="N29" s="7"/>
       <c r="O29" s="7"/>
       <c r="P29" s="7"/>
-      <c r="Q29" s="1"/>
-    </row>
-    <row r="30" spans="1:17">
+    </row>
+    <row r="30" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A30" s="10"/>
       <c r="B30" s="9"/>
       <c r="C30" s="1"/>
@@ -1281,9 +1301,8 @@
       <c r="N30" s="7"/>
       <c r="O30" s="7"/>
       <c r="P30" s="7"/>
-      <c r="Q30" s="1"/>
-    </row>
-    <row r="31" spans="1:17">
+    </row>
+    <row r="31" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A31" s="10"/>
       <c r="B31" s="9"/>
       <c r="C31" s="1"/>
@@ -1300,9 +1319,8 @@
       <c r="N31" s="7"/>
       <c r="O31" s="7"/>
       <c r="P31" s="7"/>
-      <c r="Q31" s="1"/>
-    </row>
-    <row r="32" spans="1:17">
+    </row>
+    <row r="32" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A32" s="10"/>
       <c r="B32" s="9"/>
       <c r="C32" s="1"/>
@@ -1319,9 +1337,8 @@
       <c r="N32" s="7"/>
       <c r="O32" s="7"/>
       <c r="P32" s="7"/>
-      <c r="Q32" s="1"/>
-    </row>
-    <row r="33" spans="1:17">
+    </row>
+    <row r="33" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A33" s="10"/>
       <c r="B33" s="9"/>
       <c r="C33" s="1"/>
@@ -1338,9 +1355,8 @@
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
       <c r="P33" s="7"/>
-      <c r="Q33" s="1"/>
-    </row>
-    <row r="34" spans="1:17">
+    </row>
+    <row r="34" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A34" s="10"/>
       <c r="B34" s="9"/>
       <c r="C34" s="1"/>
@@ -1357,9 +1373,8 @@
       <c r="N34" s="7"/>
       <c r="O34" s="7"/>
       <c r="P34" s="7"/>
-      <c r="Q34" s="1"/>
-    </row>
-    <row r="35" spans="1:17">
+    </row>
+    <row r="35" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A35" s="10"/>
       <c r="B35" s="9"/>
       <c r="C35" s="1"/>
@@ -1376,9 +1391,8 @@
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
       <c r="P35" s="7"/>
-      <c r="Q35" s="1"/>
-    </row>
-    <row r="36" spans="1:17">
+    </row>
+    <row r="36" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A36" s="10"/>
       <c r="B36" s="9"/>
       <c r="C36" s="1"/>
@@ -1395,9 +1409,8 @@
       <c r="N36" s="7"/>
       <c r="O36" s="7"/>
       <c r="P36" s="7"/>
-      <c r="Q36" s="1"/>
-    </row>
-    <row r="37" spans="1:17">
+    </row>
+    <row r="37" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A37" s="10"/>
       <c r="B37" s="9"/>
       <c r="C37" s="1"/>
@@ -1414,9 +1427,8 @@
       <c r="N37" s="7"/>
       <c r="O37" s="7"/>
       <c r="P37" s="7"/>
-      <c r="Q37" s="1"/>
-    </row>
-    <row r="38" spans="1:17">
+    </row>
+    <row r="38" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A38" s="10"/>
       <c r="B38" s="9"/>
       <c r="C38" s="1"/>
@@ -1433,9 +1445,8 @@
       <c r="N38" s="7"/>
       <c r="O38" s="7"/>
       <c r="P38" s="7"/>
-      <c r="Q38" s="1"/>
-    </row>
-    <row r="39" spans="1:17">
+    </row>
+    <row r="39" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A39" s="10"/>
       <c r="B39" s="9"/>
       <c r="C39" s="1"/>
@@ -1452,9 +1463,8 @@
       <c r="N39" s="7"/>
       <c r="O39" s="7"/>
       <c r="P39" s="7"/>
-      <c r="Q39" s="1"/>
-    </row>
-    <row r="40" spans="1:17">
+    </row>
+    <row r="40" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A40" s="10"/>
       <c r="B40" s="9"/>
       <c r="C40" s="1"/>
@@ -1471,9 +1481,8 @@
       <c r="N40" s="7"/>
       <c r="O40" s="7"/>
       <c r="P40" s="7"/>
-      <c r="Q40" s="1"/>
-    </row>
-    <row r="41" spans="1:17">
+    </row>
+    <row r="41" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A41" s="10"/>
       <c r="B41" s="9"/>
       <c r="C41" s="1"/>
@@ -1490,9 +1499,8 @@
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
       <c r="P41" s="7"/>
-      <c r="Q41" s="1"/>
-    </row>
-    <row r="42" spans="1:17">
+    </row>
+    <row r="42" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A42" s="10"/>
       <c r="B42" s="9"/>
       <c r="C42" s="1"/>
@@ -1509,9 +1517,8 @@
       <c r="N42" s="7"/>
       <c r="O42" s="7"/>
       <c r="P42" s="7"/>
-      <c r="Q42" s="1"/>
-    </row>
-    <row r="43" spans="1:17">
+    </row>
+    <row r="43" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A43" s="10"/>
       <c r="B43" s="9"/>
       <c r="C43" s="1"/>
@@ -1528,9 +1535,8 @@
       <c r="N43" s="7"/>
       <c r="O43" s="7"/>
       <c r="P43" s="7"/>
-      <c r="Q43" s="1"/>
-    </row>
-    <row r="44" spans="1:17">
+    </row>
+    <row r="44" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A44" s="10"/>
       <c r="B44" s="9"/>
       <c r="C44" s="1"/>
@@ -1547,9 +1553,8 @@
       <c r="N44" s="7"/>
       <c r="O44" s="7"/>
       <c r="P44" s="7"/>
-      <c r="Q44" s="1"/>
-    </row>
-    <row r="45" spans="1:17">
+    </row>
+    <row r="45" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A45" s="10"/>
       <c r="B45" s="9"/>
       <c r="C45" s="1"/>
@@ -1566,9 +1571,8 @@
       <c r="N45" s="7"/>
       <c r="O45" s="7"/>
       <c r="P45" s="7"/>
-      <c r="Q45" s="1"/>
-    </row>
-    <row r="46" spans="1:17">
+    </row>
+    <row r="46" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A46" s="10"/>
       <c r="B46" s="9"/>
       <c r="C46" s="1"/>
@@ -1585,9 +1589,8 @@
       <c r="N46" s="7"/>
       <c r="O46" s="7"/>
       <c r="P46" s="7"/>
-      <c r="Q46" s="1"/>
-    </row>
-    <row r="47" spans="1:17">
+    </row>
+    <row r="47" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A47" s="10"/>
       <c r="B47" s="9"/>
       <c r="C47" s="1"/>
@@ -1604,9 +1607,8 @@
       <c r="N47" s="7"/>
       <c r="O47" s="7"/>
       <c r="P47" s="7"/>
-      <c r="Q47" s="1"/>
-    </row>
-    <row r="48" spans="1:17">
+    </row>
+    <row r="48" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A48" s="10"/>
       <c r="B48" s="9"/>
       <c r="C48" s="1"/>
@@ -1623,9 +1625,8 @@
       <c r="N48" s="7"/>
       <c r="O48" s="7"/>
       <c r="P48" s="7"/>
-      <c r="Q48" s="1"/>
-    </row>
-    <row r="49" spans="1:17">
+    </row>
+    <row r="49" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A49" s="10"/>
       <c r="B49" s="9"/>
       <c r="C49" s="1"/>
@@ -1642,9 +1643,8 @@
       <c r="N49" s="7"/>
       <c r="O49" s="7"/>
       <c r="P49" s="7"/>
-      <c r="Q49" s="1"/>
-    </row>
-    <row r="50" spans="1:17">
+    </row>
+    <row r="50" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A50" s="10"/>
       <c r="B50" s="9"/>
       <c r="C50" s="1"/>
@@ -1661,9 +1661,8 @@
       <c r="N50" s="7"/>
       <c r="O50" s="7"/>
       <c r="P50" s="7"/>
-      <c r="Q50" s="1"/>
-    </row>
-    <row r="51" spans="1:17">
+    </row>
+    <row r="51" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A51" s="10"/>
       <c r="B51" s="9"/>
       <c r="C51" s="1"/>
@@ -1680,9 +1679,8 @@
       <c r="N51" s="7"/>
       <c r="O51" s="7"/>
       <c r="P51" s="7"/>
-      <c r="Q51" s="1"/>
-    </row>
-    <row r="52" spans="1:17">
+    </row>
+    <row r="52" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A52" s="10"/>
       <c r="B52" s="9"/>
       <c r="C52" s="1"/>
@@ -1699,9 +1697,8 @@
       <c r="N52" s="7"/>
       <c r="O52" s="7"/>
       <c r="P52" s="7"/>
-      <c r="Q52" s="1"/>
-    </row>
-    <row r="53" spans="1:17">
+    </row>
+    <row r="53" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A53" s="10"/>
       <c r="B53" s="9"/>
       <c r="C53" s="1"/>
@@ -1718,9 +1715,8 @@
       <c r="N53" s="7"/>
       <c r="O53" s="7"/>
       <c r="P53" s="7"/>
-      <c r="Q53" s="1"/>
-    </row>
-    <row r="54" spans="1:17">
+    </row>
+    <row r="54" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A54" s="10"/>
       <c r="B54" s="9"/>
       <c r="C54" s="1"/>
@@ -1737,9 +1733,8 @@
       <c r="N54" s="7"/>
       <c r="O54" s="7"/>
       <c r="P54" s="7"/>
-      <c r="Q54" s="1"/>
-    </row>
-    <row r="55" spans="1:17">
+    </row>
+    <row r="55" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A55" s="10"/>
       <c r="B55" s="9"/>
       <c r="C55" s="1"/>
@@ -1756,9 +1751,8 @@
       <c r="N55" s="7"/>
       <c r="O55" s="7"/>
       <c r="P55" s="7"/>
-      <c r="Q55" s="1"/>
-    </row>
-    <row r="56" spans="1:17">
+    </row>
+    <row r="56" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A56" s="10"/>
       <c r="B56" s="9"/>
       <c r="C56" s="1"/>
@@ -1775,9 +1769,8 @@
       <c r="N56" s="7"/>
       <c r="O56" s="7"/>
       <c r="P56" s="7"/>
-      <c r="Q56" s="1"/>
-    </row>
-    <row r="57" spans="1:17">
+    </row>
+    <row r="57" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A57" s="10"/>
       <c r="B57" s="9"/>
       <c r="C57" s="1"/>
@@ -1794,9 +1787,8 @@
       <c r="N57" s="7"/>
       <c r="O57" s="7"/>
       <c r="P57" s="7"/>
-      <c r="Q57" s="1"/>
-    </row>
-    <row r="58" spans="1:17">
+    </row>
+    <row r="58" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A58" s="10"/>
       <c r="B58" s="9"/>
       <c r="C58" s="1"/>
@@ -1813,9 +1805,8 @@
       <c r="N58" s="7"/>
       <c r="O58" s="7"/>
       <c r="P58" s="7"/>
-      <c r="Q58" s="1"/>
-    </row>
-    <row r="59" spans="1:17">
+    </row>
+    <row r="59" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A59" s="10"/>
       <c r="B59" s="9"/>
       <c r="C59" s="1"/>
@@ -1832,9 +1823,8 @@
       <c r="N59" s="7"/>
       <c r="O59" s="7"/>
       <c r="P59" s="7"/>
-      <c r="Q59" s="1"/>
-    </row>
-    <row r="60" spans="1:17">
+    </row>
+    <row r="60" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A60" s="10"/>
       <c r="B60" s="9"/>
       <c r="C60" s="1"/>
@@ -1851,9 +1841,8 @@
       <c r="N60" s="7"/>
       <c r="O60" s="7"/>
       <c r="P60" s="7"/>
-      <c r="Q60" s="1"/>
-    </row>
-    <row r="61" spans="1:17">
+    </row>
+    <row r="61" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A61" s="10"/>
       <c r="B61" s="9"/>
       <c r="C61" s="1"/>
@@ -1870,9 +1859,8 @@
       <c r="N61" s="7"/>
       <c r="O61" s="7"/>
       <c r="P61" s="7"/>
-      <c r="Q61" s="1"/>
-    </row>
-    <row r="62" spans="1:17">
+    </row>
+    <row r="62" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A62" s="10"/>
       <c r="B62" s="9"/>
       <c r="C62" s="1"/>
@@ -1889,9 +1877,8 @@
       <c r="N62" s="7"/>
       <c r="O62" s="7"/>
       <c r="P62" s="7"/>
-      <c r="Q62" s="1"/>
-    </row>
-    <row r="63" spans="1:17">
+    </row>
+    <row r="63" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A63" s="10"/>
       <c r="B63" s="9"/>
       <c r="C63" s="1"/>
@@ -1908,9 +1895,8 @@
       <c r="N63" s="7"/>
       <c r="O63" s="7"/>
       <c r="P63" s="7"/>
-      <c r="Q63" s="1"/>
-    </row>
-    <row r="64" spans="1:17">
+    </row>
+    <row r="64" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A64" s="10"/>
       <c r="B64" s="9"/>
       <c r="C64" s="1"/>
@@ -1927,9 +1913,8 @@
       <c r="N64" s="7"/>
       <c r="O64" s="7"/>
       <c r="P64" s="7"/>
-      <c r="Q64" s="1"/>
-    </row>
-    <row r="65" spans="1:17">
+    </row>
+    <row r="65" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A65" s="10"/>
       <c r="B65" s="9"/>
       <c r="C65" s="1"/>
@@ -1946,9 +1931,8 @@
       <c r="N65" s="7"/>
       <c r="O65" s="7"/>
       <c r="P65" s="7"/>
-      <c r="Q65" s="1"/>
-    </row>
-    <row r="66" spans="1:17">
+    </row>
+    <row r="66" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A66" s="10"/>
       <c r="B66" s="9"/>
       <c r="C66" s="1"/>
@@ -1965,9 +1949,8 @@
       <c r="N66" s="7"/>
       <c r="O66" s="7"/>
       <c r="P66" s="7"/>
-      <c r="Q66" s="1"/>
-    </row>
-    <row r="67" spans="1:17">
+    </row>
+    <row r="67" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A67" s="10"/>
       <c r="B67" s="9"/>
       <c r="C67" s="1"/>
@@ -1984,9 +1967,8 @@
       <c r="N67" s="7"/>
       <c r="O67" s="7"/>
       <c r="P67" s="7"/>
-      <c r="Q67" s="1"/>
-    </row>
-    <row r="68" spans="1:17">
+    </row>
+    <row r="68" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A68" s="10"/>
       <c r="B68" s="9"/>
       <c r="C68" s="1"/>
@@ -2003,9 +1985,8 @@
       <c r="N68" s="7"/>
       <c r="O68" s="7"/>
       <c r="P68" s="7"/>
-      <c r="Q68" s="1"/>
-    </row>
-    <row r="69" spans="1:17">
+    </row>
+    <row r="69" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A69" s="10"/>
       <c r="B69" s="9"/>
       <c r="C69" s="1"/>
@@ -2022,9 +2003,8 @@
       <c r="N69" s="7"/>
       <c r="O69" s="7"/>
       <c r="P69" s="7"/>
-      <c r="Q69" s="1"/>
-    </row>
-    <row r="70" spans="1:17">
+    </row>
+    <row r="70" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A70" s="10"/>
       <c r="B70" s="9"/>
       <c r="C70" s="1"/>
@@ -2041,9 +2021,8 @@
       <c r="N70" s="7"/>
       <c r="O70" s="7"/>
       <c r="P70" s="7"/>
-      <c r="Q70" s="1"/>
-    </row>
-    <row r="71" spans="1:17">
+    </row>
+    <row r="71" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A71" s="10"/>
       <c r="B71" s="9"/>
       <c r="C71" s="1"/>
@@ -2060,9 +2039,8 @@
       <c r="N71" s="7"/>
       <c r="O71" s="7"/>
       <c r="P71" s="7"/>
-      <c r="Q71" s="1"/>
-    </row>
-    <row r="72" spans="1:17">
+    </row>
+    <row r="72" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A72" s="10"/>
       <c r="B72" s="9"/>
       <c r="C72" s="1"/>
@@ -2079,9 +2057,8 @@
       <c r="N72" s="7"/>
       <c r="O72" s="7"/>
       <c r="P72" s="7"/>
-      <c r="Q72" s="1"/>
-    </row>
-    <row r="73" spans="1:17">
+    </row>
+    <row r="73" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A73" s="10"/>
       <c r="B73" s="9"/>
       <c r="C73" s="1"/>
@@ -2098,9 +2075,8 @@
       <c r="N73" s="7"/>
       <c r="O73" s="7"/>
       <c r="P73" s="7"/>
-      <c r="Q73" s="1"/>
-    </row>
-    <row r="74" spans="1:17">
+    </row>
+    <row r="74" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A74" s="10"/>
       <c r="B74" s="9"/>
       <c r="C74" s="1"/>
@@ -2117,9 +2093,8 @@
       <c r="N74" s="7"/>
       <c r="O74" s="7"/>
       <c r="P74" s="7"/>
-      <c r="Q74" s="1"/>
-    </row>
-    <row r="75" spans="1:17">
+    </row>
+    <row r="75" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A75" s="10"/>
       <c r="B75" s="9"/>
       <c r="C75" s="1"/>
@@ -2136,9 +2111,8 @@
       <c r="N75" s="7"/>
       <c r="O75" s="7"/>
       <c r="P75" s="7"/>
-      <c r="Q75" s="1"/>
-    </row>
-    <row r="76" spans="1:17">
+    </row>
+    <row r="76" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A76" s="10"/>
       <c r="B76" s="9"/>
       <c r="C76" s="1"/>
@@ -2155,9 +2129,8 @@
       <c r="N76" s="7"/>
       <c r="O76" s="7"/>
       <c r="P76" s="7"/>
-      <c r="Q76" s="1"/>
-    </row>
-    <row r="77" spans="1:17">
+    </row>
+    <row r="77" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A77" s="10"/>
       <c r="B77" s="9"/>
       <c r="C77" s="1"/>
@@ -2174,9 +2147,8 @@
       <c r="N77" s="7"/>
       <c r="O77" s="7"/>
       <c r="P77" s="7"/>
-      <c r="Q77" s="1"/>
-    </row>
-    <row r="78" spans="1:17">
+    </row>
+    <row r="78" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A78" s="10"/>
       <c r="B78" s="9"/>
       <c r="C78" s="1"/>
@@ -2193,9 +2165,8 @@
       <c r="N78" s="7"/>
       <c r="O78" s="7"/>
       <c r="P78" s="7"/>
-      <c r="Q78" s="1"/>
-    </row>
-    <row r="79" spans="1:17">
+    </row>
+    <row r="79" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A79" s="10"/>
       <c r="B79" s="9"/>
       <c r="C79" s="1"/>
@@ -2212,9 +2183,8 @@
       <c r="N79" s="7"/>
       <c r="O79" s="7"/>
       <c r="P79" s="7"/>
-      <c r="Q79" s="1"/>
-    </row>
-    <row r="80" spans="1:17">
+    </row>
+    <row r="80" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A80" s="10"/>
       <c r="B80" s="9"/>
       <c r="C80" s="1"/>
@@ -2231,9 +2201,8 @@
       <c r="N80" s="7"/>
       <c r="O80" s="7"/>
       <c r="P80" s="7"/>
-      <c r="Q80" s="1"/>
-    </row>
-    <row r="81" spans="1:17">
+    </row>
+    <row r="81" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A81" s="10"/>
       <c r="B81" s="9"/>
       <c r="C81" s="1"/>
@@ -2250,9 +2219,8 @@
       <c r="N81" s="7"/>
       <c r="O81" s="7"/>
       <c r="P81" s="7"/>
-      <c r="Q81" s="1"/>
-    </row>
-    <row r="82" spans="1:17">
+    </row>
+    <row r="82" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A82" s="10"/>
       <c r="B82" s="9"/>
       <c r="C82" s="1"/>
@@ -2269,9 +2237,8 @@
       <c r="N82" s="7"/>
       <c r="O82" s="7"/>
       <c r="P82" s="7"/>
-      <c r="Q82" s="1"/>
-    </row>
-    <row r="83" spans="1:17">
+    </row>
+    <row r="83" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A83" s="10"/>
       <c r="B83" s="9"/>
       <c r="C83" s="1"/>
@@ -2288,9 +2255,8 @@
       <c r="N83" s="7"/>
       <c r="O83" s="7"/>
       <c r="P83" s="7"/>
-      <c r="Q83" s="1"/>
-    </row>
-    <row r="84" spans="1:17">
+    </row>
+    <row r="84" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A84" s="10"/>
       <c r="B84" s="9"/>
       <c r="C84" s="1"/>
@@ -2307,9 +2273,8 @@
       <c r="N84" s="7"/>
       <c r="O84" s="7"/>
       <c r="P84" s="7"/>
-      <c r="Q84" s="1"/>
-    </row>
-    <row r="85" spans="1:17">
+    </row>
+    <row r="85" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A85" s="10"/>
       <c r="B85" s="9"/>
       <c r="C85" s="1"/>
@@ -2326,9 +2291,8 @@
       <c r="N85" s="7"/>
       <c r="O85" s="7"/>
       <c r="P85" s="7"/>
-      <c r="Q85" s="1"/>
-    </row>
-    <row r="86" spans="1:17">
+    </row>
+    <row r="86" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A86" s="10"/>
       <c r="B86" s="9"/>
       <c r="C86" s="1"/>
@@ -2345,9 +2309,8 @@
       <c r="N86" s="7"/>
       <c r="O86" s="7"/>
       <c r="P86" s="7"/>
-      <c r="Q86" s="1"/>
-    </row>
-    <row r="87" spans="1:17">
+    </row>
+    <row r="87" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A87" s="10"/>
       <c r="B87" s="9"/>
       <c r="C87" s="1"/>
@@ -2364,9 +2327,8 @@
       <c r="N87" s="7"/>
       <c r="O87" s="7"/>
       <c r="P87" s="7"/>
-      <c r="Q87" s="1"/>
-    </row>
-    <row r="88" spans="1:17">
+    </row>
+    <row r="88" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A88" s="10"/>
       <c r="B88" s="9"/>
       <c r="C88" s="1"/>
@@ -2383,9 +2345,8 @@
       <c r="N88" s="7"/>
       <c r="O88" s="7"/>
       <c r="P88" s="7"/>
-      <c r="Q88" s="1"/>
-    </row>
-    <row r="89" spans="1:17">
+    </row>
+    <row r="89" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A89" s="10"/>
       <c r="B89" s="9"/>
       <c r="C89" s="1"/>
@@ -2402,9 +2363,8 @@
       <c r="N89" s="7"/>
       <c r="O89" s="7"/>
       <c r="P89" s="7"/>
-      <c r="Q89" s="1"/>
-    </row>
-    <row r="90" spans="1:17">
+    </row>
+    <row r="90" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A90" s="10"/>
       <c r="B90" s="9"/>
       <c r="C90" s="1"/>
@@ -2421,9 +2381,8 @@
       <c r="N90" s="7"/>
       <c r="O90" s="7"/>
       <c r="P90" s="7"/>
-      <c r="Q90" s="1"/>
-    </row>
-    <row r="91" spans="1:17">
+    </row>
+    <row r="91" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A91" s="10"/>
       <c r="B91" s="9"/>
       <c r="C91" s="1"/>
@@ -2440,9 +2399,8 @@
       <c r="N91" s="7"/>
       <c r="O91" s="7"/>
       <c r="P91" s="7"/>
-      <c r="Q91" s="1"/>
-    </row>
-    <row r="92" spans="1:17">
+    </row>
+    <row r="92" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A92" s="10"/>
       <c r="B92" s="9"/>
       <c r="C92" s="1"/>
@@ -2459,9 +2417,8 @@
       <c r="N92" s="7"/>
       <c r="O92" s="7"/>
       <c r="P92" s="7"/>
-      <c r="Q92" s="1"/>
-    </row>
-    <row r="93" spans="1:17">
+    </row>
+    <row r="93" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A93" s="10"/>
       <c r="B93" s="9"/>
       <c r="C93" s="1"/>
@@ -2478,9 +2435,8 @@
       <c r="N93" s="7"/>
       <c r="O93" s="7"/>
       <c r="P93" s="7"/>
-      <c r="Q93" s="1"/>
-    </row>
-    <row r="94" spans="1:17">
+    </row>
+    <row r="94" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A94" s="10"/>
       <c r="B94" s="9"/>
       <c r="C94" s="1"/>
@@ -2497,9 +2453,8 @@
       <c r="N94" s="7"/>
       <c r="O94" s="7"/>
       <c r="P94" s="7"/>
-      <c r="Q94" s="1"/>
-    </row>
-    <row r="95" spans="1:17">
+    </row>
+    <row r="95" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A95" s="10"/>
       <c r="B95" s="9"/>
       <c r="C95" s="1"/>
@@ -2516,9 +2471,8 @@
       <c r="N95" s="7"/>
       <c r="O95" s="7"/>
       <c r="P95" s="7"/>
-      <c r="Q95" s="1"/>
-    </row>
-    <row r="96" spans="1:17">
+    </row>
+    <row r="96" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A96" s="10"/>
       <c r="B96" s="9"/>
       <c r="C96" s="1"/>
@@ -2535,9 +2489,8 @@
       <c r="N96" s="7"/>
       <c r="O96" s="7"/>
       <c r="P96" s="7"/>
-      <c r="Q96" s="1"/>
-    </row>
-    <row r="97" spans="1:17">
+    </row>
+    <row r="97" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A97" s="10"/>
       <c r="B97" s="9"/>
       <c r="C97" s="1"/>
@@ -2554,9 +2507,8 @@
       <c r="N97" s="7"/>
       <c r="O97" s="7"/>
       <c r="P97" s="7"/>
-      <c r="Q97" s="1"/>
-    </row>
-    <row r="98" spans="1:17">
+    </row>
+    <row r="98" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A98" s="10"/>
       <c r="B98" s="9"/>
       <c r="C98" s="1"/>
@@ -2573,9 +2525,8 @@
       <c r="N98" s="7"/>
       <c r="O98" s="7"/>
       <c r="P98" s="7"/>
-      <c r="Q98" s="1"/>
-    </row>
-    <row r="99" spans="1:17">
+    </row>
+    <row r="99" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A99" s="10"/>
       <c r="B99" s="9"/>
       <c r="C99" s="1"/>
@@ -2592,9 +2543,8 @@
       <c r="N99" s="7"/>
       <c r="O99" s="7"/>
       <c r="P99" s="7"/>
-      <c r="Q99" s="1"/>
-    </row>
-    <row r="100" spans="1:17">
+    </row>
+    <row r="100" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A100" s="10"/>
       <c r="B100" s="9"/>
       <c r="C100" s="1"/>
@@ -2611,9 +2561,8 @@
       <c r="N100" s="7"/>
       <c r="O100" s="7"/>
       <c r="P100" s="7"/>
-      <c r="Q100" s="1"/>
-    </row>
-    <row r="101" spans="1:17">
+    </row>
+    <row r="101" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A101" s="10"/>
       <c r="B101" s="9"/>
       <c r="C101" s="1"/>
@@ -2630,9 +2579,8 @@
       <c r="N101" s="7"/>
       <c r="O101" s="7"/>
       <c r="P101" s="7"/>
-      <c r="Q101" s="1"/>
-    </row>
-    <row r="102" spans="1:17">
+    </row>
+    <row r="102" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A102" s="10"/>
       <c r="B102" s="9"/>
       <c r="C102" s="1"/>
@@ -2649,9 +2597,8 @@
       <c r="N102" s="7"/>
       <c r="O102" s="7"/>
       <c r="P102" s="7"/>
-      <c r="Q102" s="1"/>
-    </row>
-    <row r="103" spans="1:17">
+    </row>
+    <row r="103" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A103" s="10"/>
       <c r="B103" s="9"/>
       <c r="C103" s="1"/>
@@ -2668,9 +2615,8 @@
       <c r="N103" s="7"/>
       <c r="O103" s="7"/>
       <c r="P103" s="7"/>
-      <c r="Q103" s="1"/>
-    </row>
-    <row r="104" spans="1:17">
+    </row>
+    <row r="104" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A104" s="10"/>
       <c r="B104" s="9"/>
       <c r="C104" s="1"/>
@@ -2687,9 +2633,8 @@
       <c r="N104" s="7"/>
       <c r="O104" s="7"/>
       <c r="P104" s="7"/>
-      <c r="Q104" s="1"/>
-    </row>
-    <row r="105" spans="1:17">
+    </row>
+    <row r="105" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A105" s="10"/>
       <c r="B105" s="9"/>
       <c r="C105" s="1"/>
@@ -2706,9 +2651,8 @@
       <c r="N105" s="7"/>
       <c r="O105" s="7"/>
       <c r="P105" s="7"/>
-      <c r="Q105" s="1"/>
-    </row>
-    <row r="106" spans="1:17">
+    </row>
+    <row r="106" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A106" s="10"/>
       <c r="B106" s="9"/>
       <c r="C106" s="1"/>
@@ -2725,9 +2669,8 @@
       <c r="N106" s="7"/>
       <c r="O106" s="7"/>
       <c r="P106" s="7"/>
-      <c r="Q106" s="1"/>
-    </row>
-    <row r="107" spans="1:17">
+    </row>
+    <row r="107" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A107" s="10"/>
       <c r="B107" s="9"/>
       <c r="C107" s="1"/>
@@ -2744,9 +2687,8 @@
       <c r="N107" s="7"/>
       <c r="O107" s="7"/>
       <c r="P107" s="7"/>
-      <c r="Q107" s="1"/>
-    </row>
-    <row r="108" spans="1:17">
+    </row>
+    <row r="108" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A108" s="10"/>
       <c r="B108" s="9"/>
       <c r="C108" s="1"/>
@@ -2763,9 +2705,8 @@
       <c r="N108" s="7"/>
       <c r="O108" s="7"/>
       <c r="P108" s="7"/>
-      <c r="Q108" s="1"/>
-    </row>
-    <row r="109" spans="1:17">
+    </row>
+    <row r="109" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A109" s="10"/>
       <c r="B109" s="9"/>
       <c r="C109" s="1"/>
@@ -2782,9 +2723,8 @@
       <c r="N109" s="7"/>
       <c r="O109" s="7"/>
       <c r="P109" s="7"/>
-      <c r="Q109" s="1"/>
-    </row>
-    <row r="110" spans="1:17">
+    </row>
+    <row r="110" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A110" s="10"/>
       <c r="B110" s="9"/>
       <c r="C110" s="1"/>
@@ -2801,9 +2741,8 @@
       <c r="N110" s="7"/>
       <c r="O110" s="7"/>
       <c r="P110" s="7"/>
-      <c r="Q110" s="1"/>
-    </row>
-    <row r="111" spans="1:17">
+    </row>
+    <row r="111" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A111" s="10"/>
       <c r="B111" s="9"/>
       <c r="C111" s="1"/>
@@ -2820,9 +2759,8 @@
       <c r="N111" s="7"/>
       <c r="O111" s="7"/>
       <c r="P111" s="7"/>
-      <c r="Q111" s="1"/>
-    </row>
-    <row r="112" spans="1:17">
+    </row>
+    <row r="112" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A112" s="10"/>
       <c r="B112" s="9"/>
       <c r="C112" s="1"/>
@@ -2839,9 +2777,8 @@
       <c r="N112" s="7"/>
       <c r="O112" s="7"/>
       <c r="P112" s="7"/>
-      <c r="Q112" s="1"/>
-    </row>
-    <row r="113" spans="1:17">
+    </row>
+    <row r="113" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A113" s="10"/>
       <c r="B113" s="9"/>
       <c r="C113" s="1"/>
@@ -2858,9 +2795,8 @@
       <c r="N113" s="7"/>
       <c r="O113" s="7"/>
       <c r="P113" s="7"/>
-      <c r="Q113" s="1"/>
-    </row>
-    <row r="114" spans="1:17">
+    </row>
+    <row r="114" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A114" s="10"/>
       <c r="B114" s="9"/>
       <c r="C114" s="1"/>
@@ -2877,9 +2813,8 @@
       <c r="N114" s="7"/>
       <c r="O114" s="7"/>
       <c r="P114" s="7"/>
-      <c r="Q114" s="1"/>
-    </row>
-    <row r="115" spans="1:17">
+    </row>
+    <row r="115" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A115" s="10"/>
       <c r="B115" s="9"/>
       <c r="C115" s="1"/>
@@ -2896,9 +2831,8 @@
       <c r="N115" s="7"/>
       <c r="O115" s="7"/>
       <c r="P115" s="7"/>
-      <c r="Q115" s="1"/>
-    </row>
-    <row r="116" spans="1:17">
+    </row>
+    <row r="116" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A116" s="10"/>
       <c r="B116" s="9"/>
       <c r="C116" s="1"/>
@@ -2915,9 +2849,8 @@
       <c r="N116" s="7"/>
       <c r="O116" s="7"/>
       <c r="P116" s="7"/>
-      <c r="Q116" s="1"/>
-    </row>
-    <row r="117" spans="1:17">
+    </row>
+    <row r="117" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A117" s="10"/>
       <c r="B117" s="9"/>
       <c r="C117" s="1"/>
@@ -2934,9 +2867,8 @@
       <c r="N117" s="7"/>
       <c r="O117" s="7"/>
       <c r="P117" s="7"/>
-      <c r="Q117" s="1"/>
-    </row>
-    <row r="118" spans="1:17">
+    </row>
+    <row r="118" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A118" s="10"/>
       <c r="B118" s="9"/>
       <c r="C118" s="1"/>
@@ -2953,9 +2885,8 @@
       <c r="N118" s="7"/>
       <c r="O118" s="7"/>
       <c r="P118" s="7"/>
-      <c r="Q118" s="1"/>
-    </row>
-    <row r="119" spans="1:17">
+    </row>
+    <row r="119" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A119" s="10"/>
       <c r="B119" s="9"/>
       <c r="C119" s="1"/>
@@ -2972,9 +2903,8 @@
       <c r="N119" s="7"/>
       <c r="O119" s="7"/>
       <c r="P119" s="7"/>
-      <c r="Q119" s="1"/>
-    </row>
-    <row r="120" spans="1:17">
+    </row>
+    <row r="120" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A120" s="10"/>
       <c r="B120" s="9"/>
       <c r="C120" s="1"/>
@@ -2991,9 +2921,8 @@
       <c r="N120" s="7"/>
       <c r="O120" s="7"/>
       <c r="P120" s="7"/>
-      <c r="Q120" s="1"/>
-    </row>
-    <row r="121" spans="1:17">
+    </row>
+    <row r="121" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A121" s="10"/>
       <c r="B121" s="9"/>
       <c r="C121" s="1"/>
@@ -3010,9 +2939,8 @@
       <c r="N121" s="7"/>
       <c r="O121" s="7"/>
       <c r="P121" s="7"/>
-      <c r="Q121" s="1"/>
-    </row>
-    <row r="122" spans="1:17">
+    </row>
+    <row r="122" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A122" s="10"/>
       <c r="B122" s="9"/>
       <c r="C122" s="1"/>
@@ -3029,9 +2957,8 @@
       <c r="N122" s="7"/>
       <c r="O122" s="7"/>
       <c r="P122" s="7"/>
-      <c r="Q122" s="1"/>
-    </row>
-    <row r="123" spans="1:17">
+    </row>
+    <row r="123" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A123" s="10"/>
       <c r="B123" s="9"/>
       <c r="C123" s="1"/>
@@ -3048,9 +2975,8 @@
       <c r="N123" s="7"/>
       <c r="O123" s="7"/>
       <c r="P123" s="7"/>
-      <c r="Q123" s="1"/>
-    </row>
-    <row r="124" spans="1:17">
+    </row>
+    <row r="124" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A124" s="10"/>
       <c r="B124" s="9"/>
       <c r="C124" s="1"/>
@@ -3067,9 +2993,8 @@
       <c r="N124" s="7"/>
       <c r="O124" s="7"/>
       <c r="P124" s="7"/>
-      <c r="Q124" s="1"/>
-    </row>
-    <row r="125" spans="1:17">
+    </row>
+    <row r="125" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A125" s="10"/>
       <c r="B125" s="9"/>
       <c r="C125" s="1"/>
@@ -3086,9 +3011,8 @@
       <c r="N125" s="7"/>
       <c r="O125" s="7"/>
       <c r="P125" s="7"/>
-      <c r="Q125" s="1"/>
-    </row>
-    <row r="126" spans="1:17">
+    </row>
+    <row r="126" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A126" s="10"/>
       <c r="B126" s="9"/>
       <c r="C126" s="1"/>
@@ -3105,9 +3029,8 @@
       <c r="N126" s="7"/>
       <c r="O126" s="7"/>
       <c r="P126" s="7"/>
-      <c r="Q126" s="1"/>
-    </row>
-    <row r="127" spans="1:17">
+    </row>
+    <row r="127" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A127" s="10"/>
       <c r="B127" s="9"/>
       <c r="C127" s="1"/>
@@ -3124,9 +3047,8 @@
       <c r="N127" s="7"/>
       <c r="O127" s="7"/>
       <c r="P127" s="7"/>
-      <c r="Q127" s="1"/>
-    </row>
-    <row r="128" spans="1:17">
+    </row>
+    <row r="128" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A128" s="10"/>
       <c r="B128" s="9"/>
       <c r="C128" s="1"/>
@@ -3143,9 +3065,8 @@
       <c r="N128" s="7"/>
       <c r="O128" s="7"/>
       <c r="P128" s="7"/>
-      <c r="Q128" s="1"/>
-    </row>
-    <row r="129" spans="1:17">
+    </row>
+    <row r="129" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A129" s="10"/>
       <c r="B129" s="9"/>
       <c r="C129" s="1"/>
@@ -3162,9 +3083,8 @@
       <c r="N129" s="7"/>
       <c r="O129" s="7"/>
       <c r="P129" s="7"/>
-      <c r="Q129" s="1"/>
-    </row>
-    <row r="130" spans="1:17">
+    </row>
+    <row r="130" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A130" s="10"/>
       <c r="B130" s="9"/>
       <c r="C130" s="1"/>
@@ -3181,9 +3101,8 @@
       <c r="N130" s="7"/>
       <c r="O130" s="7"/>
       <c r="P130" s="7"/>
-      <c r="Q130" s="1"/>
-    </row>
-    <row r="131" spans="1:17">
+    </row>
+    <row r="131" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A131" s="10"/>
       <c r="B131" s="9"/>
       <c r="C131" s="1"/>
@@ -3200,9 +3119,8 @@
       <c r="N131" s="7"/>
       <c r="O131" s="7"/>
       <c r="P131" s="7"/>
-      <c r="Q131" s="1"/>
-    </row>
-    <row r="132" spans="1:17">
+    </row>
+    <row r="132" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A132" s="10"/>
       <c r="B132" s="9"/>
       <c r="C132" s="1"/>
@@ -3219,9 +3137,8 @@
       <c r="N132" s="7"/>
       <c r="O132" s="7"/>
       <c r="P132" s="7"/>
-      <c r="Q132" s="1"/>
-    </row>
-    <row r="133" spans="1:17">
+    </row>
+    <row r="133" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A133" s="10"/>
       <c r="B133" s="9"/>
       <c r="C133" s="1"/>
@@ -3238,9 +3155,8 @@
       <c r="N133" s="7"/>
       <c r="O133" s="7"/>
       <c r="P133" s="7"/>
-      <c r="Q133" s="1"/>
-    </row>
-    <row r="134" spans="1:17">
+    </row>
+    <row r="134" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A134" s="10"/>
       <c r="B134" s="9"/>
       <c r="C134" s="1"/>
@@ -3257,9 +3173,8 @@
       <c r="N134" s="7"/>
       <c r="O134" s="7"/>
       <c r="P134" s="7"/>
-      <c r="Q134" s="1"/>
-    </row>
-    <row r="135" spans="1:17">
+    </row>
+    <row r="135" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A135" s="10"/>
       <c r="B135" s="9"/>
       <c r="C135" s="1"/>
@@ -3276,9 +3191,8 @@
       <c r="N135" s="7"/>
       <c r="O135" s="7"/>
       <c r="P135" s="7"/>
-      <c r="Q135" s="1"/>
-    </row>
-    <row r="136" spans="1:17">
+    </row>
+    <row r="136" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A136" s="10"/>
       <c r="B136" s="9"/>
       <c r="C136" s="1"/>
@@ -3295,9 +3209,8 @@
       <c r="N136" s="7"/>
       <c r="O136" s="7"/>
       <c r="P136" s="7"/>
-      <c r="Q136" s="1"/>
-    </row>
-    <row r="137" spans="1:17">
+    </row>
+    <row r="137" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A137" s="10"/>
       <c r="B137" s="9"/>
       <c r="C137" s="1"/>
@@ -3314,9 +3227,8 @@
       <c r="N137" s="7"/>
       <c r="O137" s="7"/>
       <c r="P137" s="7"/>
-      <c r="Q137" s="1"/>
-    </row>
-    <row r="138" spans="1:17">
+    </row>
+    <row r="138" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A138" s="10"/>
       <c r="B138" s="9"/>
       <c r="C138" s="1"/>
@@ -3333,9 +3245,8 @@
       <c r="N138" s="7"/>
       <c r="O138" s="7"/>
       <c r="P138" s="7"/>
-      <c r="Q138" s="1"/>
-    </row>
-    <row r="139" spans="1:17">
+    </row>
+    <row r="139" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A139" s="10"/>
       <c r="B139" s="9"/>
       <c r="C139" s="1"/>
@@ -3352,9 +3263,8 @@
       <c r="N139" s="7"/>
       <c r="O139" s="7"/>
       <c r="P139" s="7"/>
-      <c r="Q139" s="1"/>
-    </row>
-    <row r="140" spans="1:17">
+    </row>
+    <row r="140" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A140" s="10"/>
       <c r="B140" s="9"/>
       <c r="C140" s="1"/>
@@ -3371,9 +3281,8 @@
       <c r="N140" s="7"/>
       <c r="O140" s="7"/>
       <c r="P140" s="7"/>
-      <c r="Q140" s="1"/>
-    </row>
-    <row r="141" spans="1:17">
+    </row>
+    <row r="141" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A141" s="10"/>
       <c r="B141" s="9"/>
       <c r="C141" s="1"/>
@@ -3390,9 +3299,8 @@
       <c r="N141" s="7"/>
       <c r="O141" s="7"/>
       <c r="P141" s="7"/>
-      <c r="Q141" s="1"/>
-    </row>
-    <row r="142" spans="1:17">
+    </row>
+    <row r="142" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A142" s="10"/>
       <c r="B142" s="9"/>
       <c r="C142" s="1"/>
@@ -3409,9 +3317,8 @@
       <c r="N142" s="7"/>
       <c r="O142" s="7"/>
       <c r="P142" s="7"/>
-      <c r="Q142" s="1"/>
-    </row>
-    <row r="143" spans="1:17">
+    </row>
+    <row r="143" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A143" s="10"/>
       <c r="B143" s="9"/>
       <c r="C143" s="1"/>
@@ -3428,9 +3335,8 @@
       <c r="N143" s="7"/>
       <c r="O143" s="7"/>
       <c r="P143" s="7"/>
-      <c r="Q143" s="1"/>
-    </row>
-    <row r="144" spans="1:17">
+    </row>
+    <row r="144" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A144" s="10"/>
       <c r="B144" s="9"/>
       <c r="C144" s="1"/>
@@ -3447,9 +3353,8 @@
       <c r="N144" s="7"/>
       <c r="O144" s="7"/>
       <c r="P144" s="7"/>
-      <c r="Q144" s="1"/>
-    </row>
-    <row r="145" spans="1:17">
+    </row>
+    <row r="145" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A145" s="10"/>
       <c r="B145" s="9"/>
       <c r="C145" s="1"/>
@@ -3466,9 +3371,8 @@
       <c r="N145" s="7"/>
       <c r="O145" s="7"/>
       <c r="P145" s="7"/>
-      <c r="Q145" s="1"/>
-    </row>
-    <row r="146" spans="1:17">
+    </row>
+    <row r="146" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A146" s="10"/>
       <c r="B146" s="9"/>
       <c r="C146" s="1"/>
@@ -3485,9 +3389,8 @@
       <c r="N146" s="7"/>
       <c r="O146" s="7"/>
       <c r="P146" s="7"/>
-      <c r="Q146" s="1"/>
-    </row>
-    <row r="147" spans="1:17">
+    </row>
+    <row r="147" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A147" s="10"/>
       <c r="B147" s="9"/>
       <c r="C147" s="1"/>
@@ -3504,9 +3407,8 @@
       <c r="N147" s="7"/>
       <c r="O147" s="7"/>
       <c r="P147" s="7"/>
-      <c r="Q147" s="1"/>
-    </row>
-    <row r="148" spans="1:17">
+    </row>
+    <row r="148" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A148" s="10"/>
       <c r="B148" s="9"/>
       <c r="C148" s="1"/>
@@ -3523,9 +3425,8 @@
       <c r="N148" s="7"/>
       <c r="O148" s="7"/>
       <c r="P148" s="7"/>
-      <c r="Q148" s="1"/>
-    </row>
-    <row r="149" spans="1:17">
+    </row>
+    <row r="149" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A149" s="10"/>
       <c r="B149" s="9"/>
       <c r="C149" s="1"/>
@@ -3542,9 +3443,8 @@
       <c r="N149" s="7"/>
       <c r="O149" s="7"/>
       <c r="P149" s="7"/>
-      <c r="Q149" s="1"/>
-    </row>
-    <row r="150" spans="1:17">
+    </row>
+    <row r="150" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A150" s="10"/>
       <c r="B150" s="9"/>
       <c r="C150" s="1"/>
@@ -3561,9 +3461,8 @@
       <c r="N150" s="7"/>
       <c r="O150" s="7"/>
       <c r="P150" s="7"/>
-      <c r="Q150" s="1"/>
-    </row>
-    <row r="151" spans="1:17">
+    </row>
+    <row r="151" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A151" s="10"/>
       <c r="B151" s="9"/>
       <c r="C151" s="1"/>
@@ -3580,9 +3479,8 @@
       <c r="N151" s="7"/>
       <c r="O151" s="7"/>
       <c r="P151" s="7"/>
-      <c r="Q151" s="1"/>
-    </row>
-    <row r="152" spans="1:17">
+    </row>
+    <row r="152" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A152" s="10"/>
       <c r="B152" s="9"/>
       <c r="C152" s="1"/>
@@ -3599,9 +3497,8 @@
       <c r="N152" s="7"/>
       <c r="O152" s="7"/>
       <c r="P152" s="7"/>
-      <c r="Q152" s="1"/>
-    </row>
-    <row r="153" spans="1:17">
+    </row>
+    <row r="153" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A153" s="10"/>
       <c r="B153" s="9"/>
       <c r="C153" s="1"/>
@@ -3618,9 +3515,8 @@
       <c r="N153" s="7"/>
       <c r="O153" s="7"/>
       <c r="P153" s="7"/>
-      <c r="Q153" s="1"/>
-    </row>
-    <row r="154" spans="1:17">
+    </row>
+    <row r="154" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A154" s="10"/>
       <c r="B154" s="9"/>
       <c r="C154" s="1"/>
@@ -3637,9 +3533,8 @@
       <c r="N154" s="7"/>
       <c r="O154" s="7"/>
       <c r="P154" s="7"/>
-      <c r="Q154" s="1"/>
-    </row>
-    <row r="155" spans="1:17">
+    </row>
+    <row r="155" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A155" s="10"/>
       <c r="B155" s="9"/>
       <c r="C155" s="1"/>
@@ -3656,9 +3551,8 @@
       <c r="N155" s="7"/>
       <c r="O155" s="7"/>
       <c r="P155" s="7"/>
-      <c r="Q155" s="1"/>
-    </row>
-    <row r="156" spans="1:17">
+    </row>
+    <row r="156" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A156" s="10"/>
       <c r="B156" s="9"/>
       <c r="C156" s="1"/>
@@ -3675,9 +3569,8 @@
       <c r="N156" s="7"/>
       <c r="O156" s="7"/>
       <c r="P156" s="7"/>
-      <c r="Q156" s="1"/>
-    </row>
-    <row r="157" spans="1:17">
+    </row>
+    <row r="157" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A157" s="10"/>
       <c r="B157" s="9"/>
       <c r="C157" s="1"/>
@@ -3694,9 +3587,8 @@
       <c r="N157" s="7"/>
       <c r="O157" s="7"/>
       <c r="P157" s="7"/>
-      <c r="Q157" s="1"/>
-    </row>
-    <row r="158" spans="1:17">
+    </row>
+    <row r="158" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A158" s="10"/>
       <c r="B158" s="9"/>
       <c r="C158" s="1"/>
@@ -3713,9 +3605,8 @@
       <c r="N158" s="7"/>
       <c r="O158" s="7"/>
       <c r="P158" s="7"/>
-      <c r="Q158" s="1"/>
-    </row>
-    <row r="159" spans="1:17">
+    </row>
+    <row r="159" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A159" s="10"/>
       <c r="B159" s="9"/>
       <c r="C159" s="1"/>
@@ -3732,9 +3623,8 @@
       <c r="N159" s="7"/>
       <c r="O159" s="7"/>
       <c r="P159" s="7"/>
-      <c r="Q159" s="1"/>
-    </row>
-    <row r="160" spans="1:17">
+    </row>
+    <row r="160" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A160" s="10"/>
       <c r="B160" s="9"/>
       <c r="C160" s="1"/>
@@ -3751,9 +3641,8 @@
       <c r="N160" s="7"/>
       <c r="O160" s="7"/>
       <c r="P160" s="7"/>
-      <c r="Q160" s="1"/>
-    </row>
-    <row r="161" spans="1:17">
+    </row>
+    <row r="161" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A161" s="10"/>
       <c r="B161" s="9"/>
       <c r="C161" s="1"/>
@@ -3770,9 +3659,8 @@
       <c r="N161" s="7"/>
       <c r="O161" s="7"/>
       <c r="P161" s="7"/>
-      <c r="Q161" s="1"/>
-    </row>
-    <row r="162" spans="1:17">
+    </row>
+    <row r="162" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A162" s="10"/>
       <c r="B162" s="9"/>
       <c r="C162" s="1"/>
@@ -3789,9 +3677,8 @@
       <c r="N162" s="7"/>
       <c r="O162" s="7"/>
       <c r="P162" s="7"/>
-      <c r="Q162" s="1"/>
-    </row>
-    <row r="163" spans="1:17">
+    </row>
+    <row r="163" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A163" s="10"/>
       <c r="B163" s="9"/>
       <c r="C163" s="1"/>
@@ -3808,9 +3695,8 @@
       <c r="N163" s="7"/>
       <c r="O163" s="7"/>
       <c r="P163" s="7"/>
-      <c r="Q163" s="1"/>
-    </row>
-    <row r="164" spans="1:17">
+    </row>
+    <row r="164" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A164" s="10"/>
       <c r="B164" s="9"/>
       <c r="C164" s="1"/>
@@ -3827,9 +3713,8 @@
       <c r="N164" s="7"/>
       <c r="O164" s="7"/>
       <c r="P164" s="7"/>
-      <c r="Q164" s="1"/>
-    </row>
-    <row r="165" spans="1:17">
+    </row>
+    <row r="165" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A165" s="10"/>
       <c r="B165" s="9"/>
       <c r="C165" s="1"/>
@@ -3846,9 +3731,8 @@
       <c r="N165" s="7"/>
       <c r="O165" s="7"/>
       <c r="P165" s="7"/>
-      <c r="Q165" s="1"/>
-    </row>
-    <row r="166" spans="1:17">
+    </row>
+    <row r="166" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A166" s="10"/>
       <c r="B166" s="9"/>
       <c r="C166" s="1"/>
@@ -3865,9 +3749,8 @@
       <c r="N166" s="7"/>
       <c r="O166" s="7"/>
       <c r="P166" s="7"/>
-      <c r="Q166" s="1"/>
-    </row>
-    <row r="167" spans="1:17">
+    </row>
+    <row r="167" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A167" s="10"/>
       <c r="B167" s="9"/>
       <c r="C167" s="1"/>
@@ -3884,9 +3767,8 @@
       <c r="N167" s="7"/>
       <c r="O167" s="7"/>
       <c r="P167" s="7"/>
-      <c r="Q167" s="1"/>
-    </row>
-    <row r="168" spans="1:17">
+    </row>
+    <row r="168" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A168" s="10"/>
       <c r="B168" s="9"/>
       <c r="C168" s="1"/>
@@ -3903,9 +3785,8 @@
       <c r="N168" s="7"/>
       <c r="O168" s="7"/>
       <c r="P168" s="7"/>
-      <c r="Q168" s="1"/>
-    </row>
-    <row r="169" spans="1:17">
+    </row>
+    <row r="169" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A169" s="10"/>
       <c r="B169" s="9"/>
       <c r="C169" s="1"/>
@@ -3922,9 +3803,8 @@
       <c r="N169" s="7"/>
       <c r="O169" s="7"/>
       <c r="P169" s="7"/>
-      <c r="Q169" s="1"/>
-    </row>
-    <row r="170" spans="1:17">
+    </row>
+    <row r="170" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A170" s="10"/>
       <c r="B170" s="9"/>
       <c r="C170" s="1"/>
@@ -3941,9 +3821,8 @@
       <c r="N170" s="7"/>
       <c r="O170" s="7"/>
       <c r="P170" s="7"/>
-      <c r="Q170" s="1"/>
-    </row>
-    <row r="171" spans="1:17">
+    </row>
+    <row r="171" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A171" s="10"/>
       <c r="B171" s="9"/>
       <c r="C171" s="1"/>
@@ -3960,9 +3839,8 @@
       <c r="N171" s="7"/>
       <c r="O171" s="7"/>
       <c r="P171" s="7"/>
-      <c r="Q171" s="1"/>
-    </row>
-    <row r="172" spans="1:17">
+    </row>
+    <row r="172" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A172" s="10"/>
       <c r="B172" s="9"/>
       <c r="C172" s="1"/>
@@ -3979,9 +3857,8 @@
       <c r="N172" s="7"/>
       <c r="O172" s="7"/>
       <c r="P172" s="7"/>
-      <c r="Q172" s="1"/>
-    </row>
-    <row r="173" spans="1:17">
+    </row>
+    <row r="173" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A173" s="10"/>
       <c r="B173" s="9"/>
       <c r="C173" s="1"/>
@@ -3998,9 +3875,8 @@
       <c r="N173" s="7"/>
       <c r="O173" s="7"/>
       <c r="P173" s="7"/>
-      <c r="Q173" s="1"/>
-    </row>
-    <row r="174" spans="1:17">
+    </row>
+    <row r="174" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A174" s="10"/>
       <c r="B174" s="9"/>
       <c r="C174" s="1"/>
@@ -4017,9 +3893,8 @@
       <c r="N174" s="7"/>
       <c r="O174" s="7"/>
       <c r="P174" s="7"/>
-      <c r="Q174" s="1"/>
-    </row>
-    <row r="175" spans="1:17">
+    </row>
+    <row r="175" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A175" s="10"/>
       <c r="B175" s="9"/>
       <c r="C175" s="1"/>
@@ -4036,9 +3911,8 @@
       <c r="N175" s="7"/>
       <c r="O175" s="7"/>
       <c r="P175" s="7"/>
-      <c r="Q175" s="1"/>
-    </row>
-    <row r="176" spans="1:17">
+    </row>
+    <row r="176" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A176" s="10"/>
       <c r="B176" s="9"/>
       <c r="C176" s="1"/>
@@ -4055,9 +3929,8 @@
       <c r="N176" s="7"/>
       <c r="O176" s="7"/>
       <c r="P176" s="7"/>
-      <c r="Q176" s="1"/>
-    </row>
-    <row r="177" spans="1:17">
+    </row>
+    <row r="177" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A177" s="10"/>
       <c r="B177" s="9"/>
       <c r="C177" s="1"/>
@@ -4074,9 +3947,8 @@
       <c r="N177" s="7"/>
       <c r="O177" s="7"/>
       <c r="P177" s="7"/>
-      <c r="Q177" s="1"/>
-    </row>
-    <row r="178" spans="1:17">
+    </row>
+    <row r="178" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A178" s="10"/>
       <c r="B178" s="9"/>
       <c r="C178" s="1"/>
@@ -4093,9 +3965,8 @@
       <c r="N178" s="7"/>
       <c r="O178" s="7"/>
       <c r="P178" s="7"/>
-      <c r="Q178" s="1"/>
-    </row>
-    <row r="179" spans="1:17">
+    </row>
+    <row r="179" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A179" s="10"/>
       <c r="B179" s="9"/>
       <c r="C179" s="1"/>
@@ -4112,9 +3983,8 @@
       <c r="N179" s="7"/>
       <c r="O179" s="7"/>
       <c r="P179" s="7"/>
-      <c r="Q179" s="1"/>
-    </row>
-    <row r="180" spans="1:17">
+    </row>
+    <row r="180" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A180" s="10"/>
       <c r="B180" s="9"/>
       <c r="C180" s="1"/>
@@ -4131,9 +4001,8 @@
       <c r="N180" s="7"/>
       <c r="O180" s="7"/>
       <c r="P180" s="7"/>
-      <c r="Q180" s="1"/>
-    </row>
-    <row r="181" spans="1:17">
+    </row>
+    <row r="181" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A181" s="10"/>
       <c r="B181" s="9"/>
       <c r="C181" s="1"/>
@@ -4150,9 +4019,8 @@
       <c r="N181" s="7"/>
       <c r="O181" s="7"/>
       <c r="P181" s="7"/>
-      <c r="Q181" s="1"/>
-    </row>
-    <row r="182" spans="1:17">
+    </row>
+    <row r="182" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A182" s="10"/>
       <c r="B182" s="9"/>
       <c r="C182" s="1"/>
@@ -4169,9 +4037,8 @@
       <c r="N182" s="7"/>
       <c r="O182" s="7"/>
       <c r="P182" s="7"/>
-      <c r="Q182" s="1"/>
-    </row>
-    <row r="183" spans="1:17">
+    </row>
+    <row r="183" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A183" s="10"/>
       <c r="B183" s="9"/>
       <c r="C183" s="1"/>
@@ -4188,9 +4055,8 @@
       <c r="N183" s="7"/>
       <c r="O183" s="7"/>
       <c r="P183" s="7"/>
-      <c r="Q183" s="1"/>
-    </row>
-    <row r="184" spans="1:17">
+    </row>
+    <row r="184" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A184" s="10"/>
       <c r="B184" s="9"/>
       <c r="C184" s="1"/>
@@ -4207,9 +4073,8 @@
       <c r="N184" s="7"/>
       <c r="O184" s="7"/>
       <c r="P184" s="7"/>
-      <c r="Q184" s="1"/>
-    </row>
-    <row r="185" spans="1:17">
+    </row>
+    <row r="185" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A185" s="10"/>
       <c r="B185" s="9"/>
       <c r="C185" s="1"/>
@@ -4226,9 +4091,8 @@
       <c r="N185" s="7"/>
       <c r="O185" s="7"/>
       <c r="P185" s="7"/>
-      <c r="Q185" s="1"/>
-    </row>
-    <row r="186" spans="1:17">
+    </row>
+    <row r="186" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A186" s="10"/>
       <c r="B186" s="9"/>
       <c r="C186" s="1"/>
@@ -4245,9 +4109,8 @@
       <c r="N186" s="7"/>
       <c r="O186" s="7"/>
       <c r="P186" s="7"/>
-      <c r="Q186" s="1"/>
-    </row>
-    <row r="187" spans="1:17">
+    </row>
+    <row r="187" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A187" s="10"/>
       <c r="B187" s="9"/>
       <c r="C187" s="1"/>
@@ -4264,9 +4127,8 @@
       <c r="N187" s="7"/>
       <c r="O187" s="7"/>
       <c r="P187" s="7"/>
-      <c r="Q187" s="1"/>
-    </row>
-    <row r="188" spans="1:17">
+    </row>
+    <row r="188" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A188" s="10"/>
       <c r="B188" s="9"/>
       <c r="C188" s="1"/>
@@ -4283,9 +4145,8 @@
       <c r="N188" s="7"/>
       <c r="O188" s="7"/>
       <c r="P188" s="7"/>
-      <c r="Q188" s="1"/>
-    </row>
-    <row r="189" spans="1:17">
+    </row>
+    <row r="189" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A189" s="10"/>
       <c r="B189" s="9"/>
       <c r="C189" s="1"/>
@@ -4302,9 +4163,8 @@
       <c r="N189" s="7"/>
       <c r="O189" s="7"/>
       <c r="P189" s="7"/>
-      <c r="Q189" s="1"/>
-    </row>
-    <row r="190" spans="1:17">
+    </row>
+    <row r="190" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A190" s="10"/>
       <c r="B190" s="9"/>
       <c r="C190" s="1"/>
@@ -4321,9 +4181,8 @@
       <c r="N190" s="7"/>
       <c r="O190" s="7"/>
       <c r="P190" s="7"/>
-      <c r="Q190" s="1"/>
-    </row>
-    <row r="191" spans="1:17">
+    </row>
+    <row r="191" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A191" s="10"/>
       <c r="B191" s="9"/>
       <c r="C191" s="1"/>
@@ -4340,9 +4199,8 @@
       <c r="N191" s="7"/>
       <c r="O191" s="7"/>
       <c r="P191" s="7"/>
-      <c r="Q191" s="1"/>
-    </row>
-    <row r="192" spans="1:17">
+    </row>
+    <row r="192" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A192" s="10"/>
       <c r="B192" s="9"/>
       <c r="C192" s="1"/>
@@ -4359,9 +4217,8 @@
       <c r="N192" s="7"/>
       <c r="O192" s="7"/>
       <c r="P192" s="7"/>
-      <c r="Q192" s="1"/>
-    </row>
-    <row r="193" spans="1:17">
+    </row>
+    <row r="193" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A193" s="10"/>
       <c r="B193" s="9"/>
       <c r="C193" s="1"/>
@@ -4378,9 +4235,8 @@
       <c r="N193" s="7"/>
       <c r="O193" s="7"/>
       <c r="P193" s="7"/>
-      <c r="Q193" s="1"/>
-    </row>
-    <row r="194" spans="1:17">
+    </row>
+    <row r="194" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A194" s="10"/>
       <c r="B194" s="9"/>
       <c r="C194" s="1"/>
@@ -4397,9 +4253,8 @@
       <c r="N194" s="7"/>
       <c r="O194" s="7"/>
       <c r="P194" s="7"/>
-      <c r="Q194" s="1"/>
-    </row>
-    <row r="195" spans="1:17">
+    </row>
+    <row r="195" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A195" s="10"/>
       <c r="B195" s="9"/>
       <c r="C195" s="1"/>
@@ -4416,9 +4271,8 @@
       <c r="N195" s="7"/>
       <c r="O195" s="7"/>
       <c r="P195" s="7"/>
-      <c r="Q195" s="1"/>
-    </row>
-    <row r="196" spans="1:17">
+    </row>
+    <row r="196" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A196" s="10"/>
       <c r="B196" s="9"/>
       <c r="C196" s="1"/>
@@ -4435,9 +4289,8 @@
       <c r="N196" s="7"/>
       <c r="O196" s="7"/>
       <c r="P196" s="7"/>
-      <c r="Q196" s="1"/>
-    </row>
-    <row r="197" spans="1:17">
+    </row>
+    <row r="197" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A197" s="10"/>
       <c r="B197" s="9"/>
       <c r="C197" s="1"/>
@@ -4454,9 +4307,8 @@
       <c r="N197" s="7"/>
       <c r="O197" s="7"/>
       <c r="P197" s="7"/>
-      <c r="Q197" s="1"/>
-    </row>
-    <row r="198" spans="1:17">
+    </row>
+    <row r="198" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A198" s="10"/>
       <c r="B198" s="9"/>
       <c r="C198" s="1"/>
@@ -4473,9 +4325,8 @@
       <c r="N198" s="7"/>
       <c r="O198" s="7"/>
       <c r="P198" s="7"/>
-      <c r="Q198" s="1"/>
-    </row>
-    <row r="199" spans="1:17">
+    </row>
+    <row r="199" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A199" s="10"/>
       <c r="B199" s="9"/>
       <c r="C199" s="1"/>
@@ -4492,9 +4343,8 @@
       <c r="N199" s="7"/>
       <c r="O199" s="7"/>
       <c r="P199" s="7"/>
-      <c r="Q199" s="1"/>
-    </row>
-    <row r="200" spans="1:17">
+    </row>
+    <row r="200" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A200" s="10"/>
       <c r="B200" s="9"/>
       <c r="C200" s="1"/>
@@ -4511,9 +4361,8 @@
       <c r="N200" s="7"/>
       <c r="O200" s="7"/>
       <c r="P200" s="7"/>
-      <c r="Q200" s="1"/>
-    </row>
-    <row r="201" spans="1:17">
+    </row>
+    <row r="201" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A201" s="10"/>
       <c r="B201" s="9"/>
       <c r="C201" s="1"/>
@@ -4530,9 +4379,8 @@
       <c r="N201" s="7"/>
       <c r="O201" s="7"/>
       <c r="P201" s="7"/>
-      <c r="Q201" s="1"/>
-    </row>
-    <row r="202" spans="1:17">
+    </row>
+    <row r="202" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A202" s="10"/>
       <c r="B202" s="9"/>
       <c r="C202" s="1"/>
@@ -4549,9 +4397,8 @@
       <c r="N202" s="7"/>
       <c r="O202" s="7"/>
       <c r="P202" s="7"/>
-      <c r="Q202" s="1"/>
-    </row>
-    <row r="203" spans="1:17">
+    </row>
+    <row r="203" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A203" s="10"/>
       <c r="B203" s="9"/>
       <c r="C203" s="1"/>
@@ -4568,9 +4415,8 @@
       <c r="N203" s="7"/>
       <c r="O203" s="7"/>
       <c r="P203" s="7"/>
-      <c r="Q203" s="1"/>
-    </row>
-    <row r="204" spans="1:17">
+    </row>
+    <row r="204" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A204" s="10"/>
       <c r="B204" s="9"/>
       <c r="C204" s="1"/>
@@ -4587,9 +4433,8 @@
       <c r="N204" s="7"/>
       <c r="O204" s="7"/>
       <c r="P204" s="7"/>
-      <c r="Q204" s="1"/>
-    </row>
-    <row r="205" spans="1:17">
+    </row>
+    <row r="205" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A205" s="10"/>
       <c r="B205" s="9"/>
       <c r="C205" s="1"/>
@@ -4606,9 +4451,8 @@
       <c r="N205" s="7"/>
       <c r="O205" s="7"/>
       <c r="P205" s="7"/>
-      <c r="Q205" s="1"/>
-    </row>
-    <row r="206" spans="1:17">
+    </row>
+    <row r="206" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A206" s="10"/>
       <c r="B206" s="9"/>
       <c r="C206" s="1"/>
@@ -4625,9 +4469,8 @@
       <c r="N206" s="7"/>
       <c r="O206" s="7"/>
       <c r="P206" s="7"/>
-      <c r="Q206" s="1"/>
-    </row>
-    <row r="207" spans="1:17">
+    </row>
+    <row r="207" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A207" s="10"/>
       <c r="B207" s="9"/>
       <c r="C207" s="1"/>
@@ -4644,9 +4487,8 @@
       <c r="N207" s="7"/>
       <c r="O207" s="7"/>
       <c r="P207" s="7"/>
-      <c r="Q207" s="1"/>
-    </row>
-    <row r="208" spans="1:17">
+    </row>
+    <row r="208" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A208" s="10"/>
       <c r="B208" s="9"/>
       <c r="C208" s="1"/>
@@ -4663,9 +4505,8 @@
       <c r="N208" s="7"/>
       <c r="O208" s="7"/>
       <c r="P208" s="7"/>
-      <c r="Q208" s="1"/>
-    </row>
-    <row r="209" spans="1:17">
+    </row>
+    <row r="209" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A209" s="10"/>
       <c r="B209" s="9"/>
       <c r="C209" s="1"/>
@@ -4682,9 +4523,8 @@
       <c r="N209" s="7"/>
       <c r="O209" s="7"/>
       <c r="P209" s="7"/>
-      <c r="Q209" s="1"/>
-    </row>
-    <row r="210" spans="1:17">
+    </row>
+    <row r="210" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A210" s="10"/>
       <c r="B210" s="9"/>
       <c r="C210" s="1"/>
@@ -4701,9 +4541,8 @@
       <c r="N210" s="7"/>
       <c r="O210" s="7"/>
       <c r="P210" s="7"/>
-      <c r="Q210" s="1"/>
-    </row>
-    <row r="211" spans="1:17">
+    </row>
+    <row r="211" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A211" s="10"/>
       <c r="B211" s="9"/>
       <c r="C211" s="1"/>
@@ -4720,9 +4559,8 @@
       <c r="N211" s="7"/>
       <c r="O211" s="7"/>
       <c r="P211" s="7"/>
-      <c r="Q211" s="1"/>
-    </row>
-    <row r="212" spans="1:17">
+    </row>
+    <row r="212" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A212" s="10"/>
       <c r="B212" s="9"/>
       <c r="C212" s="1"/>
@@ -4739,9 +4577,8 @@
       <c r="N212" s="7"/>
       <c r="O212" s="7"/>
       <c r="P212" s="7"/>
-      <c r="Q212" s="1"/>
-    </row>
-    <row r="213" spans="1:17">
+    </row>
+    <row r="213" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A213" s="10"/>
       <c r="B213" s="9"/>
       <c r="C213" s="1"/>
@@ -4758,9 +4595,8 @@
       <c r="N213" s="7"/>
       <c r="O213" s="7"/>
       <c r="P213" s="7"/>
-      <c r="Q213" s="1"/>
-    </row>
-    <row r="214" spans="1:17">
+    </row>
+    <row r="214" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A214" s="10"/>
       <c r="B214" s="9"/>
       <c r="C214" s="1"/>
@@ -4777,9 +4613,8 @@
       <c r="N214" s="7"/>
       <c r="O214" s="7"/>
       <c r="P214" s="7"/>
-      <c r="Q214" s="1"/>
-    </row>
-    <row r="215" spans="1:17">
+    </row>
+    <row r="215" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A215" s="10"/>
       <c r="B215" s="9"/>
       <c r="C215" s="1"/>
@@ -4796,9 +4631,8 @@
       <c r="N215" s="7"/>
       <c r="O215" s="7"/>
       <c r="P215" s="7"/>
-      <c r="Q215" s="1"/>
-    </row>
-    <row r="216" spans="1:17">
+    </row>
+    <row r="216" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A216" s="10"/>
       <c r="B216" s="9"/>
       <c r="C216" s="1"/>
@@ -4815,9 +4649,8 @@
       <c r="N216" s="7"/>
       <c r="O216" s="7"/>
       <c r="P216" s="7"/>
-      <c r="Q216" s="1"/>
-    </row>
-    <row r="217" spans="1:17">
+    </row>
+    <row r="217" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A217" s="10"/>
       <c r="B217" s="9"/>
       <c r="C217" s="1"/>
@@ -4834,9 +4667,8 @@
       <c r="N217" s="7"/>
       <c r="O217" s="7"/>
       <c r="P217" s="7"/>
-      <c r="Q217" s="1"/>
-    </row>
-    <row r="218" spans="1:17">
+    </row>
+    <row r="218" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A218" s="10"/>
       <c r="B218" s="9"/>
       <c r="C218" s="1"/>
@@ -4853,9 +4685,8 @@
       <c r="N218" s="7"/>
       <c r="O218" s="7"/>
       <c r="P218" s="7"/>
-      <c r="Q218" s="1"/>
-    </row>
-    <row r="219" spans="1:17">
+    </row>
+    <row r="219" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A219" s="10"/>
       <c r="B219" s="9"/>
       <c r="C219" s="1"/>
@@ -4872,9 +4703,8 @@
       <c r="N219" s="7"/>
       <c r="O219" s="7"/>
       <c r="P219" s="7"/>
-      <c r="Q219" s="1"/>
-    </row>
-    <row r="220" spans="1:17">
+    </row>
+    <row r="220" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A220" s="10"/>
       <c r="B220" s="9"/>
       <c r="C220" s="1"/>
@@ -4891,9 +4721,8 @@
       <c r="N220" s="7"/>
       <c r="O220" s="7"/>
       <c r="P220" s="7"/>
-      <c r="Q220" s="1"/>
-    </row>
-    <row r="221" spans="1:17">
+    </row>
+    <row r="221" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A221" s="10"/>
       <c r="B221" s="9"/>
       <c r="C221" s="1"/>
@@ -4910,9 +4739,8 @@
       <c r="N221" s="7"/>
       <c r="O221" s="7"/>
       <c r="P221" s="7"/>
-      <c r="Q221" s="1"/>
-    </row>
-    <row r="222" spans="1:17">
+    </row>
+    <row r="222" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A222" s="10"/>
       <c r="B222" s="9"/>
       <c r="C222" s="1"/>
@@ -4929,9 +4757,8 @@
       <c r="N222" s="7"/>
       <c r="O222" s="7"/>
       <c r="P222" s="7"/>
-      <c r="Q222" s="1"/>
-    </row>
-    <row r="223" spans="1:17">
+    </row>
+    <row r="223" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A223" s="10"/>
       <c r="B223" s="9"/>
       <c r="C223" s="1"/>
@@ -4948,9 +4775,8 @@
       <c r="N223" s="7"/>
       <c r="O223" s="7"/>
       <c r="P223" s="7"/>
-      <c r="Q223" s="1"/>
-    </row>
-    <row r="224" spans="1:17">
+    </row>
+    <row r="224" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A224" s="10"/>
       <c r="B224" s="9"/>
       <c r="C224" s="1"/>
@@ -4967,9 +4793,8 @@
       <c r="N224" s="7"/>
       <c r="O224" s="7"/>
       <c r="P224" s="7"/>
-      <c r="Q224" s="1"/>
-    </row>
-    <row r="225" spans="1:17">
+    </row>
+    <row r="225" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A225" s="10"/>
       <c r="B225" s="9"/>
       <c r="C225" s="1"/>
@@ -4986,9 +4811,8 @@
       <c r="N225" s="7"/>
       <c r="O225" s="7"/>
       <c r="P225" s="7"/>
-      <c r="Q225" s="1"/>
-    </row>
-    <row r="226" spans="1:17">
+    </row>
+    <row r="226" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A226" s="10"/>
       <c r="B226" s="9"/>
       <c r="C226" s="1"/>
@@ -5005,9 +4829,8 @@
       <c r="N226" s="7"/>
       <c r="O226" s="7"/>
       <c r="P226" s="7"/>
-      <c r="Q226" s="1"/>
-    </row>
-    <row r="227" spans="1:17">
+    </row>
+    <row r="227" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A227" s="10"/>
       <c r="B227" s="9"/>
       <c r="C227" s="1"/>
@@ -5024,9 +4847,8 @@
       <c r="N227" s="7"/>
       <c r="O227" s="7"/>
       <c r="P227" s="7"/>
-      <c r="Q227" s="1"/>
-    </row>
-    <row r="228" spans="1:17">
+    </row>
+    <row r="228" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A228" s="10"/>
       <c r="B228" s="9"/>
       <c r="C228" s="1"/>
@@ -5043,9 +4865,8 @@
       <c r="N228" s="7"/>
       <c r="O228" s="7"/>
       <c r="P228" s="7"/>
-      <c r="Q228" s="1"/>
-    </row>
-    <row r="229" spans="1:17">
+    </row>
+    <row r="229" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A229" s="10"/>
       <c r="B229" s="9"/>
       <c r="C229" s="1"/>
@@ -5062,9 +4883,8 @@
       <c r="N229" s="7"/>
       <c r="O229" s="7"/>
       <c r="P229" s="7"/>
-      <c r="Q229" s="1"/>
-    </row>
-    <row r="230" spans="1:17">
+    </row>
+    <row r="230" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A230" s="10"/>
       <c r="B230" s="9"/>
       <c r="C230" s="1"/>
@@ -5081,11 +4901,10 @@
       <c r="N230" s="7"/>
       <c r="O230" s="7"/>
       <c r="P230" s="7"/>
-      <c r="Q230" s="1"/>
-    </row>
-    <row r="231" spans="1:17">
+    </row>
+    <row r="231" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A231" s="10"/>
-      <c r="B231" s="5"/>
+      <c r="B231" s="9"/>
       <c r="C231" s="1"/>
       <c r="D231" s="1"/>
       <c r="E231" s="1"/>
@@ -5100,23 +4919,79 @@
       <c r="N231" s="7"/>
       <c r="O231" s="7"/>
       <c r="P231" s="7"/>
-      <c r="Q231" s="1"/>
-    </row>
-    <row r="232" spans="1:17">
-      <c r="A232" s="8"/>
-      <c r="B232" s="5"/>
+    </row>
+    <row r="232" spans="1:16" ht="14" x14ac:dyDescent="0.2">
+      <c r="A232" s="10"/>
+      <c r="B232" s="9"/>
+      <c r="C232" s="1"/>
+      <c r="D232" s="1"/>
+      <c r="E232" s="1"/>
+      <c r="F232" s="1"/>
+      <c r="G232" s="1"/>
+      <c r="H232" s="1"/>
+      <c r="I232" s="1"/>
+      <c r="J232" s="1"/>
+      <c r="K232" s="1"/>
+      <c r="L232" s="1"/>
+      <c r="M232" s="1"/>
+      <c r="N232" s="7"/>
+      <c r="O232" s="7"/>
+      <c r="P232" s="7"/>
+    </row>
+    <row r="233" spans="1:16" ht="14" x14ac:dyDescent="0.2">
+      <c r="A233" s="10"/>
+      <c r="B233" s="9"/>
+      <c r="C233" s="1"/>
+      <c r="D233" s="1"/>
+      <c r="E233" s="1"/>
+      <c r="F233" s="1"/>
+      <c r="G233" s="1"/>
+      <c r="H233" s="1"/>
+      <c r="I233" s="1"/>
+      <c r="J233" s="1"/>
+      <c r="K233" s="1"/>
+      <c r="L233" s="1"/>
+      <c r="M233" s="1"/>
+      <c r="N233" s="7"/>
+      <c r="O233" s="7"/>
+      <c r="P233" s="7"/>
+    </row>
+    <row r="234" spans="1:16" ht="14" x14ac:dyDescent="0.2">
+      <c r="A234" s="10"/>
+      <c r="B234" s="5"/>
+      <c r="C234" s="1"/>
+      <c r="D234" s="1"/>
+      <c r="E234" s="1"/>
+      <c r="F234" s="1"/>
+      <c r="G234" s="1"/>
+      <c r="H234" s="1"/>
+      <c r="I234" s="1"/>
+      <c r="J234" s="1"/>
+      <c r="K234" s="1"/>
+      <c r="L234" s="1"/>
+      <c r="M234" s="1"/>
+      <c r="N234" s="7"/>
+      <c r="O234" s="7"/>
+      <c r="P234" s="7"/>
+    </row>
+    <row r="235" spans="1:16" ht="14" x14ac:dyDescent="0.2">
+      <c r="A235" s="8"/>
+      <c r="B235" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="N2:P2"/>
+  <mergeCells count="6">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:N4"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4" xr:uid="{A11CAA21-DA7B-4A25-8E50-8C970663190D}"/>
-    <dataValidation errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Lopetusaika" error="Lopetusajan täytyy olla aloitusajan jälkeen!_x000a_" promptTitle="Lopetusaika" prompt="Anna lopetusaika muodossa P.K.VVVV TT:MM (esim. 15.6.2023 12:35)" sqref="B232" xr:uid="{BA0AE0C4-B841-467B-886E-8D146108C67C}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Aloitusaika" prompt="Anna aloitusaika muodossa P.K.VVVV TT:MM (esim. 15.6.2023 12:35)" sqref="A5:A232" xr:uid="{1403E155-6642-49BE-A159-49D420F73634}"/>
-    <dataValidation errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="_x000a_" promptTitle="Lopetusaika" prompt="Anna lopetusaika muodossa P.K.VVVV TT:MM (esim. 15.6.2023 12:35)" sqref="B5:B231" xr:uid="{3D508563-3D50-46B1-894A-D0B20D73DBD9}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7" xr:uid="{A11CAA21-DA7B-4A25-8E50-8C970663190D}"/>
+    <dataValidation errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Lopetusaika" error="Lopetusajan täytyy olla aloitusajan jälkeen!_x000a_" promptTitle="Lopetusaika" prompt="Anna lopetusaika muodossa P.K.VVVV TT:MM (esim. 15.6.2023 12:35)" sqref="B235" xr:uid="{BA0AE0C4-B841-467B-886E-8D146108C67C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Aloitusaika" prompt="Anna aloitusaika muodossa P.K.VVVV TT:MM (esim. 15.6.2023 12:35)" sqref="A8:A235" xr:uid="{1403E155-6642-49BE-A159-49D420F73634}"/>
+    <dataValidation errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="_x000a_" promptTitle="Lopetusaika" prompt="Anna lopetusaika muodossa P.K.VVVV TT:MM (esim. 15.6.2023 12:35)" sqref="B8:B234" xr:uid="{3D508563-3D50-46B1-894A-D0B20D73DBD9}"/>
   </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5131,19 +5006,19 @@
           <x14:formula1>
             <xm:f>Valinnat!$A$2:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>N5:N231</xm:sqref>
+          <xm:sqref>N8:N234</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BFB3B0FC-61F9-4DDB-A471-8C214C701065}">
           <x14:formula1>
             <xm:f>Valinnat!$B2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>O5:O231</xm:sqref>
+          <xm:sqref>O8:O234</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3695DAF1-6B70-495B-9262-61DB611703C9}">
           <x14:formula1>
             <xm:f>Valinnat!$C2:$C$8</xm:f>
           </x14:formula1>
-          <xm:sqref>P5:P231</xm:sqref>
+          <xm:sqref>P8:P234</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5157,99 +5032,99 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
         <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>26</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6">
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B7">
         <v>31</v>
       </c>
       <c r="C7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
         <v>38</v>
-      </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>